<commit_message>
Added test results for Arduino Nano
</commit_message>
<xml_diff>
--- a/BenchmarkDocs/Results.xlsx
+++ b/BenchmarkDocs/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f0dc99f0b729840/Teilen/edge-ml/feature-extraction/BenchmarkDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="442" documentId="8_{5DA93DCD-0496-4FBE-A67D-F6BE2EADACEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{356ACF91-1B5A-4B6F-94DF-AB0CFF7E80F5}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E4B3007-A998-4A4A-BFA6-5F773B1A229E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="122">
   <si>
     <t>Arduino</t>
   </si>
@@ -306,9 +306,6 @@
     <t>ExtractOne, 1000 Werte</t>
   </si>
   <si>
-    <t>Arduino(all)</t>
-  </si>
-  <si>
     <t>307ms</t>
   </si>
   <si>
@@ -325,6 +322,84 @@
   </si>
   <si>
     <t>10ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicla </t>
+  </si>
+  <si>
+    <t>Nano</t>
+  </si>
+  <si>
+    <t>Nicla</t>
+  </si>
+  <si>
+    <t>615ms</t>
+  </si>
+  <si>
+    <t>614ms</t>
+  </si>
+  <si>
+    <t>678ms</t>
+  </si>
+  <si>
+    <t>677ms</t>
+  </si>
+  <si>
+    <t>676ms</t>
+  </si>
+  <si>
+    <t>Wortlänge</t>
+  </si>
+  <si>
+    <t>333ms</t>
+  </si>
+  <si>
+    <t>334ms</t>
+  </si>
+  <si>
+    <t>303ms</t>
+  </si>
+  <si>
+    <t>304ms</t>
+  </si>
+  <si>
+    <t>Flash</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>299816/527616 (56%)</t>
+  </si>
+  <si>
+    <t>16232/48056 (25%)</t>
+  </si>
+  <si>
+    <t>330448/983040 (33%)</t>
+  </si>
+  <si>
+    <t>50024/262144 (19%)</t>
+  </si>
+  <si>
+    <t>Sketch</t>
+  </si>
+  <si>
+    <t>Programmstart</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>864/32768</t>
+  </si>
+  <si>
+    <t>14836/210584</t>
+  </si>
+  <si>
+    <t>Max Datengröße (extractAll)</t>
   </si>
 </sst>
 </file>
@@ -676,43 +751,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B09DA97-D620-4F66-8E45-7C0B77C13B9B}">
-  <dimension ref="B1:Z66"/>
+  <dimension ref="B1:AD66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
     <col min="15" max="15" width="13.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
     <col min="17" max="17" width="12.5703125" customWidth="1"/>
     <col min="21" max="21" width="22.28515625" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
     <col min="23" max="23" width="11.42578125" customWidth="1"/>
     <col min="24" max="24" width="11.140625" customWidth="1"/>
     <col min="25" max="25" width="16.42578125" customWidth="1"/>
-    <col min="26" max="26" width="36" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" customWidth="1"/>
+    <col min="29" max="29" width="16.140625" customWidth="1"/>
+    <col min="30" max="30" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>33</v>
       </c>
@@ -725,26 +803,26 @@
       <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
         <v>0</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>7</v>
       </c>
-      <c r="P2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -760,38 +838,38 @@
       <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" t="s">
-        <v>4</v>
-      </c>
       <c r="L3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
         <v>4</v>
       </c>
       <c r="O3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q3" t="s">
         <v>4</v>
       </c>
       <c r="R3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="T3" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
@@ -807,35 +885,35 @@
       <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4" t="s">
         <v>25</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>22</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>9</v>
       </c>
-      <c r="O4">
+      <c r="R4">
         <v>1</v>
       </c>
-      <c r="P4" t="s">
+      <c r="S4" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="T4" t="s">
         <v>15</v>
       </c>
-      <c r="R4" t="s">
+      <c r="U4" t="s">
         <v>8</v>
       </c>
-      <c r="S4" t="s">
+      <c r="V4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
@@ -851,26 +929,26 @@
       <c r="G5" t="s">
         <v>28</v>
       </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5" t="s">
         <v>22</v>
       </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>23</v>
       </c>
-      <c r="O5">
-        <v>2</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="T5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>3</v>
       </c>
@@ -886,26 +964,26 @@
       <c r="G6" t="s">
         <v>28</v>
       </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6" t="s">
         <v>25</v>
       </c>
-      <c r="K6" t="s">
+      <c r="N6" t="s">
         <v>22</v>
       </c>
-      <c r="O6">
-        <v>3</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="R6">
+        <v>3</v>
+      </c>
+      <c r="S6" t="s">
         <v>12</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="T6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>4</v>
       </c>
@@ -921,26 +999,26 @@
       <c r="G7" t="s">
         <v>28</v>
       </c>
-      <c r="I7">
-        <v>4</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7" t="s">
         <v>25</v>
       </c>
-      <c r="K7" t="s">
+      <c r="N7" t="s">
         <v>22</v>
       </c>
-      <c r="O7">
-        <v>4</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="T7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>5</v>
       </c>
@@ -956,26 +1034,26 @@
       <c r="G8" t="s">
         <v>28</v>
       </c>
-      <c r="I8">
-        <v>5</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8" t="s">
         <v>22</v>
       </c>
-      <c r="K8" t="s">
+      <c r="N8" t="s">
         <v>22</v>
       </c>
-      <c r="O8">
-        <v>5</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="R8">
+        <v>5</v>
+      </c>
+      <c r="S8" t="s">
         <v>14</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="T8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>6</v>
       </c>
@@ -991,26 +1069,26 @@
       <c r="G9" t="s">
         <v>28</v>
       </c>
-      <c r="I9">
-        <v>6</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9" t="s">
         <v>25</v>
       </c>
-      <c r="K9" t="s">
+      <c r="N9" t="s">
         <v>22</v>
       </c>
-      <c r="O9">
-        <v>6</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="R9">
+        <v>6</v>
+      </c>
+      <c r="S9" t="s">
         <v>15</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="T9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>7</v>
       </c>
@@ -1026,26 +1104,26 @@
       <c r="G10" t="s">
         <v>28</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <v>7</v>
       </c>
-      <c r="J10" t="s">
+      <c r="M10" t="s">
         <v>25</v>
       </c>
-      <c r="K10" t="s">
+      <c r="N10" t="s">
         <v>24</v>
       </c>
-      <c r="O10">
+      <c r="R10">
         <v>7</v>
       </c>
-      <c r="P10" t="s">
+      <c r="S10" t="s">
         <v>14</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="T10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>8</v>
       </c>
@@ -1061,26 +1139,26 @@
       <c r="G11" t="s">
         <v>28</v>
       </c>
-      <c r="I11">
+      <c r="L11">
         <v>8</v>
       </c>
-      <c r="J11" t="s">
+      <c r="M11" t="s">
         <v>25</v>
       </c>
-      <c r="K11" t="s">
+      <c r="N11" t="s">
         <v>22</v>
       </c>
-      <c r="O11">
+      <c r="R11">
         <v>8</v>
       </c>
-      <c r="P11" t="s">
+      <c r="S11" t="s">
         <v>16</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="T11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>9</v>
       </c>
@@ -1096,26 +1174,26 @@
       <c r="G12" t="s">
         <v>28</v>
       </c>
-      <c r="I12">
+      <c r="L12">
         <v>9</v>
       </c>
-      <c r="J12" t="s">
+      <c r="M12" t="s">
         <v>22</v>
       </c>
-      <c r="K12" t="s">
+      <c r="N12" t="s">
         <v>22</v>
       </c>
-      <c r="O12">
+      <c r="R12">
         <v>9</v>
       </c>
-      <c r="P12" t="s">
+      <c r="S12" t="s">
         <v>17</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="T12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>10</v>
       </c>
@@ -1131,31 +1209,31 @@
       <c r="G13" t="s">
         <v>28</v>
       </c>
-      <c r="I13">
+      <c r="L13">
         <v>10</v>
       </c>
-      <c r="J13" t="s">
+      <c r="M13" t="s">
         <v>25</v>
       </c>
-      <c r="K13" t="s">
+      <c r="N13" t="s">
         <v>22</v>
       </c>
-      <c r="O13">
+      <c r="R13">
         <v>10</v>
       </c>
-      <c r="P13" t="s">
+      <c r="S13" t="s">
         <v>18</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="T13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -1166,22 +1244,37 @@
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>90</v>
-      </c>
-      <c r="I17" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" t="s">
+        <v>97</v>
+      </c>
+      <c r="L17" t="s">
         <v>1</v>
       </c>
-      <c r="J17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" t="s">
-        <v>90</v>
+      <c r="M17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O17" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>97</v>
       </c>
       <c r="U17" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="V17" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>5</v>
       </c>
@@ -1197,20 +1290,35 @@
       <c r="G18" t="s">
         <v>4</v>
       </c>
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
       <c r="I18" t="s">
-        <v>5</v>
-      </c>
-      <c r="J18" t="s">
-        <v>3</v>
-      </c>
-      <c r="K18" t="s">
         <v>4</v>
       </c>
       <c r="L18" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M18" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="N18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O18" t="s">
+        <v>3</v>
+      </c>
+      <c r="P18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>3</v>
+      </c>
+      <c r="R18" t="s">
+        <v>4</v>
+      </c>
+      <c r="T18" t="s">
+        <v>104</v>
       </c>
       <c r="U18" t="s">
         <v>34</v>
@@ -1228,10 +1336,19 @@
         <v>51</v>
       </c>
       <c r="Z18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>1</v>
       </c>
@@ -1242,19 +1359,34 @@
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G19" t="s">
-        <v>93</v>
-      </c>
-      <c r="I19">
+        <v>92</v>
+      </c>
+      <c r="H19" t="s">
+        <v>107</v>
+      </c>
+      <c r="I19" t="s">
+        <v>105</v>
+      </c>
+      <c r="L19">
         <v>1</v>
       </c>
-      <c r="J19" t="s">
+      <c r="M19" t="s">
         <v>25</v>
       </c>
-      <c r="K19" t="s">
-        <v>95</v>
+      <c r="N19" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>99</v>
+      </c>
+      <c r="R19" t="s">
+        <v>101</v>
+      </c>
+      <c r="T19">
+        <v>4</v>
       </c>
       <c r="U19" t="s">
         <v>35</v>
@@ -1265,8 +1397,14 @@
       <c r="W19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z19">
+        <v>2</v>
+      </c>
+      <c r="AA19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>2</v>
       </c>
@@ -1277,19 +1415,34 @@
         <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
-      </c>
-      <c r="I20">
-        <v>2</v>
-      </c>
-      <c r="J20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" t="s">
+        <v>107</v>
+      </c>
+      <c r="I20" t="s">
+        <v>105</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20" t="s">
         <v>25</v>
       </c>
-      <c r="K20" t="s">
-        <v>96</v>
+      <c r="N20" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>99</v>
+      </c>
+      <c r="R20" t="s">
+        <v>102</v>
+      </c>
+      <c r="T20">
+        <v>12</v>
       </c>
       <c r="U20" t="s">
         <v>36</v>
@@ -1300,8 +1453,14 @@
       <c r="W20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z20">
+        <v>4</v>
+      </c>
+      <c r="AA20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>3</v>
       </c>
@@ -1312,19 +1471,34 @@
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G21" t="s">
-        <v>93</v>
-      </c>
-      <c r="I21">
-        <v>3</v>
-      </c>
-      <c r="J21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" t="s">
+        <v>107</v>
+      </c>
+      <c r="I21" t="s">
+        <v>106</v>
+      </c>
+      <c r="L21">
+        <v>3</v>
+      </c>
+      <c r="M21" t="s">
         <v>25</v>
       </c>
-      <c r="K21" t="s">
-        <v>95</v>
+      <c r="N21" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>99</v>
+      </c>
+      <c r="R21" t="s">
+        <v>103</v>
+      </c>
+      <c r="T21">
+        <v>18</v>
       </c>
       <c r="U21" t="s">
         <v>37</v>
@@ -1335,8 +1509,14 @@
       <c r="W21">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z21">
+        <v>53</v>
+      </c>
+      <c r="AA21">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>4</v>
       </c>
@@ -1347,19 +1527,34 @@
         <v>27</v>
       </c>
       <c r="F22" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" t="s">
         <v>92</v>
       </c>
-      <c r="G22" t="s">
-        <v>93</v>
-      </c>
-      <c r="I22">
-        <v>4</v>
-      </c>
-      <c r="J22" t="s">
+      <c r="H22" t="s">
+        <v>107</v>
+      </c>
+      <c r="I22" t="s">
+        <v>106</v>
+      </c>
+      <c r="L22">
+        <v>4</v>
+      </c>
+      <c r="M22" t="s">
         <v>25</v>
       </c>
-      <c r="K22" t="s">
-        <v>95</v>
+      <c r="N22" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>100</v>
+      </c>
+      <c r="R22" t="s">
+        <v>103</v>
+      </c>
+      <c r="T22">
+        <v>6</v>
       </c>
       <c r="U22" t="s">
         <v>38</v>
@@ -1370,8 +1565,14 @@
       <c r="W22">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z22">
+        <v>16</v>
+      </c>
+      <c r="AA22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>5</v>
       </c>
@@ -1382,19 +1583,34 @@
         <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G23" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" t="s">
+        <v>107</v>
+      </c>
+      <c r="I23" t="s">
+        <v>105</v>
+      </c>
+      <c r="L23">
+        <v>5</v>
+      </c>
+      <c r="M23" t="s">
+        <v>25</v>
+      </c>
+      <c r="N23" t="s">
         <v>94</v>
       </c>
-      <c r="I23">
-        <v>5</v>
-      </c>
-      <c r="J23" t="s">
-        <v>25</v>
-      </c>
-      <c r="K23" t="s">
-        <v>95</v>
+      <c r="Q23" t="s">
+        <v>99</v>
+      </c>
+      <c r="R23" t="s">
+        <v>102</v>
+      </c>
+      <c r="T23">
+        <v>15</v>
       </c>
       <c r="U23" t="s">
         <v>39</v>
@@ -1405,8 +1621,14 @@
       <c r="W23">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z23">
+        <v>19</v>
+      </c>
+      <c r="AA23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>6</v>
       </c>
@@ -1417,19 +1639,34 @@
         <v>27</v>
       </c>
       <c r="F24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" t="s">
         <v>92</v>
       </c>
-      <c r="G24" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24">
-        <v>6</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="H24" t="s">
+        <v>108</v>
+      </c>
+      <c r="I24" t="s">
+        <v>105</v>
+      </c>
+      <c r="L24">
+        <v>6</v>
+      </c>
+      <c r="M24" t="s">
+        <v>94</v>
+      </c>
+      <c r="N24" t="s">
         <v>95</v>
       </c>
-      <c r="K24" t="s">
-        <v>96</v>
+      <c r="Q24" t="s">
+        <v>100</v>
+      </c>
+      <c r="R24" t="s">
+        <v>102</v>
+      </c>
+      <c r="T24">
+        <v>11</v>
       </c>
       <c r="U24" t="s">
         <v>40</v>
@@ -1440,8 +1677,14 @@
       <c r="W24">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z24">
+        <v>19</v>
+      </c>
+      <c r="AA24">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>7</v>
       </c>
@@ -1452,19 +1695,34 @@
         <v>27</v>
       </c>
       <c r="F25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
-      </c>
-      <c r="I25">
+        <v>93</v>
+      </c>
+      <c r="H25" t="s">
+        <v>107</v>
+      </c>
+      <c r="I25" t="s">
+        <v>105</v>
+      </c>
+      <c r="L25">
         <v>7</v>
       </c>
-      <c r="J25" t="s">
+      <c r="M25" t="s">
         <v>25</v>
       </c>
-      <c r="K25" t="s">
-        <v>96</v>
+      <c r="N25" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>100</v>
+      </c>
+      <c r="R25" t="s">
+        <v>102</v>
+      </c>
+      <c r="T25">
+        <v>14</v>
       </c>
       <c r="U25" t="s">
         <v>41</v>
@@ -1475,8 +1733,14 @@
       <c r="W25">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z25">
+        <v>34</v>
+      </c>
+      <c r="AA25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>8</v>
       </c>
@@ -1487,19 +1751,34 @@
         <v>27</v>
       </c>
       <c r="F26" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" t="s">
         <v>92</v>
       </c>
-      <c r="G26" t="s">
-        <v>93</v>
-      </c>
-      <c r="I26">
+      <c r="H26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" t="s">
+        <v>106</v>
+      </c>
+      <c r="L26">
         <v>8</v>
       </c>
-      <c r="J26" t="s">
+      <c r="M26" t="s">
+        <v>94</v>
+      </c>
+      <c r="N26" t="s">
         <v>95</v>
       </c>
-      <c r="K26" t="s">
-        <v>96</v>
+      <c r="Q26" t="s">
+        <v>99</v>
+      </c>
+      <c r="R26" t="s">
+        <v>101</v>
+      </c>
+      <c r="T26">
+        <v>7</v>
       </c>
       <c r="U26" t="s">
         <v>42</v>
@@ -1510,8 +1789,14 @@
       <c r="W26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z26">
+        <v>6</v>
+      </c>
+      <c r="AA26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>9</v>
       </c>
@@ -1522,19 +1807,34 @@
         <v>27</v>
       </c>
       <c r="F27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G27" t="s">
-        <v>93</v>
-      </c>
-      <c r="I27">
+        <v>92</v>
+      </c>
+      <c r="H27" t="s">
+        <v>108</v>
+      </c>
+      <c r="I27" t="s">
+        <v>106</v>
+      </c>
+      <c r="L27">
         <v>9</v>
       </c>
-      <c r="J27" t="s">
+      <c r="M27" t="s">
+        <v>94</v>
+      </c>
+      <c r="N27" t="s">
         <v>95</v>
       </c>
-      <c r="K27" t="s">
-        <v>96</v>
+      <c r="Q27" t="s">
+        <v>99</v>
+      </c>
+      <c r="R27" t="s">
+        <v>103</v>
+      </c>
+      <c r="T27">
+        <v>7</v>
       </c>
       <c r="U27" t="s">
         <v>43</v>
@@ -1545,8 +1845,14 @@
       <c r="W27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z27">
+        <v>5</v>
+      </c>
+      <c r="AA27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>10</v>
       </c>
@@ -1557,19 +1863,34 @@
         <v>6</v>
       </c>
       <c r="F28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G28" t="s">
+        <v>93</v>
+      </c>
+      <c r="H28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" t="s">
+        <v>106</v>
+      </c>
+      <c r="L28">
+        <v>10</v>
+      </c>
+      <c r="M28" t="s">
+        <v>25</v>
+      </c>
+      <c r="N28" t="s">
         <v>94</v>
       </c>
-      <c r="I28">
-        <v>10</v>
-      </c>
-      <c r="J28" t="s">
-        <v>25</v>
-      </c>
-      <c r="K28" t="s">
-        <v>95</v>
+      <c r="Q28" t="s">
+        <v>99</v>
+      </c>
+      <c r="R28" t="s">
+        <v>101</v>
+      </c>
+      <c r="T28">
+        <v>3</v>
       </c>
       <c r="U28" t="s">
         <v>44</v>
@@ -1580,8 +1901,17 @@
       <c r="W28">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z28">
+        <v>6</v>
+      </c>
+      <c r="AA28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T29">
+        <v>10</v>
+      </c>
       <c r="U29" t="s">
         <v>45</v>
       </c>
@@ -1591,8 +1921,17 @@
       <c r="W29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z29">
+        <v>3</v>
+      </c>
+      <c r="AA29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T30">
+        <v>8</v>
+      </c>
       <c r="U30" t="s">
         <v>46</v>
       </c>
@@ -1602,8 +1941,17 @@
       <c r="W30">
         <v>178</v>
       </c>
-    </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z30">
+        <v>178</v>
+      </c>
+      <c r="AA30">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T31">
+        <v>8</v>
+      </c>
       <c r="U31" t="s">
         <v>47</v>
       </c>
@@ -1613,8 +1961,17 @@
       <c r="W31">
         <v>178</v>
       </c>
-    </row>
-    <row r="32" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Z31">
+        <v>178</v>
+      </c>
+      <c r="AA31">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T32">
+        <v>10</v>
+      </c>
       <c r="U32" t="s">
         <v>48</v>
       </c>
@@ -1624,8 +1981,55 @@
       <c r="W32">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z32">
+        <v>4</v>
+      </c>
+      <c r="AA32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" t="s">
+        <v>116</v>
+      </c>
+      <c r="G33" t="s">
+        <v>117</v>
+      </c>
+      <c r="H33" t="s">
+        <v>118</v>
+      </c>
+      <c r="K33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" t="s">
+        <v>112</v>
+      </c>
+      <c r="F34" t="s">
+        <v>98</v>
+      </c>
+      <c r="J34" t="s">
+        <v>98</v>
+      </c>
+      <c r="T34">
+        <v>3</v>
+      </c>
       <c r="U34" t="s">
         <v>49</v>
       </c>
@@ -1635,8 +2039,38 @@
       <c r="W34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z34">
+        <v>1</v>
+      </c>
+      <c r="AA34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" t="s">
+        <v>97</v>
+      </c>
+      <c r="G35" t="s">
+        <v>119</v>
+      </c>
+      <c r="H35" t="s">
+        <v>120</v>
+      </c>
+      <c r="J35" t="s">
+        <v>97</v>
+      </c>
+      <c r="T35">
+        <v>7</v>
+      </c>
       <c r="U35" t="s">
         <v>50</v>
       </c>
@@ -1646,8 +2080,17 @@
       <c r="W35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z35">
+        <v>1</v>
+      </c>
+      <c r="AA35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T36">
+        <v>3</v>
+      </c>
       <c r="U36" t="s">
         <v>52</v>
       </c>
@@ -1657,8 +2100,17 @@
       <c r="W36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z36">
+        <v>1</v>
+      </c>
+      <c r="AA36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T37">
+        <v>20</v>
+      </c>
       <c r="U37" t="s">
         <v>85</v>
       </c>
@@ -1668,8 +2120,17 @@
       <c r="W37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z37">
+        <v>3</v>
+      </c>
+      <c r="AA37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T38">
+        <v>20</v>
+      </c>
       <c r="U38" t="s">
         <v>86</v>
       </c>
@@ -1679,8 +2140,17 @@
       <c r="W38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z38">
+        <v>3</v>
+      </c>
+      <c r="AA38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T39">
+        <v>21</v>
+      </c>
       <c r="U39" t="s">
         <v>87</v>
       </c>
@@ -1690,8 +2160,17 @@
       <c r="W39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z39">
+        <v>2</v>
+      </c>
+      <c r="AA39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T40">
+        <v>21</v>
+      </c>
       <c r="U40" t="s">
         <v>88</v>
       </c>
@@ -1701,8 +2180,20 @@
       <c r="W40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z40">
+        <v>2</v>
+      </c>
+      <c r="AA40">
+        <v>1</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T41">
+        <v>14</v>
+      </c>
       <c r="U41" t="s">
         <v>53</v>
       </c>
@@ -1712,11 +2203,17 @@
       <c r="W41">
         <v>16</v>
       </c>
-      <c r="Z41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z41">
+        <v>15</v>
+      </c>
+      <c r="AA41">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T43">
+        <v>14</v>
+      </c>
       <c r="U43" t="s">
         <v>54</v>
       </c>
@@ -1726,8 +2223,17 @@
       <c r="W43">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z43">
+        <v>5</v>
+      </c>
+      <c r="AA43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T44">
+        <v>10</v>
+      </c>
       <c r="U44" t="s">
         <v>55</v>
       </c>
@@ -1737,8 +2243,17 @@
       <c r="W44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z44">
+        <v>5</v>
+      </c>
+      <c r="AA44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T45">
+        <v>18</v>
+      </c>
       <c r="U45" t="s">
         <v>56</v>
       </c>
@@ -1748,8 +2263,20 @@
       <c r="W45">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z45">
+        <v>5</v>
+      </c>
+      <c r="AA45">
+        <v>5</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T46">
+        <v>15</v>
+      </c>
       <c r="U46" t="s">
         <v>57</v>
       </c>
@@ -1759,11 +2286,17 @@
       <c r="W46">
         <v>18</v>
       </c>
-      <c r="Z46" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="48" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z46">
+        <v>17</v>
+      </c>
+      <c r="AA46">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="T48">
+        <v>3</v>
+      </c>
       <c r="U48" t="s">
         <v>59</v>
       </c>
@@ -1773,8 +2306,20 @@
       <c r="W48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z48">
+        <v>1</v>
+      </c>
+      <c r="AA48">
+        <v>2</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T49">
+        <v>11</v>
+      </c>
       <c r="U49" t="s">
         <v>60</v>
       </c>
@@ -1784,11 +2329,17 @@
       <c r="W49">
         <v>3</v>
       </c>
-      <c r="Z49" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z49">
+        <v>2</v>
+      </c>
+      <c r="AA49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T50">
+        <v>14</v>
+      </c>
       <c r="U50" t="s">
         <v>61</v>
       </c>
@@ -1798,8 +2349,20 @@
       <c r="W50">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z50">
+        <v>2</v>
+      </c>
+      <c r="AA50">
+        <v>2</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T51">
+        <v>11</v>
+      </c>
       <c r="U51" t="s">
         <v>62</v>
       </c>
@@ -1809,11 +2372,17 @@
       <c r="W51">
         <v>3</v>
       </c>
-      <c r="Z51" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="52" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z51">
+        <v>2</v>
+      </c>
+      <c r="AA51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T52">
+        <v>16</v>
+      </c>
       <c r="U52" t="s">
         <v>63</v>
       </c>
@@ -1823,8 +2392,20 @@
       <c r="W52">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z52">
+        <v>4</v>
+      </c>
+      <c r="AA52">
+        <v>4</v>
+      </c>
+      <c r="AD52" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T53">
+        <v>11</v>
+      </c>
       <c r="U53" t="s">
         <v>64</v>
       </c>
@@ -1834,11 +2415,17 @@
       <c r="W53">
         <v>2</v>
       </c>
-      <c r="Z53" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="54" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z53">
+        <v>2</v>
+      </c>
+      <c r="AA53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T54">
+        <v>16</v>
+      </c>
       <c r="U54" t="s">
         <v>65</v>
       </c>
@@ -1848,8 +2435,17 @@
       <c r="W54">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z54">
+        <v>4</v>
+      </c>
+      <c r="AA54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T55">
+        <v>16</v>
+      </c>
       <c r="U55" t="s">
         <v>66</v>
       </c>
@@ -1859,8 +2455,20 @@
       <c r="W55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z55">
+        <v>3</v>
+      </c>
+      <c r="AA55">
+        <v>3</v>
+      </c>
+      <c r="AD55" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T56">
+        <v>8</v>
+      </c>
       <c r="U56" t="s">
         <v>67</v>
       </c>
@@ -1870,11 +2478,17 @@
       <c r="W56">
         <v>15</v>
       </c>
-      <c r="Z56" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="57" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z56">
+        <v>15</v>
+      </c>
+      <c r="AA56">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T57">
+        <v>19</v>
+      </c>
       <c r="U57" t="s">
         <v>68</v>
       </c>
@@ -1884,8 +2498,17 @@
       <c r="W57">
         <v>31</v>
       </c>
-    </row>
-    <row r="58" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z57">
+        <v>32</v>
+      </c>
+      <c r="AA57">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T58">
+        <v>17</v>
+      </c>
       <c r="U58" t="s">
         <v>69</v>
       </c>
@@ -1895,8 +2518,17 @@
       <c r="W58">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z58">
+        <v>4</v>
+      </c>
+      <c r="AA58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T59">
+        <v>17</v>
+      </c>
       <c r="U59" t="s">
         <v>70</v>
       </c>
@@ -1906,8 +2538,22 @@
       <c r="W59">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z59">
+        <v>4</v>
+      </c>
+      <c r="AA59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="AD60" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T61">
+        <v>15</v>
+      </c>
       <c r="U61" t="s">
         <v>71</v>
       </c>
@@ -1917,26 +2563,41 @@
       <c r="W61">
         <v>13</v>
       </c>
-      <c r="Z61" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="63" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="Z61">
+        <v>12</v>
+      </c>
+      <c r="AA61">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T63">
+        <v>4</v>
+      </c>
       <c r="U63" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="21:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="20:30" x14ac:dyDescent="0.25">
+      <c r="T64">
+        <v>3</v>
+      </c>
       <c r="U64" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="20:21" x14ac:dyDescent="0.25">
+      <c r="T65">
+        <v>3</v>
+      </c>
       <c r="U65" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="20:21" x14ac:dyDescent="0.25">
+      <c r="T66">
+        <v>4</v>
+      </c>
       <c r="U66" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Moved memoryInfo out of sketch, extended benchmark functionality and created call by reference median function
</commit_message>
<xml_diff>
--- a/BenchmarkDocs/Results.xlsx
+++ b/BenchmarkDocs/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f0dc99f0b729840/Teilen/edge-ml/feature-extraction/BenchmarkDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E4B3007-A998-4A4A-BFA6-5F773B1A229E}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA44EA29-9033-4AB0-AE79-19D3134E8FBF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="125">
   <si>
     <t>Arduino</t>
   </si>
@@ -400,6 +400,15 @@
   </si>
   <si>
     <t>Max Datengröße (extractAll)</t>
+  </si>
+  <si>
+    <t>352/3072</t>
+  </si>
+  <si>
+    <t>11676/48056</t>
+  </si>
+  <si>
+    <t>980*8/36380 = 21.5%</t>
   </si>
 </sst>
 </file>
@@ -753,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B09DA97-D620-4F66-8E45-7C0B77C13B9B}">
   <dimension ref="B1:AD66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,8 +2033,17 @@
       <c r="F34" t="s">
         <v>98</v>
       </c>
+      <c r="G34" t="s">
+        <v>122</v>
+      </c>
+      <c r="H34" t="s">
+        <v>123</v>
+      </c>
       <c r="J34" t="s">
         <v>98</v>
+      </c>
+      <c r="K34" t="s">
+        <v>124</v>
       </c>
       <c r="T34">
         <v>3</v>

</xml_diff>

<commit_message>
Initialize values with pointer, added more benchmarking results
</commit_message>
<xml_diff>
--- a/BenchmarkDocs/Results.xlsx
+++ b/BenchmarkDocs/Results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f0dc99f0b729840/Teilen/edge-ml/feature-extraction/BenchmarkDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA44EA29-9033-4AB0-AE79-19D3134E8FBF}"/>
+  <xr:revisionPtr revIDLastSave="342" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C7025E1-C50C-4A71-9E37-CCC61C5E5AE3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
+    <workbookView xWindow="13875" yWindow="150" windowWidth="14670" windowHeight="14280" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="325">
   <si>
     <t>Arduino</t>
   </si>
@@ -372,9 +373,6 @@
     <t>299816/527616 (56%)</t>
   </si>
   <si>
-    <t>16232/48056 (25%)</t>
-  </si>
-  <si>
     <t>330448/983040 (33%)</t>
   </si>
   <si>
@@ -409,6 +407,609 @@
   </si>
   <si>
     <t>980*8/36380 = 21.5%</t>
+  </si>
+  <si>
+    <t>Leerer Sketch</t>
+  </si>
+  <si>
+    <t>43252/527616 (8%)</t>
+  </si>
+  <si>
+    <t>9752/64288 (15%)</t>
+  </si>
+  <si>
+    <t>Serial begin</t>
+  </si>
+  <si>
+    <t>Memory Info</t>
+  </si>
+  <si>
+    <t>43316/527616 (8%)</t>
+  </si>
+  <si>
+    <t>44444/527616 (8%)</t>
+  </si>
+  <si>
+    <t>16232/64288 (25%)</t>
+  </si>
+  <si>
+    <t>62772/527616 (8%)</t>
+  </si>
+  <si>
+    <t>9840/64288 (15%)</t>
+  </si>
+  <si>
+    <t>260/54536</t>
+  </si>
+  <si>
+    <t>11668/54448</t>
+  </si>
+  <si>
+    <t>Data in Header</t>
+  </si>
+  <si>
+    <t>Mit Data_100</t>
+  </si>
+  <si>
+    <t>11748/54448</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mit 1*Data_10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mit 2*Data_10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mit 3*Data_10 </t>
+  </si>
+  <si>
+    <t>11828/54448</t>
+  </si>
+  <si>
+    <t>63156/527616 (11%)</t>
+  </si>
+  <si>
+    <t>11908/54448</t>
+  </si>
+  <si>
+    <t>12708/54448</t>
+  </si>
+  <si>
+    <t>20708/54448</t>
+  </si>
+  <si>
+    <t>63220/527616 (11%)</t>
+  </si>
+  <si>
+    <t>Mit 1*Data_1000</t>
+  </si>
+  <si>
+    <t>Mit 4*Data_1000</t>
+  </si>
+  <si>
+    <t>44708/54448</t>
+  </si>
+  <si>
+    <t>63248/527616 (11%)</t>
+  </si>
+  <si>
+    <t>Mit 5*Data_1000</t>
+  </si>
+  <si>
+    <t>Overflow</t>
+  </si>
+  <si>
+    <t>Stand: 31.01.</t>
+  </si>
+  <si>
+    <t>31.01. Lauf1</t>
+  </si>
+  <si>
+    <t>31.01. Lauf2</t>
+  </si>
+  <si>
+    <t>01.02. Lauf1</t>
+  </si>
+  <si>
+    <t>01.02. Lauf2</t>
+  </si>
+  <si>
+    <t>02.02. Lauf1</t>
+  </si>
+  <si>
+    <t>02.02. Lauf2</t>
+  </si>
+  <si>
+    <t>Neu: Pointer</t>
+  </si>
+  <si>
+    <t>710151 µs</t>
+  </si>
+  <si>
+    <t>710023 µs</t>
+  </si>
+  <si>
+    <t>709897 µs</t>
+  </si>
+  <si>
+    <t>710090 µs</t>
+  </si>
+  <si>
+    <t>710035 µs</t>
+  </si>
+  <si>
+    <t>709909 µs</t>
+  </si>
+  <si>
+    <t>709944 µs</t>
+  </si>
+  <si>
+    <t>709940 µs</t>
+  </si>
+  <si>
+    <t>710416 µs</t>
+  </si>
+  <si>
+    <t>710356 µs</t>
+  </si>
+  <si>
+    <t>646743 µs</t>
+  </si>
+  <si>
+    <t>646708 µs</t>
+  </si>
+  <si>
+    <t>646588 µs</t>
+  </si>
+  <si>
+    <t>646512 µs</t>
+  </si>
+  <si>
+    <t>646796 µs</t>
+  </si>
+  <si>
+    <t>646774 µs</t>
+  </si>
+  <si>
+    <t>646795 µs</t>
+  </si>
+  <si>
+    <t>646801 µs</t>
+  </si>
+  <si>
+    <t>646736 µs</t>
+  </si>
+  <si>
+    <t>646543 µs</t>
+  </si>
+  <si>
+    <t>348602 µs</t>
+  </si>
+  <si>
+    <t>348504 µs</t>
+  </si>
+  <si>
+    <t>348622 µs</t>
+  </si>
+  <si>
+    <t>348671 µs</t>
+  </si>
+  <si>
+    <t>348547 µs</t>
+  </si>
+  <si>
+    <t>348649 µs</t>
+  </si>
+  <si>
+    <t>348501 µs</t>
+  </si>
+  <si>
+    <t>348626 µs</t>
+  </si>
+  <si>
+    <t>348506 µs</t>
+  </si>
+  <si>
+    <t>348524 µs</t>
+  </si>
+  <si>
+    <t>318178 µs</t>
+  </si>
+  <si>
+    <t>318054 µs</t>
+  </si>
+  <si>
+    <t>318285 µs</t>
+  </si>
+  <si>
+    <t>318189 µs</t>
+  </si>
+  <si>
+    <t>318206 µs</t>
+  </si>
+  <si>
+    <t>318171 µs</t>
+  </si>
+  <si>
+    <t>318377 µs</t>
+  </si>
+  <si>
+    <t>318200 µs</t>
+  </si>
+  <si>
+    <t>318055 µs</t>
+  </si>
+  <si>
+    <t>318152 µs</t>
+  </si>
+  <si>
+    <t>336272 µs</t>
+  </si>
+  <si>
+    <t>336334 µs</t>
+  </si>
+  <si>
+    <t>336337 µs</t>
+  </si>
+  <si>
+    <t>336202 µs</t>
+  </si>
+  <si>
+    <t>336323 µs</t>
+  </si>
+  <si>
+    <t>336314 µs</t>
+  </si>
+  <si>
+    <t>336255 µs</t>
+  </si>
+  <si>
+    <t>336282 µs</t>
+  </si>
+  <si>
+    <t>336300 µs</t>
+  </si>
+  <si>
+    <t>336296 µs</t>
+  </si>
+  <si>
+    <t>308093 µs</t>
+  </si>
+  <si>
+    <t>308170 µs</t>
+  </si>
+  <si>
+    <t>308165 µs</t>
+  </si>
+  <si>
+    <t>307893 µs</t>
+  </si>
+  <si>
+    <t>308153 µs</t>
+  </si>
+  <si>
+    <t>308144 µs</t>
+  </si>
+  <si>
+    <t>308109 µs</t>
+  </si>
+  <si>
+    <t>308118 µs</t>
+  </si>
+  <si>
+    <t>308175 µs</t>
+  </si>
+  <si>
+    <t>308131 µs</t>
+  </si>
+  <si>
+    <t>682122 µs</t>
+  </si>
+  <si>
+    <t>682167 µs</t>
+  </si>
+  <si>
+    <t>682250 µs</t>
+  </si>
+  <si>
+    <t>681873 µs</t>
+  </si>
+  <si>
+    <t>682075 µs</t>
+  </si>
+  <si>
+    <t>681653 µs</t>
+  </si>
+  <si>
+    <t>682146 µs</t>
+  </si>
+  <si>
+    <t>682145 µs</t>
+  </si>
+  <si>
+    <t>682037 µs</t>
+  </si>
+  <si>
+    <t>682225 µs</t>
+  </si>
+  <si>
+    <t>623863 µs</t>
+  </si>
+  <si>
+    <t>624164 µs</t>
+  </si>
+  <si>
+    <t>624151 µs</t>
+  </si>
+  <si>
+    <t>624051 µs</t>
+  </si>
+  <si>
+    <t>623815 µs</t>
+  </si>
+  <si>
+    <t>624116 µs</t>
+  </si>
+  <si>
+    <t>624148 µs</t>
+  </si>
+  <si>
+    <t>624134 µs</t>
+  </si>
+  <si>
+    <t>624101 µs</t>
+  </si>
+  <si>
+    <t>623799 µs</t>
+  </si>
+  <si>
+    <t>1639 µs</t>
+  </si>
+  <si>
+    <t>4630 µs</t>
+  </si>
+  <si>
+    <t>52201 µs</t>
+  </si>
+  <si>
+    <t>15579 µs</t>
+  </si>
+  <si>
+    <t>19193 µs</t>
+  </si>
+  <si>
+    <t>18477 µs</t>
+  </si>
+  <si>
+    <t>33520 µs</t>
+  </si>
+  <si>
+    <t>5822 µs</t>
+  </si>
+  <si>
+    <t>4641 µs</t>
+  </si>
+  <si>
+    <t>5741 µs</t>
+  </si>
+  <si>
+    <t>2914 µs</t>
+  </si>
+  <si>
+    <t>181033 µs</t>
+  </si>
+  <si>
+    <t>181693 µs</t>
+  </si>
+  <si>
+    <t>4074 µs</t>
+  </si>
+  <si>
+    <t>1303 µs</t>
+  </si>
+  <si>
+    <t>1194 µs</t>
+  </si>
+  <si>
+    <t>1150 µs</t>
+  </si>
+  <si>
+    <t>2829 µs</t>
+  </si>
+  <si>
+    <t>2704 µs</t>
+  </si>
+  <si>
+    <t>1709 µs</t>
+  </si>
+  <si>
+    <t>1204 µs</t>
+  </si>
+  <si>
+    <t>16089 µs</t>
+  </si>
+  <si>
+    <t>5007 µs</t>
+  </si>
+  <si>
+    <t>5298 µs</t>
+  </si>
+  <si>
+    <t>5098 µs</t>
+  </si>
+  <si>
+    <t>17526 µs</t>
+  </si>
+  <si>
+    <t>1653 µs</t>
+  </si>
+  <si>
+    <t>2774 µs</t>
+  </si>
+  <si>
+    <t>2944 µs</t>
+  </si>
+  <si>
+    <t>2278 µs</t>
+  </si>
+  <si>
+    <t>2098 µs</t>
+  </si>
+  <si>
+    <t>3882 µs</t>
+  </si>
+  <si>
+    <t>3696 µs</t>
+  </si>
+  <si>
+    <t>2930 µs</t>
+  </si>
+  <si>
+    <t>15644 µs</t>
+  </si>
+  <si>
+    <t>31208 µs</t>
+  </si>
+  <si>
+    <t>3562 µs</t>
+  </si>
+  <si>
+    <t>3449 µs</t>
+  </si>
+  <si>
+    <t>12547 µs</t>
+  </si>
+  <si>
+    <t>105728 µs</t>
+  </si>
+  <si>
+    <t>6454577 µs</t>
+  </si>
+  <si>
+    <t>9137022 µs</t>
+  </si>
+  <si>
+    <t>17405915 µs</t>
+  </si>
+  <si>
+    <t>105697 µs</t>
+  </si>
+  <si>
+    <t>6754891 µs</t>
+  </si>
+  <si>
+    <t>9151238 µs</t>
+  </si>
+  <si>
+    <t>17193792 µs</t>
+  </si>
+  <si>
+    <t>5006 µs</t>
+  </si>
+  <si>
+    <t>51232 µs</t>
+  </si>
+  <si>
+    <t>18071 µs</t>
+  </si>
+  <si>
+    <t>21733 µs</t>
+  </si>
+  <si>
+    <t>20745 µs</t>
+  </si>
+  <si>
+    <t>38519 µs</t>
+  </si>
+  <si>
+    <t>6425 µs</t>
+  </si>
+  <si>
+    <t>5010 µs</t>
+  </si>
+  <si>
+    <t>6402 µs</t>
+  </si>
+  <si>
+    <t>3002 µs</t>
+  </si>
+  <si>
+    <t>180421 µs</t>
+  </si>
+  <si>
+    <t>181140 µs</t>
+  </si>
+  <si>
+    <t>4475 µs</t>
+  </si>
+  <si>
+    <t>1239 µs</t>
+  </si>
+  <si>
+    <t>1236 µs</t>
+  </si>
+  <si>
+    <t>1120 µs</t>
+  </si>
+  <si>
+    <t>2657 µs</t>
+  </si>
+  <si>
+    <t>2763 µs</t>
+  </si>
+  <si>
+    <t>1181 µs</t>
+  </si>
+  <si>
+    <t>1733 µs</t>
+  </si>
+  <si>
+    <t>18755 µs</t>
+  </si>
+  <si>
+    <t>5013 µs</t>
+  </si>
+  <si>
+    <t>5246 µs</t>
+  </si>
+  <si>
+    <t>20116 µs</t>
+  </si>
+  <si>
+    <t>1575 µs</t>
+  </si>
+  <si>
+    <t>2761 µs</t>
+  </si>
+  <si>
+    <t>2865 µs</t>
+  </si>
+  <si>
+    <t>2306 µs</t>
+  </si>
+  <si>
+    <t>3934 µs</t>
+  </si>
+  <si>
+    <t>3739 µs</t>
+  </si>
+  <si>
+    <t>2116 µs</t>
+  </si>
+  <si>
+    <t>3113 µs</t>
+  </si>
+  <si>
+    <t>18096 µs</t>
+  </si>
+  <si>
+    <t>36332 µs</t>
+  </si>
+  <si>
+    <t>3544 µs</t>
+  </si>
+  <si>
+    <t>3455 µs</t>
   </si>
 </sst>
 </file>
@@ -762,13 +1363,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B09DA97-D620-4F66-8E45-7C0B77C13B9B}">
   <dimension ref="B1:AD66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AB47" sqref="AB47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
@@ -1999,7 +2600,7 @@
     </row>
     <row r="33" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C33" t="s">
         <v>109</v>
@@ -2008,16 +2609,16 @@
         <v>110</v>
       </c>
       <c r="F33" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33" t="s">
         <v>116</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>117</v>
       </c>
-      <c r="H33" t="s">
-        <v>118</v>
-      </c>
       <c r="K33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="2:30" x14ac:dyDescent="0.25">
@@ -2028,22 +2629,22 @@
         <v>111</v>
       </c>
       <c r="D34" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="F34" t="s">
         <v>98</v>
       </c>
       <c r="G34" t="s">
+        <v>121</v>
+      </c>
+      <c r="H34" t="s">
         <v>122</v>
-      </c>
-      <c r="H34" t="s">
-        <v>123</v>
       </c>
       <c r="J34" t="s">
         <v>98</v>
       </c>
       <c r="K34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T34">
         <v>3</v>
@@ -2069,19 +2670,19 @@
         <v>97</v>
       </c>
       <c r="C35" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" t="s">
         <v>113</v>
-      </c>
-      <c r="D35" t="s">
-        <v>114</v>
       </c>
       <c r="F35" t="s">
         <v>97</v>
       </c>
       <c r="G35" t="s">
+        <v>118</v>
+      </c>
+      <c r="H35" t="s">
         <v>119</v>
-      </c>
-      <c r="H35" t="s">
-        <v>120</v>
       </c>
       <c r="J35" t="s">
         <v>97</v>
@@ -2166,6 +2767,18 @@
       </c>
     </row>
     <row r="39" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" t="s">
+        <v>117</v>
+      </c>
       <c r="T39">
         <v>21</v>
       </c>
@@ -2186,6 +2799,15 @@
       </c>
     </row>
     <row r="40" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" t="s">
+        <v>126</v>
+      </c>
       <c r="T40">
         <v>21</v>
       </c>
@@ -2209,6 +2831,15 @@
       </c>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" t="s">
+        <v>126</v>
+      </c>
       <c r="T41">
         <v>14</v>
       </c>
@@ -2228,7 +2859,33 @@
         <v>16</v>
       </c>
     </row>
+    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" t="s">
+        <v>134</v>
+      </c>
+    </row>
     <row r="43" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" t="s">
+        <v>135</v>
+      </c>
       <c r="T43">
         <v>14</v>
       </c>
@@ -2249,6 +2906,18 @@
       </c>
     </row>
     <row r="44" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>139</v>
+      </c>
+      <c r="C44" t="s">
+        <v>143</v>
+      </c>
+      <c r="D44" t="s">
+        <v>133</v>
+      </c>
+      <c r="E44" t="s">
+        <v>138</v>
+      </c>
       <c r="T44">
         <v>10</v>
       </c>
@@ -2269,6 +2938,18 @@
       </c>
     </row>
     <row r="45" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45" t="s">
+        <v>133</v>
+      </c>
+      <c r="E45" t="s">
+        <v>142</v>
+      </c>
       <c r="T45">
         <v>18</v>
       </c>
@@ -2292,6 +2973,18 @@
       </c>
     </row>
     <row r="46" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" t="s">
+        <v>143</v>
+      </c>
+      <c r="D46" t="s">
+        <v>133</v>
+      </c>
+      <c r="E46" t="s">
+        <v>144</v>
+      </c>
       <c r="T46">
         <v>15</v>
       </c>
@@ -2311,7 +3004,33 @@
         <v>17</v>
       </c>
     </row>
+    <row r="47" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" t="s">
+        <v>133</v>
+      </c>
+      <c r="E47" t="s">
+        <v>145</v>
+      </c>
+    </row>
     <row r="48" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" t="s">
+        <v>147</v>
+      </c>
+      <c r="D48" t="s">
+        <v>133</v>
+      </c>
+      <c r="E48" t="s">
+        <v>146</v>
+      </c>
       <c r="T48">
         <v>3</v>
       </c>
@@ -2334,7 +3053,19 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>149</v>
+      </c>
+      <c r="C49" t="s">
+        <v>151</v>
+      </c>
+      <c r="D49" t="s">
+        <v>133</v>
+      </c>
+      <c r="E49" t="s">
+        <v>150</v>
+      </c>
       <c r="T49">
         <v>11</v>
       </c>
@@ -2354,7 +3085,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" t="s">
+        <v>151</v>
+      </c>
+      <c r="D50" t="s">
+        <v>133</v>
+      </c>
+      <c r="E50" t="s">
+        <v>153</v>
+      </c>
       <c r="T50">
         <v>14</v>
       </c>
@@ -2377,7 +3120,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T51">
         <v>11</v>
       </c>
@@ -2397,7 +3140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T52">
         <v>16</v>
       </c>
@@ -2420,7 +3163,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T53">
         <v>11</v>
       </c>
@@ -2440,7 +3183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T54">
         <v>16</v>
       </c>
@@ -2460,7 +3203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T55">
         <v>16</v>
       </c>
@@ -2483,7 +3226,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T56">
         <v>8</v>
       </c>
@@ -2503,7 +3246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T57">
         <v>19</v>
       </c>
@@ -2523,7 +3266,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T58">
         <v>17</v>
       </c>
@@ -2543,7 +3286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T59">
         <v>17</v>
       </c>
@@ -2563,12 +3306,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:30" x14ac:dyDescent="0.25">
       <c r="AD60" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T61">
         <v>15</v>
       </c>
@@ -2588,7 +3331,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T63">
         <v>4</v>
       </c>
@@ -2596,7 +3339,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="20:30" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T64">
         <v>3</v>
       </c>
@@ -2624,4 +3367,937 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DC238C-8F4B-441F-9A1D-B395F114E22E}">
+  <dimension ref="B2:AE52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="P23" workbookViewId="0">
+      <selection activeCell="S45" sqref="S45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="18" max="18" width="23.5703125" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" customWidth="1"/>
+    <col min="31" max="31" width="39.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" t="s">
+        <v>97</v>
+      </c>
+      <c r="R3" t="s">
+        <v>89</v>
+      </c>
+      <c r="S3" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" t="s">
+        <v>155</v>
+      </c>
+      <c r="T4" t="s">
+        <v>156</v>
+      </c>
+      <c r="U4" t="s">
+        <v>157</v>
+      </c>
+      <c r="V4" t="s">
+        <v>158</v>
+      </c>
+      <c r="W4" t="s">
+        <v>159</v>
+      </c>
+      <c r="X4" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G5" t="s">
+        <v>202</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>172</v>
+      </c>
+      <c r="L5" t="s">
+        <v>162</v>
+      </c>
+      <c r="M5" t="s">
+        <v>232</v>
+      </c>
+      <c r="N5" t="s">
+        <v>222</v>
+      </c>
+      <c r="R5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" t="s">
+        <v>242</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" t="s">
+        <v>213</v>
+      </c>
+      <c r="G6" t="s">
+        <v>203</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>173</v>
+      </c>
+      <c r="L6" t="s">
+        <v>163</v>
+      </c>
+      <c r="M6" t="s">
+        <v>233</v>
+      </c>
+      <c r="N6" t="s">
+        <v>223</v>
+      </c>
+      <c r="R6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" t="s">
+        <v>289</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" t="s">
+        <v>204</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
+        <v>174</v>
+      </c>
+      <c r="L7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M7" t="s">
+        <v>234</v>
+      </c>
+      <c r="N7" t="s">
+        <v>224</v>
+      </c>
+      <c r="R7" t="s">
+        <v>37</v>
+      </c>
+      <c r="S7" t="s">
+        <v>290</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>195</v>
+      </c>
+      <c r="E8" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" t="s">
+        <v>215</v>
+      </c>
+      <c r="G8" t="s">
+        <v>205</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8" t="s">
+        <v>175</v>
+      </c>
+      <c r="L8" t="s">
+        <v>165</v>
+      </c>
+      <c r="M8" t="s">
+        <v>235</v>
+      </c>
+      <c r="N8" t="s">
+        <v>225</v>
+      </c>
+      <c r="R8" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" t="s">
+        <v>291</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F9" t="s">
+        <v>216</v>
+      </c>
+      <c r="G9" t="s">
+        <v>206</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9" t="s">
+        <v>176</v>
+      </c>
+      <c r="L9" t="s">
+        <v>166</v>
+      </c>
+      <c r="M9" t="s">
+        <v>236</v>
+      </c>
+      <c r="N9" t="s">
+        <v>226</v>
+      </c>
+      <c r="R9" t="s">
+        <v>39</v>
+      </c>
+      <c r="S9" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" t="s">
+        <v>187</v>
+      </c>
+      <c r="F10" t="s">
+        <v>217</v>
+      </c>
+      <c r="G10" t="s">
+        <v>207</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+      <c r="K10" t="s">
+        <v>177</v>
+      </c>
+      <c r="L10" t="s">
+        <v>167</v>
+      </c>
+      <c r="M10" t="s">
+        <v>237</v>
+      </c>
+      <c r="N10" t="s">
+        <v>227</v>
+      </c>
+      <c r="R10" t="s">
+        <v>40</v>
+      </c>
+      <c r="S10" t="s">
+        <v>293</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" t="s">
+        <v>218</v>
+      </c>
+      <c r="G11" t="s">
+        <v>208</v>
+      </c>
+      <c r="J11">
+        <v>7</v>
+      </c>
+      <c r="K11" t="s">
+        <v>178</v>
+      </c>
+      <c r="L11" t="s">
+        <v>168</v>
+      </c>
+      <c r="M11" t="s">
+        <v>238</v>
+      </c>
+      <c r="N11" t="s">
+        <v>228</v>
+      </c>
+      <c r="R11" t="s">
+        <v>41</v>
+      </c>
+      <c r="S11" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" t="s">
+        <v>189</v>
+      </c>
+      <c r="F12" t="s">
+        <v>219</v>
+      </c>
+      <c r="G12" t="s">
+        <v>209</v>
+      </c>
+      <c r="J12">
+        <v>8</v>
+      </c>
+      <c r="K12" t="s">
+        <v>179</v>
+      </c>
+      <c r="L12" t="s">
+        <v>169</v>
+      </c>
+      <c r="M12" t="s">
+        <v>239</v>
+      </c>
+      <c r="N12" t="s">
+        <v>229</v>
+      </c>
+      <c r="R12" t="s">
+        <v>42</v>
+      </c>
+      <c r="S12" t="s">
+        <v>295</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" t="s">
+        <v>190</v>
+      </c>
+      <c r="F13" t="s">
+        <v>220</v>
+      </c>
+      <c r="G13" t="s">
+        <v>210</v>
+      </c>
+      <c r="J13">
+        <v>9</v>
+      </c>
+      <c r="K13" t="s">
+        <v>180</v>
+      </c>
+      <c r="L13" t="s">
+        <v>170</v>
+      </c>
+      <c r="M13" t="s">
+        <v>240</v>
+      </c>
+      <c r="N13" t="s">
+        <v>230</v>
+      </c>
+      <c r="R13" t="s">
+        <v>43</v>
+      </c>
+      <c r="S13" t="s">
+        <v>296</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>201</v>
+      </c>
+      <c r="E14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F14" t="s">
+        <v>221</v>
+      </c>
+      <c r="G14" t="s">
+        <v>211</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14" t="s">
+        <v>181</v>
+      </c>
+      <c r="L14" t="s">
+        <v>171</v>
+      </c>
+      <c r="M14" t="s">
+        <v>241</v>
+      </c>
+      <c r="N14" t="s">
+        <v>231</v>
+      </c>
+      <c r="R14" t="s">
+        <v>44</v>
+      </c>
+      <c r="S14" t="s">
+        <v>297</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="R15" t="s">
+        <v>45</v>
+      </c>
+      <c r="S15" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="R16" t="s">
+        <v>46</v>
+      </c>
+      <c r="S16" t="s">
+        <v>299</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="17" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R17" t="s">
+        <v>47</v>
+      </c>
+      <c r="S17" t="s">
+        <v>300</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R18" t="s">
+        <v>48</v>
+      </c>
+      <c r="S18" t="s">
+        <v>301</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="20" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R20" t="s">
+        <v>49</v>
+      </c>
+      <c r="S20" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R21" t="s">
+        <v>50</v>
+      </c>
+      <c r="S21" t="s">
+        <v>303</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R22" t="s">
+        <v>52</v>
+      </c>
+      <c r="S22" t="s">
+        <v>304</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R23" t="s">
+        <v>85</v>
+      </c>
+      <c r="S23" t="s">
+        <v>306</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="24" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R24" t="s">
+        <v>86</v>
+      </c>
+      <c r="S24" t="s">
+        <v>305</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R25" t="s">
+        <v>87</v>
+      </c>
+      <c r="S25" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R26" t="s">
+        <v>88</v>
+      </c>
+      <c r="S26" t="s">
+        <v>307</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R27" t="s">
+        <v>53</v>
+      </c>
+      <c r="S27" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="29" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R29" t="s">
+        <v>54</v>
+      </c>
+      <c r="S29" t="s">
+        <v>310</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="30" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R30" t="s">
+        <v>55</v>
+      </c>
+      <c r="S30" t="s">
+        <v>311</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="31" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R31" t="s">
+        <v>56</v>
+      </c>
+      <c r="S31" t="s">
+        <v>310</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R32" t="s">
+        <v>57</v>
+      </c>
+      <c r="S32" t="s">
+        <v>312</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="34" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R34" t="s">
+        <v>59</v>
+      </c>
+      <c r="S34" t="s">
+        <v>313</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>268</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R35" t="s">
+        <v>60</v>
+      </c>
+      <c r="S35" t="s">
+        <v>314</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="36" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R36" t="s">
+        <v>61</v>
+      </c>
+      <c r="S36" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>270</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R37" t="s">
+        <v>62</v>
+      </c>
+      <c r="S37" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="38" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R38" t="s">
+        <v>63</v>
+      </c>
+      <c r="S38" t="s">
+        <v>317</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>273</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R39" t="s">
+        <v>64</v>
+      </c>
+      <c r="S39" t="s">
+        <v>319</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="40" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R40" t="s">
+        <v>65</v>
+      </c>
+      <c r="S40" t="s">
+        <v>318</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="41" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R41" t="s">
+        <v>66</v>
+      </c>
+      <c r="S41" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>275</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R42" t="s">
+        <v>67</v>
+      </c>
+      <c r="S42" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="43" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R43" t="s">
+        <v>68</v>
+      </c>
+      <c r="S43" t="s">
+        <v>322</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="44" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R44" t="s">
+        <v>69</v>
+      </c>
+      <c r="S44" t="s">
+        <v>323</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="45" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R45" t="s">
+        <v>70</v>
+      </c>
+      <c r="S45" t="s">
+        <v>324</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="46" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="AE46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="R47" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="49" spans="18:25" x14ac:dyDescent="0.25">
+      <c r="R49" t="s">
+        <v>72</v>
+      </c>
+      <c r="S49" t="s">
+        <v>288</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="50" spans="18:25" x14ac:dyDescent="0.25">
+      <c r="R50" t="s">
+        <v>73</v>
+      </c>
+      <c r="S50" t="s">
+        <v>285</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="51" spans="18:25" x14ac:dyDescent="0.25">
+      <c r="R51" t="s">
+        <v>74</v>
+      </c>
+      <c r="S51" t="s">
+        <v>286</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="52" spans="18:25" x14ac:dyDescent="0.25">
+      <c r="R52" t="s">
+        <v>75</v>
+      </c>
+      <c r="S52" t="s">
+        <v>287</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>283</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More Datasets, new benchmarks
</commit_message>
<xml_diff>
--- a/BenchmarkDocs/Results.xlsx
+++ b/BenchmarkDocs/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f0dc99f0b729840/Teilen/edge-ml/feature-extraction/BenchmarkDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="342" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C7025E1-C50C-4A71-9E37-CCC61C5E5AE3}"/>
+  <xr:revisionPtr revIDLastSave="702" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E545AD2-9E33-4C95-B3B9-1D4BCDEB7E56}"/>
   <bookViews>
-    <workbookView xWindow="13875" yWindow="150" windowWidth="14670" windowHeight="14280" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="169">
   <si>
     <t>Arduino</t>
   </si>
@@ -502,524 +502,77 @@
     <t>Stand: 31.01.</t>
   </si>
   <si>
-    <t>31.01. Lauf1</t>
-  </si>
-  <si>
-    <t>31.01. Lauf2</t>
-  </si>
-  <si>
-    <t>01.02. Lauf1</t>
-  </si>
-  <si>
-    <t>01.02. Lauf2</t>
-  </si>
-  <si>
-    <t>02.02. Lauf1</t>
-  </si>
-  <si>
-    <t>02.02. Lauf2</t>
-  </si>
-  <si>
     <t>Neu: Pointer</t>
   </si>
   <si>
-    <t>710151 µs</t>
-  </si>
-  <si>
-    <t>710023 µs</t>
-  </si>
-  <si>
-    <t>709897 µs</t>
-  </si>
-  <si>
-    <t>710090 µs</t>
-  </si>
-  <si>
-    <t>710035 µs</t>
-  </si>
-  <si>
-    <t>709909 µs</t>
-  </si>
-  <si>
-    <t>709944 µs</t>
-  </si>
-  <si>
-    <t>709940 µs</t>
-  </si>
-  <si>
-    <t>710416 µs</t>
-  </si>
-  <si>
-    <t>710356 µs</t>
-  </si>
-  <si>
-    <t>646743 µs</t>
-  </si>
-  <si>
-    <t>646708 µs</t>
-  </si>
-  <si>
-    <t>646588 µs</t>
-  </si>
-  <si>
-    <t>646512 µs</t>
-  </si>
-  <si>
-    <t>646796 µs</t>
-  </si>
-  <si>
-    <t>646774 µs</t>
-  </si>
-  <si>
-    <t>646795 µs</t>
-  </si>
-  <si>
-    <t>646801 µs</t>
-  </si>
-  <si>
-    <t>646736 µs</t>
-  </si>
-  <si>
-    <t>646543 µs</t>
-  </si>
-  <si>
-    <t>348602 µs</t>
-  </si>
-  <si>
-    <t>348504 µs</t>
-  </si>
-  <si>
-    <t>348622 µs</t>
-  </si>
-  <si>
-    <t>348671 µs</t>
-  </si>
-  <si>
-    <t>348547 µs</t>
-  </si>
-  <si>
-    <t>348649 µs</t>
-  </si>
-  <si>
-    <t>348501 µs</t>
-  </si>
-  <si>
-    <t>348626 µs</t>
-  </si>
-  <si>
-    <t>348506 µs</t>
-  </si>
-  <si>
-    <t>348524 µs</t>
-  </si>
-  <si>
-    <t>318178 µs</t>
-  </si>
-  <si>
-    <t>318054 µs</t>
-  </si>
-  <si>
-    <t>318285 µs</t>
-  </si>
-  <si>
-    <t>318189 µs</t>
-  </si>
-  <si>
-    <t>318206 µs</t>
-  </si>
-  <si>
-    <t>318171 µs</t>
-  </si>
-  <si>
-    <t>318377 µs</t>
-  </si>
-  <si>
-    <t>318200 µs</t>
-  </si>
-  <si>
-    <t>318055 µs</t>
-  </si>
-  <si>
-    <t>318152 µs</t>
-  </si>
-  <si>
-    <t>336272 µs</t>
-  </si>
-  <si>
-    <t>336334 µs</t>
-  </si>
-  <si>
-    <t>336337 µs</t>
-  </si>
-  <si>
-    <t>336202 µs</t>
-  </si>
-  <si>
-    <t>336323 µs</t>
-  </si>
-  <si>
-    <t>336314 µs</t>
-  </si>
-  <si>
-    <t>336255 µs</t>
-  </si>
-  <si>
-    <t>336282 µs</t>
-  </si>
-  <si>
-    <t>336300 µs</t>
-  </si>
-  <si>
-    <t>336296 µs</t>
-  </si>
-  <si>
-    <t>308093 µs</t>
-  </si>
-  <si>
-    <t>308170 µs</t>
-  </si>
-  <si>
-    <t>308165 µs</t>
-  </si>
-  <si>
-    <t>307893 µs</t>
-  </si>
-  <si>
-    <t>308153 µs</t>
-  </si>
-  <si>
-    <t>308144 µs</t>
-  </si>
-  <si>
-    <t>308109 µs</t>
-  </si>
-  <si>
-    <t>308118 µs</t>
-  </si>
-  <si>
-    <t>308175 µs</t>
-  </si>
-  <si>
-    <t>308131 µs</t>
-  </si>
-  <si>
-    <t>682122 µs</t>
-  </si>
-  <si>
-    <t>682167 µs</t>
-  </si>
-  <si>
-    <t>682250 µs</t>
-  </si>
-  <si>
-    <t>681873 µs</t>
-  </si>
-  <si>
-    <t>682075 µs</t>
-  </si>
-  <si>
-    <t>681653 µs</t>
-  </si>
-  <si>
-    <t>682146 µs</t>
-  </si>
-  <si>
-    <t>682145 µs</t>
-  </si>
-  <si>
-    <t>682037 µs</t>
-  </si>
-  <si>
-    <t>682225 µs</t>
-  </si>
-  <si>
-    <t>623863 µs</t>
-  </si>
-  <si>
-    <t>624164 µs</t>
-  </si>
-  <si>
-    <t>624151 µs</t>
-  </si>
-  <si>
-    <t>624051 µs</t>
-  </si>
-  <si>
-    <t>623815 µs</t>
-  </si>
-  <si>
-    <t>624116 µs</t>
-  </si>
-  <si>
-    <t>624148 µs</t>
-  </si>
-  <si>
-    <t>624134 µs</t>
-  </si>
-  <si>
-    <t>624101 µs</t>
-  </si>
-  <si>
-    <t>623799 µs</t>
-  </si>
-  <si>
-    <t>1639 µs</t>
-  </si>
-  <si>
-    <t>4630 µs</t>
-  </si>
-  <si>
-    <t>52201 µs</t>
-  </si>
-  <si>
-    <t>15579 µs</t>
-  </si>
-  <si>
-    <t>19193 µs</t>
-  </si>
-  <si>
-    <t>18477 µs</t>
-  </si>
-  <si>
-    <t>33520 µs</t>
-  </si>
-  <si>
-    <t>5822 µs</t>
-  </si>
-  <si>
-    <t>4641 µs</t>
-  </si>
-  <si>
-    <t>5741 µs</t>
-  </si>
-  <si>
-    <t>2914 µs</t>
-  </si>
-  <si>
-    <t>181033 µs</t>
-  </si>
-  <si>
-    <t>181693 µs</t>
-  </si>
-  <si>
-    <t>4074 µs</t>
-  </si>
-  <si>
-    <t>1303 µs</t>
-  </si>
-  <si>
-    <t>1194 µs</t>
-  </si>
-  <si>
-    <t>1150 µs</t>
-  </si>
-  <si>
-    <t>2829 µs</t>
-  </si>
-  <si>
-    <t>2704 µs</t>
-  </si>
-  <si>
-    <t>1709 µs</t>
-  </si>
-  <si>
-    <t>1204 µs</t>
-  </si>
-  <si>
-    <t>16089 µs</t>
-  </si>
-  <si>
-    <t>5007 µs</t>
-  </si>
-  <si>
-    <t>5298 µs</t>
-  </si>
-  <si>
-    <t>5098 µs</t>
-  </si>
-  <si>
-    <t>17526 µs</t>
-  </si>
-  <si>
-    <t>1653 µs</t>
-  </si>
-  <si>
-    <t>2774 µs</t>
-  </si>
-  <si>
-    <t>2944 µs</t>
-  </si>
-  <si>
-    <t>2278 µs</t>
-  </si>
-  <si>
-    <t>2098 µs</t>
-  </si>
-  <si>
-    <t>3882 µs</t>
-  </si>
-  <si>
-    <t>3696 µs</t>
-  </si>
-  <si>
-    <t>2930 µs</t>
-  </si>
-  <si>
-    <t>15644 µs</t>
-  </si>
-  <si>
-    <t>31208 µs</t>
-  </si>
-  <si>
-    <t>3562 µs</t>
-  </si>
-  <si>
-    <t>3449 µs</t>
-  </si>
-  <si>
-    <t>12547 µs</t>
-  </si>
-  <si>
-    <t>105728 µs</t>
-  </si>
-  <si>
-    <t>6454577 µs</t>
-  </si>
-  <si>
-    <t>9137022 µs</t>
-  </si>
-  <si>
-    <t>17405915 µs</t>
-  </si>
-  <si>
-    <t>105697 µs</t>
-  </si>
-  <si>
-    <t>6754891 µs</t>
-  </si>
-  <si>
-    <t>9151238 µs</t>
-  </si>
-  <si>
-    <t>17193792 µs</t>
-  </si>
-  <si>
-    <t>5006 µs</t>
-  </si>
-  <si>
-    <t>51232 µs</t>
-  </si>
-  <si>
-    <t>18071 µs</t>
-  </si>
-  <si>
-    <t>21733 µs</t>
-  </si>
-  <si>
-    <t>20745 µs</t>
-  </si>
-  <si>
-    <t>38519 µs</t>
-  </si>
-  <si>
-    <t>6425 µs</t>
-  </si>
-  <si>
-    <t>5010 µs</t>
-  </si>
-  <si>
-    <t>6402 µs</t>
-  </si>
-  <si>
-    <t>3002 µs</t>
-  </si>
-  <si>
-    <t>180421 µs</t>
-  </si>
-  <si>
-    <t>181140 µs</t>
-  </si>
-  <si>
-    <t>4475 µs</t>
-  </si>
-  <si>
-    <t>1239 µs</t>
-  </si>
-  <si>
-    <t>1236 µs</t>
-  </si>
-  <si>
-    <t>1120 µs</t>
-  </si>
-  <si>
-    <t>2657 µs</t>
-  </si>
-  <si>
-    <t>2763 µs</t>
-  </si>
-  <si>
-    <t>1181 µs</t>
-  </si>
-  <si>
-    <t>1733 µs</t>
-  </si>
-  <si>
-    <t>18755 µs</t>
-  </si>
-  <si>
-    <t>5013 µs</t>
-  </si>
-  <si>
-    <t>5246 µs</t>
-  </si>
-  <si>
-    <t>20116 µs</t>
-  </si>
-  <si>
-    <t>1575 µs</t>
-  </si>
-  <si>
-    <t>2761 µs</t>
-  </si>
-  <si>
-    <t>2865 µs</t>
-  </si>
-  <si>
-    <t>2306 µs</t>
-  </si>
-  <si>
-    <t>3934 µs</t>
-  </si>
-  <si>
-    <t>3739 µs</t>
-  </si>
-  <si>
-    <t>2116 µs</t>
-  </si>
-  <si>
-    <t>3113 µs</t>
-  </si>
-  <si>
-    <t>18096 µs</t>
-  </si>
-  <si>
-    <t>36332 µs</t>
-  </si>
-  <si>
-    <t>3544 µs</t>
-  </si>
-  <si>
-    <t>3455 µs</t>
+    <t xml:space="preserve">31.01. </t>
+  </si>
+  <si>
+    <t>01.02.</t>
+  </si>
+  <si>
+    <t>02.02.</t>
+  </si>
+  <si>
+    <t>03.02.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04.02. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">05.02. </t>
+  </si>
+  <si>
+    <t>Stand: 01.02.</t>
+  </si>
+  <si>
+    <t>Neu:Exclude</t>
+  </si>
+  <si>
+    <t>Summe Zeiten</t>
+  </si>
+  <si>
+    <t>Zeiten in µs</t>
+  </si>
+  <si>
+    <t>100 Werte</t>
+  </si>
+  <si>
+    <t>1500 Werte</t>
+  </si>
+  <si>
+    <t>Averages</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1045,8 +598,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1363,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B09DA97-D620-4F66-8E45-7C0B77C13B9B}">
   <dimension ref="B1:AD66"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AB47" sqref="AB47"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3371,10 +2926,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DC238C-8F4B-441F-9A1D-B395F114E22E}">
-  <dimension ref="B2:AE52"/>
+  <dimension ref="A1:AS54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P23" workbookViewId="0">
-      <selection activeCell="S45" sqref="S45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3384,35 +2939,35 @@
     <col min="12" max="12" width="13" customWidth="1"/>
     <col min="14" max="14" width="12.5703125" customWidth="1"/>
     <col min="16" max="16" width="13.140625" customWidth="1"/>
-    <col min="18" max="18" width="23.5703125" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
     <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" customWidth="1"/>
     <col min="30" max="30" width="12.140625" customWidth="1"/>
-    <col min="31" max="31" width="39.42578125" customWidth="1"/>
+    <col min="31" max="31" width="9.5703125" customWidth="1"/>
+    <col min="32" max="32" width="23.5703125" customWidth="1"/>
+    <col min="45" max="45" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="2:31" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
+      <c r="J3" t="s">
         <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" t="s">
-        <v>97</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1</v>
       </c>
       <c r="K3" t="s">
         <v>96</v>
@@ -3420,35 +2975,29 @@
       <c r="M3" t="s">
         <v>97</v>
       </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
       <c r="R3" t="s">
+        <v>96</v>
+      </c>
+      <c r="T3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF3" t="s">
         <v>89</v>
       </c>
-      <c r="S3" t="s">
+      <c r="AG3" t="s">
         <v>98</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AM3" t="s">
         <v>97</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AS3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
-      </c>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
         <v>5</v>
       </c>
@@ -3464,840 +3013,1948 @@
       <c r="N4" t="s">
         <v>4</v>
       </c>
+      <c r="Q4" t="s">
+        <v>5</v>
+      </c>
       <c r="R4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF4" t="s">
         <v>34</v>
       </c>
-      <c r="S4" t="s">
-        <v>155</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="AG4" t="s">
         <v>156</v>
       </c>
-      <c r="U4" t="s">
+      <c r="AH4" t="s">
         <v>157</v>
       </c>
-      <c r="V4" t="s">
+      <c r="AI4" t="s">
         <v>158</v>
       </c>
-      <c r="W4" t="s">
+      <c r="AJ4" t="s">
         <v>159</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AK4" t="s">
         <v>160</v>
       </c>
-      <c r="Y4" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="AL4" t="s">
+        <v>161</v>
+      </c>
+      <c r="AM4" t="s">
         <v>156</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AN4" t="s">
         <v>157</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AO4" t="s">
         <v>158</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AP4" t="s">
         <v>159</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AQ4" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>192</v>
-      </c>
-      <c r="E5" t="s">
-        <v>182</v>
-      </c>
-      <c r="F5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G5" t="s">
-        <v>202</v>
-      </c>
+      <c r="AR4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J5">
         <v>1</v>
       </c>
-      <c r="K5" t="s">
-        <v>172</v>
-      </c>
-      <c r="L5" t="s">
-        <v>162</v>
-      </c>
-      <c r="M5" t="s">
-        <v>232</v>
-      </c>
-      <c r="N5" t="s">
-        <v>222</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="K5">
+        <v>318178</v>
+      </c>
+      <c r="L5">
+        <v>348602</v>
+      </c>
+      <c r="M5">
+        <v>308093</v>
+      </c>
+      <c r="N5">
+        <v>336272</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>646743</v>
+      </c>
+      <c r="S5">
+        <v>710151</v>
+      </c>
+      <c r="T5">
+        <v>623863</v>
+      </c>
+      <c r="U5">
+        <v>682122</v>
+      </c>
+      <c r="AF5" t="s">
         <v>35</v>
       </c>
-      <c r="S5" t="s">
-        <v>242</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>193</v>
-      </c>
-      <c r="E6" t="s">
-        <v>183</v>
-      </c>
-      <c r="F6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G6" t="s">
-        <v>203</v>
-      </c>
+      <c r="AG5">
+        <v>1639</v>
+      </c>
+      <c r="AH5">
+        <v>1626</v>
+      </c>
+      <c r="AM5">
+        <v>1639</v>
+      </c>
+      <c r="AN5">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J6">
         <v>2</v>
       </c>
-      <c r="K6" t="s">
-        <v>173</v>
-      </c>
-      <c r="L6" t="s">
-        <v>163</v>
-      </c>
-      <c r="M6" t="s">
-        <v>233</v>
-      </c>
-      <c r="N6" t="s">
-        <v>223</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="K6">
+        <v>318054</v>
+      </c>
+      <c r="L6">
+        <v>348504</v>
+      </c>
+      <c r="M6">
+        <v>308170</v>
+      </c>
+      <c r="N6">
+        <v>336334</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>646708</v>
+      </c>
+      <c r="S6">
+        <v>710023</v>
+      </c>
+      <c r="T6">
+        <v>624164</v>
+      </c>
+      <c r="U6">
+        <v>682167</v>
+      </c>
+      <c r="AF6" t="s">
         <v>36</v>
       </c>
-      <c r="S6" t="s">
-        <v>289</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>194</v>
-      </c>
-      <c r="E7" t="s">
-        <v>184</v>
-      </c>
-      <c r="F7" t="s">
-        <v>214</v>
-      </c>
-      <c r="G7" t="s">
-        <v>204</v>
-      </c>
+      <c r="AG6">
+        <v>5006</v>
+      </c>
+      <c r="AH6">
+        <v>5197</v>
+      </c>
+      <c r="AM6">
+        <v>4630</v>
+      </c>
+      <c r="AN6">
+        <v>4628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J7">
         <v>3</v>
       </c>
-      <c r="K7" t="s">
-        <v>174</v>
-      </c>
-      <c r="L7" t="s">
-        <v>164</v>
-      </c>
-      <c r="M7" t="s">
-        <v>234</v>
-      </c>
-      <c r="N7" t="s">
-        <v>224</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="K7">
+        <v>318285</v>
+      </c>
+      <c r="L7">
+        <v>348622</v>
+      </c>
+      <c r="M7">
+        <v>308165</v>
+      </c>
+      <c r="N7">
+        <v>336337</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="R7">
+        <v>646588</v>
+      </c>
+      <c r="S7">
+        <v>709897</v>
+      </c>
+      <c r="T7">
+        <v>624151</v>
+      </c>
+      <c r="U7">
+        <v>682250</v>
+      </c>
+      <c r="AF7" t="s">
         <v>37</v>
       </c>
-      <c r="S7" t="s">
-        <v>290</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>195</v>
-      </c>
-      <c r="E8" t="s">
-        <v>185</v>
-      </c>
-      <c r="F8" t="s">
-        <v>215</v>
-      </c>
-      <c r="G8" t="s">
-        <v>205</v>
-      </c>
+      <c r="AG7">
+        <v>51232</v>
+      </c>
+      <c r="AH7">
+        <v>51639</v>
+      </c>
+      <c r="AM7">
+        <v>52201</v>
+      </c>
+      <c r="AN7">
+        <v>52873</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J8">
         <v>4</v>
       </c>
-      <c r="K8" t="s">
-        <v>175</v>
-      </c>
-      <c r="L8" t="s">
-        <v>165</v>
-      </c>
-      <c r="M8" t="s">
-        <v>235</v>
-      </c>
-      <c r="N8" t="s">
-        <v>225</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="K8">
+        <v>318189</v>
+      </c>
+      <c r="L8">
+        <v>348671</v>
+      </c>
+      <c r="M8">
+        <v>307893</v>
+      </c>
+      <c r="N8">
+        <v>336202</v>
+      </c>
+      <c r="Q8">
+        <v>4</v>
+      </c>
+      <c r="R8">
+        <v>646512</v>
+      </c>
+      <c r="S8">
+        <v>710090</v>
+      </c>
+      <c r="T8">
+        <v>624051</v>
+      </c>
+      <c r="U8">
+        <v>681873</v>
+      </c>
+      <c r="AF8" t="s">
         <v>38</v>
       </c>
-      <c r="S8" t="s">
-        <v>291</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>196</v>
-      </c>
-      <c r="E9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F9" t="s">
-        <v>216</v>
-      </c>
-      <c r="G9" t="s">
-        <v>206</v>
-      </c>
+      <c r="AG8">
+        <v>18071</v>
+      </c>
+      <c r="AH8">
+        <v>17160</v>
+      </c>
+      <c r="AM8">
+        <v>15579</v>
+      </c>
+      <c r="AN8">
+        <v>15766</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J9">
         <v>5</v>
       </c>
-      <c r="K9" t="s">
-        <v>176</v>
-      </c>
-      <c r="L9" t="s">
-        <v>166</v>
-      </c>
-      <c r="M9" t="s">
-        <v>236</v>
-      </c>
-      <c r="N9" t="s">
-        <v>226</v>
-      </c>
-      <c r="R9" t="s">
+      <c r="K9">
+        <v>318206</v>
+      </c>
+      <c r="L9">
+        <v>348547</v>
+      </c>
+      <c r="M9">
+        <v>308153</v>
+      </c>
+      <c r="N9">
+        <v>336323</v>
+      </c>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="R9">
+        <v>646796</v>
+      </c>
+      <c r="S9">
+        <v>710035</v>
+      </c>
+      <c r="T9">
+        <v>623815</v>
+      </c>
+      <c r="U9">
+        <v>682075</v>
+      </c>
+      <c r="AF9" t="s">
         <v>39</v>
       </c>
-      <c r="S9" t="s">
-        <v>292</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E10" t="s">
-        <v>187</v>
-      </c>
-      <c r="F10" t="s">
-        <v>217</v>
-      </c>
-      <c r="G10" t="s">
-        <v>207</v>
-      </c>
+      <c r="AG9">
+        <v>21733</v>
+      </c>
+      <c r="AH9">
+        <v>20716</v>
+      </c>
+      <c r="AM9">
+        <v>19193</v>
+      </c>
+      <c r="AN9">
+        <v>19348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J10">
         <v>6</v>
       </c>
-      <c r="K10" t="s">
-        <v>177</v>
-      </c>
-      <c r="L10" t="s">
-        <v>167</v>
-      </c>
-      <c r="M10" t="s">
-        <v>237</v>
-      </c>
-      <c r="N10" t="s">
-        <v>227</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="K10">
+        <v>318171</v>
+      </c>
+      <c r="L10">
+        <v>348649</v>
+      </c>
+      <c r="M10">
+        <v>308144</v>
+      </c>
+      <c r="N10">
+        <v>336314</v>
+      </c>
+      <c r="Q10">
+        <v>6</v>
+      </c>
+      <c r="R10">
+        <v>646774</v>
+      </c>
+      <c r="S10">
+        <v>709909</v>
+      </c>
+      <c r="T10">
+        <v>624116</v>
+      </c>
+      <c r="U10">
+        <v>681653</v>
+      </c>
+      <c r="AF10" t="s">
         <v>40</v>
       </c>
-      <c r="S10" t="s">
-        <v>293</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E11" t="s">
-        <v>188</v>
-      </c>
-      <c r="F11" t="s">
-        <v>218</v>
-      </c>
-      <c r="G11" t="s">
-        <v>208</v>
-      </c>
+      <c r="AG10">
+        <v>20745</v>
+      </c>
+      <c r="AH10">
+        <v>19860</v>
+      </c>
+      <c r="AM10">
+        <v>18477</v>
+      </c>
+      <c r="AN10">
+        <v>18687</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J11">
         <v>7</v>
       </c>
-      <c r="K11" t="s">
-        <v>178</v>
-      </c>
-      <c r="L11" t="s">
-        <v>168</v>
-      </c>
-      <c r="M11" t="s">
-        <v>238</v>
-      </c>
-      <c r="N11" t="s">
-        <v>228</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="K11">
+        <v>318377</v>
+      </c>
+      <c r="L11">
+        <v>348501</v>
+      </c>
+      <c r="M11">
+        <v>308109</v>
+      </c>
+      <c r="N11">
+        <v>336255</v>
+      </c>
+      <c r="Q11">
+        <v>7</v>
+      </c>
+      <c r="R11">
+        <v>646795</v>
+      </c>
+      <c r="S11">
+        <v>709944</v>
+      </c>
+      <c r="T11">
+        <v>624148</v>
+      </c>
+      <c r="U11">
+        <v>682146</v>
+      </c>
+      <c r="AF11" t="s">
         <v>41</v>
       </c>
-      <c r="S11" t="s">
-        <v>294</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>199</v>
-      </c>
-      <c r="E12" t="s">
-        <v>189</v>
-      </c>
-      <c r="F12" t="s">
-        <v>219</v>
-      </c>
-      <c r="G12" t="s">
-        <v>209</v>
-      </c>
+      <c r="AG11">
+        <v>38519</v>
+      </c>
+      <c r="AH11">
+        <v>36629</v>
+      </c>
+      <c r="AM11">
+        <v>33520</v>
+      </c>
+      <c r="AN11">
+        <v>33835</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J12">
         <v>8</v>
       </c>
-      <c r="K12" t="s">
-        <v>179</v>
-      </c>
-      <c r="L12" t="s">
-        <v>169</v>
-      </c>
-      <c r="M12" t="s">
-        <v>239</v>
-      </c>
-      <c r="N12" t="s">
-        <v>229</v>
-      </c>
-      <c r="R12" t="s">
+      <c r="K12">
+        <v>318200</v>
+      </c>
+      <c r="L12">
+        <v>348626</v>
+      </c>
+      <c r="M12">
+        <v>308118</v>
+      </c>
+      <c r="N12">
+        <v>336282</v>
+      </c>
+      <c r="Q12">
+        <v>8</v>
+      </c>
+      <c r="R12">
+        <v>646801</v>
+      </c>
+      <c r="S12">
+        <v>709940</v>
+      </c>
+      <c r="T12">
+        <v>624134</v>
+      </c>
+      <c r="U12">
+        <v>682145</v>
+      </c>
+      <c r="AF12" t="s">
         <v>42</v>
       </c>
-      <c r="S12" t="s">
-        <v>295</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E13" t="s">
-        <v>190</v>
-      </c>
-      <c r="F13" t="s">
-        <v>220</v>
-      </c>
-      <c r="G13" t="s">
-        <v>210</v>
-      </c>
+      <c r="AG12">
+        <v>6425</v>
+      </c>
+      <c r="AH12">
+        <v>6179</v>
+      </c>
+      <c r="AM12">
+        <v>5822</v>
+      </c>
+      <c r="AN12">
+        <v>5845</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J13">
         <v>9</v>
       </c>
-      <c r="K13" t="s">
-        <v>180</v>
-      </c>
-      <c r="L13" t="s">
-        <v>170</v>
-      </c>
-      <c r="M13" t="s">
-        <v>240</v>
-      </c>
-      <c r="N13" t="s">
-        <v>230</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="K13">
+        <v>318055</v>
+      </c>
+      <c r="L13">
+        <v>348506</v>
+      </c>
+      <c r="M13">
+        <v>308175</v>
+      </c>
+      <c r="N13">
+        <v>336300</v>
+      </c>
+      <c r="Q13">
+        <v>9</v>
+      </c>
+      <c r="R13">
+        <v>646736</v>
+      </c>
+      <c r="S13">
+        <v>710416</v>
+      </c>
+      <c r="T13">
+        <v>624101</v>
+      </c>
+      <c r="U13">
+        <v>682037</v>
+      </c>
+      <c r="AF13" t="s">
         <v>43</v>
       </c>
-      <c r="S13" t="s">
-        <v>296</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>201</v>
-      </c>
-      <c r="E14" t="s">
-        <v>191</v>
-      </c>
-      <c r="F14" t="s">
-        <v>221</v>
-      </c>
-      <c r="G14" t="s">
-        <v>211</v>
-      </c>
+      <c r="AG13">
+        <v>5010</v>
+      </c>
+      <c r="AH13">
+        <v>5203</v>
+      </c>
+      <c r="AM13">
+        <v>4641</v>
+      </c>
+      <c r="AN13">
+        <v>4694</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J14">
         <v>10</v>
       </c>
-      <c r="K14" t="s">
-        <v>181</v>
-      </c>
-      <c r="L14" t="s">
-        <v>171</v>
-      </c>
-      <c r="M14" t="s">
-        <v>241</v>
-      </c>
-      <c r="N14" t="s">
-        <v>231</v>
-      </c>
-      <c r="R14" t="s">
+      <c r="K14">
+        <v>318152</v>
+      </c>
+      <c r="L14">
+        <v>348524</v>
+      </c>
+      <c r="M14">
+        <v>308131</v>
+      </c>
+      <c r="N14">
+        <v>336296</v>
+      </c>
+      <c r="Q14">
+        <v>10</v>
+      </c>
+      <c r="R14">
+        <v>646543</v>
+      </c>
+      <c r="S14">
+        <v>710356</v>
+      </c>
+      <c r="T14">
+        <v>623799</v>
+      </c>
+      <c r="U14">
+        <v>682225</v>
+      </c>
+      <c r="AF14" t="s">
         <v>44</v>
       </c>
-      <c r="S14" t="s">
-        <v>297</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="15" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="R15" t="s">
+      <c r="AG14">
+        <v>6402</v>
+      </c>
+      <c r="AH14">
+        <v>6169</v>
+      </c>
+      <c r="AM14">
+        <v>5741</v>
+      </c>
+      <c r="AN14">
+        <v>5824</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AF15" t="s">
         <v>45</v>
       </c>
-      <c r="S15" t="s">
-        <v>298</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="R16" t="s">
+      <c r="AG15">
+        <v>3002</v>
+      </c>
+      <c r="AH15">
+        <v>3022</v>
+      </c>
+      <c r="AM15">
+        <v>2914</v>
+      </c>
+      <c r="AN15">
+        <v>2778</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K16">
+        <f>AVERAGE(K5:K14)</f>
+        <v>318186.7</v>
+      </c>
+      <c r="L16">
+        <f>AVERAGE(L5:L14)</f>
+        <v>348575.2</v>
+      </c>
+      <c r="M16">
+        <f>AVERAGE(M5:M14)</f>
+        <v>308115.09999999998</v>
+      </c>
+      <c r="N16">
+        <f>AVERAGE(N5:N14)</f>
+        <v>336291.5</v>
+      </c>
+      <c r="R16">
+        <f>AVERAGE(R5:R14)</f>
+        <v>646699.6</v>
+      </c>
+      <c r="S16">
+        <f>AVERAGE(S5:S14)</f>
+        <v>710076.1</v>
+      </c>
+      <c r="T16">
+        <f>AVERAGE(T5:T14)</f>
+        <v>624034.19999999995</v>
+      </c>
+      <c r="U16">
+        <f>AVERAGE(U5:U14)</f>
+        <v>682069.3</v>
+      </c>
+      <c r="AF16" t="s">
         <v>46</v>
       </c>
-      <c r="S16" t="s">
-        <v>299</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="17" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R17" t="s">
+      <c r="AG16">
+        <v>180421</v>
+      </c>
+      <c r="AH16">
+        <v>178078</v>
+      </c>
+      <c r="AM16">
+        <v>181033</v>
+      </c>
+      <c r="AN16">
+        <v>181761</v>
+      </c>
+    </row>
+    <row r="17" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AF17" t="s">
         <v>47</v>
       </c>
-      <c r="S17" t="s">
-        <v>300</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="18" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R18" t="s">
+      <c r="AG17">
+        <v>181140</v>
+      </c>
+      <c r="AH17">
+        <v>178906</v>
+      </c>
+      <c r="AM17">
+        <v>181693</v>
+      </c>
+      <c r="AN17">
+        <v>182843</v>
+      </c>
+    </row>
+    <row r="18" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF18" t="s">
         <v>48</v>
       </c>
-      <c r="S18" t="s">
-        <v>301</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="20" spans="18:31" x14ac:dyDescent="0.25">
+      <c r="AG18">
+        <v>4475</v>
+      </c>
+      <c r="AH18">
+        <v>4325</v>
+      </c>
+      <c r="AM18">
+        <v>4074</v>
+      </c>
+      <c r="AN18">
+        <v>4067</v>
+      </c>
+    </row>
+    <row r="19" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" t="s">
+        <v>97</v>
+      </c>
+      <c r="J19" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" t="s">
+        <v>96</v>
+      </c>
+      <c r="M19" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
+        <v>96</v>
+      </c>
+      <c r="T19" t="s">
+        <v>97</v>
+      </c>
+      <c r="X19" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" t="s">
+        <v>3</v>
+      </c>
+      <c r="L20" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>5</v>
+      </c>
       <c r="R20" t="s">
+        <v>3</v>
+      </c>
+      <c r="S20" t="s">
+        <v>4</v>
+      </c>
+      <c r="T20" t="s">
+        <v>3</v>
+      </c>
+      <c r="U20" t="s">
+        <v>4</v>
+      </c>
+      <c r="X20" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF20" t="s">
         <v>49</v>
       </c>
-      <c r="S20" t="s">
-        <v>302</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="21" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R21" t="s">
+      <c r="AG20">
+        <v>1239</v>
+      </c>
+      <c r="AH20">
+        <v>1235</v>
+      </c>
+      <c r="AM20">
+        <v>1303</v>
+      </c>
+      <c r="AN20">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="21" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>65548</v>
+      </c>
+      <c r="E21">
+        <v>70984</v>
+      </c>
+      <c r="F21">
+        <v>64512</v>
+      </c>
+      <c r="G21">
+        <v>69824</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>312440</v>
+      </c>
+      <c r="L21">
+        <v>341885</v>
+      </c>
+      <c r="M21">
+        <v>311123</v>
+      </c>
+      <c r="N21">
+        <v>338788</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>633599</v>
+      </c>
+      <c r="S21">
+        <v>694962</v>
+      </c>
+      <c r="T21">
+        <v>630182</v>
+      </c>
+      <c r="U21">
+        <v>688722</v>
+      </c>
+      <c r="X21">
+        <v>1</v>
+      </c>
+      <c r="Y21">
+        <v>955387</v>
+      </c>
+      <c r="Z21">
+        <v>1048922</v>
+      </c>
+      <c r="AA21">
+        <v>950177</v>
+      </c>
+      <c r="AB21">
+        <v>1037941</v>
+      </c>
+      <c r="AF21" t="s">
         <v>50</v>
       </c>
-      <c r="S21" t="s">
-        <v>303</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="22" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R22" t="s">
+      <c r="AG21">
+        <v>1236</v>
+      </c>
+      <c r="AH21">
+        <v>1154</v>
+      </c>
+      <c r="AM21">
+        <v>1194</v>
+      </c>
+      <c r="AN21">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="22" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>65521</v>
+      </c>
+      <c r="E22">
+        <v>71019</v>
+      </c>
+      <c r="F22">
+        <v>64395</v>
+      </c>
+      <c r="G22">
+        <v>69938</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>312342</v>
+      </c>
+      <c r="L22">
+        <v>341963</v>
+      </c>
+      <c r="M22">
+        <v>311279</v>
+      </c>
+      <c r="N22">
+        <v>339559</v>
+      </c>
+      <c r="Q22">
+        <v>2</v>
+      </c>
+      <c r="R22">
+        <v>633595</v>
+      </c>
+      <c r="S22">
+        <v>695081</v>
+      </c>
+      <c r="T22">
+        <v>630087</v>
+      </c>
+      <c r="U22">
+        <v>689691</v>
+      </c>
+      <c r="X22">
+        <v>2</v>
+      </c>
+      <c r="Y22">
+        <v>955341</v>
+      </c>
+      <c r="Z22">
+        <v>1049119</v>
+      </c>
+      <c r="AA22">
+        <v>948832</v>
+      </c>
+      <c r="AB22">
+        <v>1036980</v>
+      </c>
+      <c r="AF22" t="s">
         <v>52</v>
       </c>
-      <c r="S22" t="s">
-        <v>304</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="23" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R23" t="s">
+      <c r="AG22">
+        <v>1120</v>
+      </c>
+      <c r="AH22">
+        <v>1110</v>
+      </c>
+      <c r="AM22">
+        <v>1150</v>
+      </c>
+      <c r="AN22">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="23" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>65522</v>
+      </c>
+      <c r="E23">
+        <v>70991</v>
+      </c>
+      <c r="F23">
+        <v>64467</v>
+      </c>
+      <c r="G23">
+        <v>69946</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <v>312342</v>
+      </c>
+      <c r="L23">
+        <v>341885</v>
+      </c>
+      <c r="M23">
+        <v>311316</v>
+      </c>
+      <c r="N23">
+        <v>339230</v>
+      </c>
+      <c r="Q23">
+        <v>3</v>
+      </c>
+      <c r="R23">
+        <v>633605</v>
+      </c>
+      <c r="S23">
+        <v>694757</v>
+      </c>
+      <c r="T23">
+        <v>630480</v>
+      </c>
+      <c r="U23">
+        <v>688558</v>
+      </c>
+      <c r="X23">
+        <v>3</v>
+      </c>
+      <c r="Y23">
+        <v>955336</v>
+      </c>
+      <c r="Z23">
+        <v>1049266</v>
+      </c>
+      <c r="AA23">
+        <v>949162</v>
+      </c>
+      <c r="AB23">
+        <v>1037777</v>
+      </c>
+      <c r="AF23" t="s">
         <v>85</v>
       </c>
-      <c r="S23" t="s">
-        <v>306</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="24" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R24" t="s">
+      <c r="AG23">
+        <v>2763</v>
+      </c>
+      <c r="AH23">
+        <v>2748</v>
+      </c>
+      <c r="AM23">
+        <v>2829</v>
+      </c>
+      <c r="AN23">
+        <v>2846</v>
+      </c>
+    </row>
+    <row r="24" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>65526</v>
+      </c>
+      <c r="E24">
+        <v>70971</v>
+      </c>
+      <c r="F24">
+        <v>64484</v>
+      </c>
+      <c r="G24">
+        <v>69974</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>312337</v>
+      </c>
+      <c r="L24">
+        <v>341944</v>
+      </c>
+      <c r="M24">
+        <v>311378</v>
+      </c>
+      <c r="N24">
+        <v>339473</v>
+      </c>
+      <c r="Q24">
+        <v>4</v>
+      </c>
+      <c r="R24">
+        <v>633611</v>
+      </c>
+      <c r="S24">
+        <v>694988</v>
+      </c>
+      <c r="T24">
+        <v>630757</v>
+      </c>
+      <c r="U24">
+        <v>689055</v>
+      </c>
+      <c r="X24">
+        <v>4</v>
+      </c>
+      <c r="Y24">
+        <v>955309</v>
+      </c>
+      <c r="Z24">
+        <v>1049122</v>
+      </c>
+      <c r="AA24">
+        <v>950154</v>
+      </c>
+      <c r="AB24">
+        <v>1038887</v>
+      </c>
+      <c r="AF24" t="s">
         <v>86</v>
       </c>
-      <c r="S24" t="s">
-        <v>305</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="25" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R25" t="s">
+      <c r="AG24">
+        <v>2657</v>
+      </c>
+      <c r="AH24">
+        <v>2646</v>
+      </c>
+      <c r="AM24">
+        <v>2704</v>
+      </c>
+      <c r="AN24">
+        <v>2730</v>
+      </c>
+    </row>
+    <row r="25" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>65501</v>
+      </c>
+      <c r="E25">
+        <v>70990</v>
+      </c>
+      <c r="F25">
+        <v>64487</v>
+      </c>
+      <c r="G25">
+        <v>69826</v>
+      </c>
+      <c r="J25">
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <v>312440</v>
+      </c>
+      <c r="L25">
+        <v>341819</v>
+      </c>
+      <c r="M25">
+        <v>310779</v>
+      </c>
+      <c r="N25">
+        <v>339682</v>
+      </c>
+      <c r="Q25">
+        <v>5</v>
+      </c>
+      <c r="R25">
+        <v>633675</v>
+      </c>
+      <c r="S25">
+        <v>694871</v>
+      </c>
+      <c r="T25">
+        <v>631090</v>
+      </c>
+      <c r="U25">
+        <v>689086</v>
+      </c>
+      <c r="X25">
+        <v>5</v>
+      </c>
+      <c r="Y25">
+        <v>955264</v>
+      </c>
+      <c r="Z25">
+        <v>1049049</v>
+      </c>
+      <c r="AA25">
+        <v>948760</v>
+      </c>
+      <c r="AB25">
+        <v>1039566</v>
+      </c>
+      <c r="AF25" t="s">
         <v>87</v>
       </c>
-      <c r="S25" t="s">
-        <v>308</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="26" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R26" t="s">
+      <c r="AG25">
+        <v>1733</v>
+      </c>
+      <c r="AH25">
+        <v>1696</v>
+      </c>
+      <c r="AM25">
+        <v>1709</v>
+      </c>
+      <c r="AN25">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="26" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>65507</v>
+      </c>
+      <c r="E26">
+        <v>70972</v>
+      </c>
+      <c r="F26">
+        <v>64465</v>
+      </c>
+      <c r="G26">
+        <v>69892</v>
+      </c>
+      <c r="J26">
+        <v>6</v>
+      </c>
+      <c r="K26">
+        <v>312437</v>
+      </c>
+      <c r="L26">
+        <v>341749</v>
+      </c>
+      <c r="M26">
+        <v>311035</v>
+      </c>
+      <c r="N26">
+        <v>339611</v>
+      </c>
+      <c r="Q26">
+        <v>6</v>
+      </c>
+      <c r="R26">
+        <v>633654</v>
+      </c>
+      <c r="S26">
+        <v>695094</v>
+      </c>
+      <c r="T26">
+        <v>629417</v>
+      </c>
+      <c r="U26">
+        <v>689572</v>
+      </c>
+      <c r="X26">
+        <v>6</v>
+      </c>
+      <c r="Y26">
+        <v>955299</v>
+      </c>
+      <c r="Z26">
+        <v>1048858</v>
+      </c>
+      <c r="AA26">
+        <v>948588</v>
+      </c>
+      <c r="AB26">
+        <v>1037235</v>
+      </c>
+      <c r="AF26" t="s">
         <v>88</v>
       </c>
-      <c r="S26" t="s">
-        <v>307</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE26" t="s">
+      <c r="AG26">
+        <v>1181</v>
+      </c>
+      <c r="AH26">
+        <v>1206</v>
+      </c>
+      <c r="AM26">
+        <v>1204</v>
+      </c>
+      <c r="AN26">
+        <v>1218</v>
+      </c>
+      <c r="AS26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R27" t="s">
+    <row r="27" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>65501</v>
+      </c>
+      <c r="E27">
+        <v>70966</v>
+      </c>
+      <c r="F27">
+        <v>64480</v>
+      </c>
+      <c r="G27">
+        <v>69910</v>
+      </c>
+      <c r="J27">
+        <v>7</v>
+      </c>
+      <c r="K27">
+        <v>312393</v>
+      </c>
+      <c r="L27">
+        <v>341836</v>
+      </c>
+      <c r="M27">
+        <v>311121</v>
+      </c>
+      <c r="N27">
+        <v>339921</v>
+      </c>
+      <c r="Q27">
+        <v>7</v>
+      </c>
+      <c r="R27">
+        <v>633632</v>
+      </c>
+      <c r="S27">
+        <v>695011</v>
+      </c>
+      <c r="T27">
+        <v>629913</v>
+      </c>
+      <c r="U27">
+        <v>688023</v>
+      </c>
+      <c r="X27">
+        <v>7</v>
+      </c>
+      <c r="Y27">
+        <v>955278</v>
+      </c>
+      <c r="Z27">
+        <v>1048383</v>
+      </c>
+      <c r="AA27">
+        <v>949404</v>
+      </c>
+      <c r="AB27">
+        <v>1038155</v>
+      </c>
+      <c r="AF27" t="s">
         <v>53</v>
       </c>
-      <c r="S27" t="s">
-        <v>309</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="29" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R29" t="s">
+      <c r="AG27">
+        <v>18755</v>
+      </c>
+      <c r="AH27">
+        <v>17684</v>
+      </c>
+      <c r="AM27">
+        <v>16089</v>
+      </c>
+      <c r="AN27">
+        <v>16233</v>
+      </c>
+    </row>
+    <row r="28" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>65530</v>
+      </c>
+      <c r="E28">
+        <v>70976</v>
+      </c>
+      <c r="F28">
+        <v>64339</v>
+      </c>
+      <c r="G28">
+        <v>69892</v>
+      </c>
+      <c r="J28">
+        <v>8</v>
+      </c>
+      <c r="K28">
+        <v>312448</v>
+      </c>
+      <c r="L28">
+        <v>341838</v>
+      </c>
+      <c r="M28">
+        <v>311271</v>
+      </c>
+      <c r="N28">
+        <v>339975</v>
+      </c>
+      <c r="Q28">
+        <v>8</v>
+      </c>
+      <c r="R28">
+        <v>633258</v>
+      </c>
+      <c r="S28">
+        <v>695023</v>
+      </c>
+      <c r="T28">
+        <v>630273</v>
+      </c>
+      <c r="U28">
+        <v>688594</v>
+      </c>
+      <c r="X28">
+        <v>8</v>
+      </c>
+      <c r="Y28">
+        <v>955330</v>
+      </c>
+      <c r="Z28">
+        <v>1049036</v>
+      </c>
+      <c r="AA28">
+        <v>950286</v>
+      </c>
+      <c r="AB28">
+        <v>1039427</v>
+      </c>
+    </row>
+    <row r="29" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>65529</v>
+      </c>
+      <c r="E29">
+        <v>70975</v>
+      </c>
+      <c r="F29">
+        <v>64474</v>
+      </c>
+      <c r="G29">
+        <v>69920</v>
+      </c>
+      <c r="J29">
+        <v>9</v>
+      </c>
+      <c r="K29">
+        <v>312433</v>
+      </c>
+      <c r="L29">
+        <v>341896</v>
+      </c>
+      <c r="M29">
+        <v>311449</v>
+      </c>
+      <c r="N29">
+        <v>339275</v>
+      </c>
+      <c r="Q29">
+        <v>9</v>
+      </c>
+      <c r="R29">
+        <v>633626</v>
+      </c>
+      <c r="S29">
+        <v>695020</v>
+      </c>
+      <c r="T29">
+        <v>630526</v>
+      </c>
+      <c r="U29">
+        <v>688715</v>
+      </c>
+      <c r="X29">
+        <v>9</v>
+      </c>
+      <c r="Y29">
+        <v>955264</v>
+      </c>
+      <c r="Z29">
+        <v>1049069</v>
+      </c>
+      <c r="AA29">
+        <v>949125</v>
+      </c>
+      <c r="AB29">
+        <v>1039303</v>
+      </c>
+      <c r="AF29" t="s">
         <v>54</v>
       </c>
-      <c r="S29" t="s">
-        <v>310</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="30" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R30" t="s">
+      <c r="AG29">
+        <v>5013</v>
+      </c>
+      <c r="AH29">
+        <v>4984</v>
+      </c>
+      <c r="AM29">
+        <v>5007</v>
+      </c>
+      <c r="AN29">
+        <v>4628</v>
+      </c>
+    </row>
+    <row r="30" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>65530</v>
+      </c>
+      <c r="E30">
+        <v>70996</v>
+      </c>
+      <c r="F30">
+        <v>64492</v>
+      </c>
+      <c r="G30">
+        <v>69934</v>
+      </c>
+      <c r="J30">
+        <v>10</v>
+      </c>
+      <c r="K30">
+        <v>312460</v>
+      </c>
+      <c r="L30">
+        <v>341833</v>
+      </c>
+      <c r="M30">
+        <v>311361</v>
+      </c>
+      <c r="N30">
+        <v>339318</v>
+      </c>
+      <c r="Q30">
+        <v>10</v>
+      </c>
+      <c r="R30">
+        <v>633149</v>
+      </c>
+      <c r="S30">
+        <v>694961</v>
+      </c>
+      <c r="T30">
+        <v>630779</v>
+      </c>
+      <c r="U30">
+        <v>689655</v>
+      </c>
+      <c r="X30">
+        <v>10</v>
+      </c>
+      <c r="Y30">
+        <v>955413</v>
+      </c>
+      <c r="Z30">
+        <v>1049184</v>
+      </c>
+      <c r="AA30">
+        <v>950649</v>
+      </c>
+      <c r="AB30">
+        <v>1037778</v>
+      </c>
+      <c r="AF30" t="s">
         <v>55</v>
       </c>
-      <c r="S30" t="s">
-        <v>311</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="31" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R31" t="s">
+      <c r="AG30">
+        <v>5246</v>
+      </c>
+      <c r="AH30">
+        <v>5237</v>
+      </c>
+      <c r="AM30">
+        <v>5298</v>
+      </c>
+      <c r="AN30">
+        <v>5283</v>
+      </c>
+    </row>
+    <row r="31" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AF31" t="s">
         <v>56</v>
       </c>
-      <c r="S31" t="s">
-        <v>310</v>
-      </c>
-      <c r="Y31" t="s">
-        <v>266</v>
-      </c>
-      <c r="AE31" t="s">
+      <c r="AG31">
+        <v>5013</v>
+      </c>
+      <c r="AH31">
+        <v>4975</v>
+      </c>
+      <c r="AM31">
+        <v>5098</v>
+      </c>
+      <c r="AN31">
+        <v>5267</v>
+      </c>
+      <c r="AS31" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R32" t="s">
+    <row r="32" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D32">
+        <f>AVERAGE(D21:D30)</f>
+        <v>65521.5</v>
+      </c>
+      <c r="E32">
+        <f>AVERAGE(E21:E30)</f>
+        <v>70984</v>
+      </c>
+      <c r="F32">
+        <f>AVERAGE(F21:F30)</f>
+        <v>64459.5</v>
+      </c>
+      <c r="G32">
+        <f>AVERAGE(G21:G30)</f>
+        <v>69905.600000000006</v>
+      </c>
+      <c r="K32">
+        <f>AVERAGE(K21:K30)</f>
+        <v>312407.2</v>
+      </c>
+      <c r="L32">
+        <f>AVERAGE(L21:L30)</f>
+        <v>341864.8</v>
+      </c>
+      <c r="M32">
+        <f>AVERAGE(M21:M30)</f>
+        <v>311211.2</v>
+      </c>
+      <c r="N32">
+        <f>AVERAGE(N21:N30)</f>
+        <v>339483.2</v>
+      </c>
+      <c r="R32">
+        <f>AVERAGE(R21:R30)</f>
+        <v>633540.4</v>
+      </c>
+      <c r="S32">
+        <f>AVERAGE(S21:S30)</f>
+        <v>694976.8</v>
+      </c>
+      <c r="T32">
+        <f>AVERAGE(T21:T30)</f>
+        <v>630350.4</v>
+      </c>
+      <c r="U32">
+        <f>AVERAGE(U21:U30)</f>
+        <v>688967.1</v>
+      </c>
+      <c r="Y32">
+        <f>AVERAGE(Y21:Y30)</f>
+        <v>955322.1</v>
+      </c>
+      <c r="Z32">
+        <f>AVERAGE(Z21:Z30)</f>
+        <v>1049000.8</v>
+      </c>
+      <c r="AA32">
+        <f>AVERAGE(AA21:AA30)</f>
+        <v>949513.7</v>
+      </c>
+      <c r="AB32">
+        <f>AVERAGE(AB21:AB30)</f>
+        <v>1038304.9</v>
+      </c>
+      <c r="AF32" t="s">
         <v>57</v>
       </c>
-      <c r="S32" t="s">
-        <v>312</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="34" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R34" t="s">
+      <c r="AG32">
+        <v>20116</v>
+      </c>
+      <c r="AH32">
+        <v>19135</v>
+      </c>
+      <c r="AM32">
+        <v>17526</v>
+      </c>
+      <c r="AN32">
+        <v>17953</v>
+      </c>
+    </row>
+    <row r="34" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF34" t="s">
         <v>59</v>
       </c>
-      <c r="S34" t="s">
-        <v>313</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>268</v>
-      </c>
-      <c r="AE34" t="s">
+      <c r="AG34">
+        <v>1575</v>
+      </c>
+      <c r="AH34">
+        <v>1551</v>
+      </c>
+      <c r="AM34">
+        <v>1653</v>
+      </c>
+      <c r="AN34">
+        <v>1822</v>
+      </c>
+      <c r="AS34" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R35" t="s">
+    <row r="35" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF35" t="s">
         <v>60</v>
       </c>
-      <c r="S35" t="s">
-        <v>314</v>
-      </c>
-      <c r="Y35" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="36" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R36" t="s">
+      <c r="AG35">
+        <v>2761</v>
+      </c>
+      <c r="AH35">
+        <v>2701</v>
+      </c>
+      <c r="AM35">
+        <v>2774</v>
+      </c>
+      <c r="AN35">
+        <v>2817</v>
+      </c>
+    </row>
+    <row r="36" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF36" t="s">
         <v>61</v>
       </c>
-      <c r="S36" t="s">
-        <v>315</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>270</v>
-      </c>
-      <c r="AE36" t="s">
+      <c r="AG36">
+        <v>2865</v>
+      </c>
+      <c r="AH36">
+        <v>2879</v>
+      </c>
+      <c r="AM36">
+        <v>2944</v>
+      </c>
+      <c r="AN36">
+        <v>2896</v>
+      </c>
+      <c r="AS36" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R37" t="s">
+    <row r="37" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF37" t="s">
         <v>62</v>
       </c>
-      <c r="S37" t="s">
-        <v>316</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="38" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R38" t="s">
+      <c r="AG37">
+        <v>2306</v>
+      </c>
+      <c r="AH37">
+        <v>2220</v>
+      </c>
+      <c r="AM37">
+        <v>2278</v>
+      </c>
+      <c r="AN37">
+        <v>2361</v>
+      </c>
+    </row>
+    <row r="38" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF38" t="s">
         <v>63</v>
       </c>
-      <c r="S38" t="s">
-        <v>317</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>273</v>
-      </c>
-      <c r="AE38" t="s">
+      <c r="AG38">
+        <v>3934</v>
+      </c>
+      <c r="AH38">
+        <v>3848</v>
+      </c>
+      <c r="AM38">
+        <v>3882</v>
+      </c>
+      <c r="AN38">
+        <v>3965</v>
+      </c>
+      <c r="AS38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R39" t="s">
+    <row r="39" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF39" t="s">
         <v>64</v>
       </c>
-      <c r="S39" t="s">
-        <v>319</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="40" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R40" t="s">
+      <c r="AG39">
+        <v>2116</v>
+      </c>
+      <c r="AH39">
+        <v>2038</v>
+      </c>
+      <c r="AM39">
+        <v>2098</v>
+      </c>
+      <c r="AN39">
+        <v>2154</v>
+      </c>
+    </row>
+    <row r="40" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF40" t="s">
         <v>65</v>
       </c>
-      <c r="S40" t="s">
-        <v>318</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="41" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R41" t="s">
+      <c r="AG40">
+        <v>3739</v>
+      </c>
+      <c r="AH40">
+        <v>3662</v>
+      </c>
+      <c r="AM40">
+        <v>3696</v>
+      </c>
+      <c r="AN40">
+        <v>3772</v>
+      </c>
+    </row>
+    <row r="41" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF41" t="s">
         <v>66</v>
       </c>
-      <c r="S41" t="s">
-        <v>320</v>
-      </c>
-      <c r="Y41" t="s">
-        <v>275</v>
-      </c>
-      <c r="AE41" t="s">
+      <c r="AG41">
+        <v>3113</v>
+      </c>
+      <c r="AH41">
+        <v>3102</v>
+      </c>
+      <c r="AM41">
+        <v>2930</v>
+      </c>
+      <c r="AN41">
+        <v>2878</v>
+      </c>
+      <c r="AS41" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R42" t="s">
+    <row r="42" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF42" t="s">
         <v>67</v>
       </c>
-      <c r="S42" t="s">
-        <v>321</v>
-      </c>
-      <c r="Y42" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="43" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R43" t="s">
+      <c r="AG42">
+        <v>18096</v>
+      </c>
+      <c r="AH42">
+        <v>17182</v>
+      </c>
+      <c r="AM42">
+        <v>15644</v>
+      </c>
+      <c r="AN42">
+        <v>15788</v>
+      </c>
+    </row>
+    <row r="43" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF43" t="s">
         <v>68</v>
       </c>
-      <c r="S43" t="s">
-        <v>322</v>
-      </c>
-      <c r="Y43" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="44" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R44" t="s">
+      <c r="AG43">
+        <v>36332</v>
+      </c>
+      <c r="AH43">
+        <v>34340</v>
+      </c>
+      <c r="AM43">
+        <v>31208</v>
+      </c>
+      <c r="AN43">
+        <v>31852</v>
+      </c>
+    </row>
+    <row r="44" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF44" t="s">
         <v>69</v>
       </c>
-      <c r="S44" t="s">
-        <v>323</v>
-      </c>
-      <c r="Y44" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="45" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R45" t="s">
+      <c r="AG44">
+        <v>3544</v>
+      </c>
+      <c r="AH44">
+        <v>3491</v>
+      </c>
+      <c r="AM44">
+        <v>3562</v>
+      </c>
+      <c r="AN44">
+        <v>3562</v>
+      </c>
+    </row>
+    <row r="45" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF45" t="s">
         <v>70</v>
       </c>
-      <c r="S45" t="s">
-        <v>324</v>
-      </c>
-      <c r="Y45" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="46" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="AE46" t="s">
+      <c r="AG45">
+        <v>3455</v>
+      </c>
+      <c r="AH45">
+        <v>3373</v>
+      </c>
+      <c r="AM45">
+        <v>3449</v>
+      </c>
+      <c r="AN45">
+        <v>3545</v>
+      </c>
+    </row>
+    <row r="46" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF46" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG46">
+        <v>13334</v>
+      </c>
+      <c r="AH46">
+        <v>13194</v>
+      </c>
+      <c r="AM46">
+        <v>12547</v>
+      </c>
+      <c r="AN46">
+        <v>12551</v>
+      </c>
+      <c r="AS46" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R47" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y47" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="49" spans="18:25" x14ac:dyDescent="0.25">
-      <c r="R49" t="s">
+    <row r="48" spans="32:45" x14ac:dyDescent="0.25">
+      <c r="AF48" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG48">
+        <f>SUM(AG5:AG46)</f>
+        <v>707062</v>
+      </c>
+      <c r="AH48">
+        <f>SUM(AH5:AH46)</f>
+        <v>692100</v>
+      </c>
+      <c r="AM48">
+        <f>SUM(AM5:AM46)</f>
+        <v>680933</v>
+      </c>
+      <c r="AN48">
+        <f>SUM(AN5:AN46)</f>
+        <v>686255</v>
+      </c>
+    </row>
+    <row r="51" spans="32:40" x14ac:dyDescent="0.25">
+      <c r="AF51" t="s">
         <v>72</v>
       </c>
-      <c r="S49" t="s">
-        <v>288</v>
-      </c>
-      <c r="Y49" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="50" spans="18:25" x14ac:dyDescent="0.25">
-      <c r="R50" t="s">
+      <c r="AG51">
+        <v>17193792</v>
+      </c>
+      <c r="AH51">
+        <v>17071077</v>
+      </c>
+      <c r="AM51">
+        <v>17405915</v>
+      </c>
+      <c r="AN51">
+        <v>17508299</v>
+      </c>
+    </row>
+    <row r="52" spans="32:40" x14ac:dyDescent="0.25">
+      <c r="AF52" t="s">
         <v>73</v>
       </c>
-      <c r="S50" t="s">
-        <v>285</v>
-      </c>
-      <c r="Y50" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="51" spans="18:25" x14ac:dyDescent="0.25">
-      <c r="R51" t="s">
+      <c r="AG52">
+        <v>105697</v>
+      </c>
+      <c r="AH52">
+        <v>103453</v>
+      </c>
+      <c r="AM52">
+        <v>105728</v>
+      </c>
+      <c r="AN52">
+        <v>107789</v>
+      </c>
+    </row>
+    <row r="53" spans="32:40" x14ac:dyDescent="0.25">
+      <c r="AF53" t="s">
         <v>74</v>
       </c>
-      <c r="S51" t="s">
-        <v>286</v>
-      </c>
-      <c r="Y51" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="52" spans="18:25" x14ac:dyDescent="0.25">
-      <c r="R52" t="s">
+      <c r="AG53">
+        <v>6754891</v>
+      </c>
+      <c r="AH53">
+        <v>6611764</v>
+      </c>
+      <c r="AM53">
+        <v>6454577</v>
+      </c>
+      <c r="AN53">
+        <v>6531258</v>
+      </c>
+    </row>
+    <row r="54" spans="32:40" x14ac:dyDescent="0.25">
+      <c r="AF54" t="s">
         <v>75</v>
       </c>
-      <c r="S52" t="s">
-        <v>287</v>
-      </c>
-      <c r="Y52" t="s">
-        <v>283</v>
+      <c r="AG54">
+        <v>9151238</v>
+      </c>
+      <c r="AH54">
+        <v>8975617</v>
+      </c>
+      <c r="AM54">
+        <v>9137022</v>
+      </c>
+      <c r="AN54">
+        <v>9176671</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replaced double with float, fixed geometric mean, new benchmark results
</commit_message>
<xml_diff>
--- a/BenchmarkDocs/Results.xlsx
+++ b/BenchmarkDocs/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f0dc99f0b729840/Teilen/edge-ml/feature-extraction/BenchmarkDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="970" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF0211AB-71CE-489B-8E25-3822A8BA14DE}"/>
+  <xr:revisionPtr revIDLastSave="1257" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B9FCEEB-C682-4095-9202-07A7BAED7199}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
+    <workbookView xWindow="12585" yWindow="150" windowWidth="15960" windowHeight="14280" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="175">
   <si>
     <t>Arduino</t>
   </si>
@@ -514,12 +514,6 @@
     <t>02.02.</t>
   </si>
   <si>
-    <t>03.02.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04.02. </t>
-  </si>
-  <si>
     <t xml:space="preserve">05.02. </t>
   </si>
   <si>
@@ -556,10 +550,16 @@
     <t>auto_n = 1000, n = 1000, cep_length = 1000</t>
   </si>
   <si>
-    <t>Neu:GeoMean</t>
-  </si>
-  <si>
-    <t>Stand: 03.02.</t>
+    <t>Neu:geo,float</t>
+  </si>
+  <si>
+    <t>Stand: 04.02.</t>
+  </si>
+  <si>
+    <t>04.02.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06.02. </t>
   </si>
 </sst>
 </file>
@@ -2944,10 +2944,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DC238C-8F4B-441F-9A1D-B395F114E22E}">
-  <dimension ref="A1:AS54"/>
+  <dimension ref="A1:AS64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA62" sqref="AA62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2970,7 +2970,7 @@
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.25">
@@ -3060,13 +3060,13 @@
         <v>158</v>
       </c>
       <c r="AJ4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AK4" t="s">
         <v>159</v>
       </c>
-      <c r="AK4" t="s">
-        <v>160</v>
-      </c>
       <c r="AL4" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="AM4" t="s">
         <v>156</v>
@@ -3078,13 +3078,13 @@
         <v>158</v>
       </c>
       <c r="AP4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AQ4" t="s">
         <v>159</v>
       </c>
-      <c r="AQ4" t="s">
-        <v>160</v>
-      </c>
       <c r="AR4" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
@@ -3130,6 +3130,9 @@
       <c r="AI5">
         <v>1600</v>
       </c>
+      <c r="AJ5">
+        <v>128</v>
+      </c>
       <c r="AM5">
         <v>1639</v>
       </c>
@@ -3138,6 +3141,9 @@
       </c>
       <c r="AO5">
         <v>1622</v>
+      </c>
+      <c r="AP5">
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
@@ -3183,6 +3189,9 @@
       <c r="AI6">
         <v>5190</v>
       </c>
+      <c r="AJ6">
+        <v>317</v>
+      </c>
       <c r="AM6">
         <v>4630</v>
       </c>
@@ -3192,6 +3201,9 @@
       <c r="AO6">
         <v>4663</v>
       </c>
+      <c r="AP6">
+        <v>391</v>
+      </c>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J7">
@@ -3236,6 +3248,9 @@
       <c r="AI7">
         <v>51380</v>
       </c>
+      <c r="AJ7">
+        <v>2128</v>
+      </c>
       <c r="AM7">
         <v>52201</v>
       </c>
@@ -3245,6 +3260,9 @@
       <c r="AO7">
         <v>52940</v>
       </c>
+      <c r="AP7">
+        <v>2140</v>
+      </c>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="J8">
@@ -3289,6 +3307,9 @@
       <c r="AI8">
         <v>17133</v>
       </c>
+      <c r="AJ8">
+        <v>2269</v>
+      </c>
       <c r="AM8">
         <v>15579</v>
       </c>
@@ -3297,6 +3318,9 @@
       </c>
       <c r="AO8">
         <v>15857</v>
+      </c>
+      <c r="AP8">
+        <v>2351</v>
       </c>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
@@ -3342,6 +3366,9 @@
       <c r="AI9">
         <v>20717</v>
       </c>
+      <c r="AJ9">
+        <v>3922</v>
+      </c>
       <c r="AM9">
         <v>19193</v>
       </c>
@@ -3350,6 +3377,9 @@
       </c>
       <c r="AO9">
         <v>19443</v>
+      </c>
+      <c r="AP9">
+        <v>3977</v>
       </c>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.25">
@@ -3395,6 +3425,9 @@
       <c r="AI10">
         <v>19860</v>
       </c>
+      <c r="AJ10">
+        <v>3830</v>
+      </c>
       <c r="AM10">
         <v>18477</v>
       </c>
@@ -3403,6 +3436,9 @@
       </c>
       <c r="AO10">
         <v>18758</v>
+      </c>
+      <c r="AP10">
+        <v>3875</v>
       </c>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
@@ -3448,6 +3484,9 @@
       <c r="AI11">
         <v>36627</v>
       </c>
+      <c r="AJ11">
+        <v>5377</v>
+      </c>
       <c r="AM11">
         <v>33520</v>
       </c>
@@ -3456,6 +3495,9 @@
       </c>
       <c r="AO11">
         <v>34072</v>
+      </c>
+      <c r="AP11">
+        <v>5439</v>
       </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
@@ -3501,6 +3543,9 @@
       <c r="AI12">
         <v>6194</v>
       </c>
+      <c r="AJ12">
+        <v>11866</v>
+      </c>
       <c r="AM12">
         <v>5822</v>
       </c>
@@ -3509,6 +3554,9 @@
       </c>
       <c r="AO12">
         <v>5832</v>
+      </c>
+      <c r="AP12">
+        <v>12347</v>
       </c>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
@@ -3554,6 +3602,9 @@
       <c r="AI13">
         <v>5200</v>
       </c>
+      <c r="AJ13">
+        <v>289</v>
+      </c>
       <c r="AM13">
         <v>4641</v>
       </c>
@@ -3562,6 +3613,9 @@
       </c>
       <c r="AO13">
         <v>4662</v>
+      </c>
+      <c r="AP13">
+        <v>435</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -3607,6 +3661,9 @@
       <c r="AI14">
         <v>6163</v>
       </c>
+      <c r="AJ14">
+        <v>11888</v>
+      </c>
       <c r="AM14">
         <v>5741</v>
       </c>
@@ -3615,6 +3672,9 @@
       </c>
       <c r="AO14">
         <v>5746</v>
+      </c>
+      <c r="AP14">
+        <v>12335</v>
       </c>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.25">
@@ -3630,6 +3690,9 @@
       <c r="AI15">
         <v>3022</v>
       </c>
+      <c r="AJ15">
+        <v>11716</v>
+      </c>
       <c r="AM15">
         <v>2914</v>
       </c>
@@ -3639,10 +3702,13 @@
       <c r="AO15">
         <v>2820</v>
       </c>
+      <c r="AP15">
+        <v>12271</v>
+      </c>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K16">
         <f>AVERAGE(K5:K14)</f>
@@ -3688,6 +3754,9 @@
       <c r="AI16">
         <v>178088</v>
       </c>
+      <c r="AJ16">
+        <v>172595</v>
+      </c>
       <c r="AM16">
         <v>181033</v>
       </c>
@@ -3696,6 +3765,9 @@
       </c>
       <c r="AO16">
         <v>181849</v>
+      </c>
+      <c r="AP16">
+        <v>176635</v>
       </c>
     </row>
     <row r="17" spans="2:45" x14ac:dyDescent="0.25">
@@ -3711,6 +3783,9 @@
       <c r="AI17">
         <v>178905</v>
       </c>
+      <c r="AJ17">
+        <v>173288</v>
+      </c>
       <c r="AM17">
         <v>181693</v>
       </c>
@@ -3720,13 +3795,16 @@
       <c r="AO17">
         <v>182862</v>
       </c>
+      <c r="AP17">
+        <v>177095</v>
+      </c>
     </row>
     <row r="18" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AF18" t="s">
         <v>48</v>
@@ -3740,6 +3818,9 @@
       <c r="AI18">
         <v>4324</v>
       </c>
+      <c r="AJ18">
+        <v>989</v>
+      </c>
       <c r="AM18">
         <v>4074</v>
       </c>
@@ -3748,6 +3829,9 @@
       </c>
       <c r="AO18">
         <v>4069</v>
+      </c>
+      <c r="AP18">
+        <v>1030</v>
       </c>
     </row>
     <row r="19" spans="2:45" x14ac:dyDescent="0.25">
@@ -3755,7 +3839,7 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D19" t="s">
         <v>96</v>
@@ -3782,7 +3866,7 @@
         <v>97</v>
       </c>
       <c r="X19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Y19" t="s">
         <v>96</v>
@@ -3864,6 +3948,9 @@
       <c r="AI20">
         <v>1236</v>
       </c>
+      <c r="AJ20">
+        <v>175</v>
+      </c>
       <c r="AM20">
         <v>1303</v>
       </c>
@@ -3872,6 +3959,9 @@
       </c>
       <c r="AO20">
         <v>1309</v>
+      </c>
+      <c r="AP20">
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="2:45" x14ac:dyDescent="0.25">
@@ -3947,6 +4037,9 @@
       <c r="AI21">
         <v>1153</v>
       </c>
+      <c r="AJ21">
+        <v>219</v>
+      </c>
       <c r="AM21">
         <v>1194</v>
       </c>
@@ -3955,6 +4048,9 @@
       </c>
       <c r="AO21">
         <v>1238</v>
+      </c>
+      <c r="AP21">
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="2:45" x14ac:dyDescent="0.25">
@@ -4030,6 +4126,9 @@
       <c r="AI22">
         <v>1110</v>
       </c>
+      <c r="AJ22">
+        <v>176</v>
+      </c>
       <c r="AM22">
         <v>1150</v>
       </c>
@@ -4039,6 +4138,9 @@
       <c r="AO22">
         <v>1172</v>
       </c>
+      <c r="AP22">
+        <v>258</v>
+      </c>
     </row>
     <row r="23" spans="2:45" x14ac:dyDescent="0.25">
       <c r="C23">
@@ -4113,6 +4215,9 @@
       <c r="AI23">
         <v>2805</v>
       </c>
+      <c r="AJ23">
+        <v>828</v>
+      </c>
       <c r="AM23">
         <v>2829</v>
       </c>
@@ -4122,6 +4227,9 @@
       <c r="AO23">
         <v>2903</v>
       </c>
+      <c r="AP23">
+        <v>802</v>
+      </c>
     </row>
     <row r="24" spans="2:45" x14ac:dyDescent="0.25">
       <c r="C24">
@@ -4196,6 +4304,9 @@
       <c r="AI24">
         <v>2620</v>
       </c>
+      <c r="AJ24">
+        <v>797</v>
+      </c>
       <c r="AM24">
         <v>2704</v>
       </c>
@@ -4204,6 +4315,9 @@
       </c>
       <c r="AO24">
         <v>2706</v>
+      </c>
+      <c r="AP24">
+        <v>802</v>
       </c>
     </row>
     <row r="25" spans="2:45" x14ac:dyDescent="0.25">
@@ -4279,6 +4393,9 @@
       <c r="AI25">
         <v>1667</v>
       </c>
+      <c r="AJ25">
+        <v>305</v>
+      </c>
       <c r="AM25">
         <v>1709</v>
       </c>
@@ -4287,6 +4404,9 @@
       </c>
       <c r="AO25">
         <v>1777</v>
+      </c>
+      <c r="AP25">
+        <v>301</v>
       </c>
     </row>
     <row r="26" spans="2:45" x14ac:dyDescent="0.25">
@@ -4362,6 +4482,9 @@
       <c r="AI26">
         <v>1179</v>
       </c>
+      <c r="AJ26">
+        <v>237</v>
+      </c>
       <c r="AM26">
         <v>1204</v>
       </c>
@@ -4370,6 +4493,9 @@
       </c>
       <c r="AO26">
         <v>1252</v>
+      </c>
+      <c r="AP26">
+        <v>217</v>
       </c>
       <c r="AS26" t="s">
         <v>76</v>
@@ -4448,6 +4574,9 @@
       <c r="AI27">
         <v>17711</v>
       </c>
+      <c r="AJ27">
+        <v>2626</v>
+      </c>
       <c r="AM27">
         <v>16089</v>
       </c>
@@ -4456,6 +4585,9 @@
       </c>
       <c r="AO27">
         <v>16367</v>
+      </c>
+      <c r="AP27">
+        <v>2679</v>
       </c>
     </row>
     <row r="28" spans="2:45" x14ac:dyDescent="0.25">
@@ -4593,6 +4725,9 @@
       <c r="AI29">
         <v>4968</v>
       </c>
+      <c r="AJ29">
+        <v>1868</v>
+      </c>
       <c r="AM29">
         <v>5007</v>
       </c>
@@ -4601,6 +4736,9 @@
       </c>
       <c r="AO29">
         <v>5058</v>
+      </c>
+      <c r="AP29">
+        <v>1885</v>
       </c>
     </row>
     <row r="30" spans="2:45" x14ac:dyDescent="0.25">
@@ -4676,6 +4814,9 @@
       <c r="AI30">
         <v>5223</v>
       </c>
+      <c r="AJ30">
+        <v>1854</v>
+      </c>
       <c r="AM30">
         <v>5298</v>
       </c>
@@ -4684,6 +4825,9 @@
       </c>
       <c r="AO30">
         <v>5331</v>
+      </c>
+      <c r="AP30">
+        <v>1885</v>
       </c>
     </row>
     <row r="31" spans="2:45" x14ac:dyDescent="0.25">
@@ -4699,6 +4843,9 @@
       <c r="AI31">
         <v>4965</v>
       </c>
+      <c r="AJ31">
+        <v>1903</v>
+      </c>
       <c r="AM31">
         <v>5098</v>
       </c>
@@ -4708,13 +4855,16 @@
       <c r="AO31">
         <v>5308</v>
       </c>
+      <c r="AP31">
+        <v>1966</v>
+      </c>
       <c r="AS31" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="32" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D32">
         <f>AVERAGE(D21:D30)</f>
@@ -4792,6 +4942,9 @@
       <c r="AI32">
         <v>19096</v>
       </c>
+      <c r="AJ32">
+        <v>2868</v>
+      </c>
       <c r="AM32">
         <v>17526</v>
       </c>
@@ -4801,10 +4954,13 @@
       <c r="AO32">
         <v>18025</v>
       </c>
+      <c r="AP32">
+        <v>2863</v>
+      </c>
     </row>
     <row r="34" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AF34" t="s">
         <v>59</v>
@@ -4818,6 +4974,9 @@
       <c r="AI34">
         <v>1551</v>
       </c>
+      <c r="AJ34">
+        <v>128</v>
+      </c>
       <c r="AM34">
         <v>1653</v>
       </c>
@@ -4826,6 +4985,9 @@
       </c>
       <c r="AO34">
         <v>1840</v>
+      </c>
+      <c r="AP34">
+        <v>156</v>
       </c>
       <c r="AS34" t="s">
         <v>78</v>
@@ -4836,7 +4998,7 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D35" t="s">
         <v>96</v>
@@ -4863,7 +5025,7 @@
         <v>97</v>
       </c>
       <c r="X35" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Y35" t="s">
         <v>96</v>
@@ -4883,6 +5045,9 @@
       <c r="AI35">
         <v>2728</v>
       </c>
+      <c r="AJ35">
+        <v>514</v>
+      </c>
       <c r="AM35">
         <v>2774</v>
       </c>
@@ -4891,6 +5056,9 @@
       </c>
       <c r="AO35">
         <v>2831</v>
+      </c>
+      <c r="AP35">
+        <v>424</v>
       </c>
     </row>
     <row r="36" spans="2:45" x14ac:dyDescent="0.25">
@@ -4966,6 +5134,9 @@
       <c r="AI36">
         <v>2879</v>
       </c>
+      <c r="AJ36">
+        <v>312</v>
+      </c>
       <c r="AM36">
         <v>2944</v>
       </c>
@@ -4974,6 +5145,9 @@
       </c>
       <c r="AO36">
         <v>2884</v>
+      </c>
+      <c r="AP36">
+        <v>316</v>
       </c>
       <c r="AS36" t="s">
         <v>79</v>
@@ -5052,6 +5226,9 @@
       <c r="AI37">
         <v>2247</v>
       </c>
+      <c r="AJ37">
+        <v>331</v>
+      </c>
       <c r="AM37">
         <v>2278</v>
       </c>
@@ -5060,6 +5237,9 @@
       </c>
       <c r="AO37">
         <v>2375</v>
+      </c>
+      <c r="AP37">
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="2:45" x14ac:dyDescent="0.25">
@@ -5135,6 +5315,9 @@
       <c r="AI38">
         <v>3842</v>
       </c>
+      <c r="AJ38">
+        <v>492</v>
+      </c>
       <c r="AM38">
         <v>3882</v>
       </c>
@@ -5144,6 +5327,9 @@
       <c r="AO38">
         <v>3948</v>
       </c>
+      <c r="AP38">
+        <v>395</v>
+      </c>
       <c r="AS38" t="s">
         <v>79</v>
       </c>
@@ -5221,6 +5407,9 @@
       <c r="AI39">
         <v>2038</v>
       </c>
+      <c r="AJ39">
+        <v>233</v>
+      </c>
       <c r="AM39">
         <v>2098</v>
       </c>
@@ -5230,6 +5419,9 @@
       <c r="AO39">
         <v>2156</v>
       </c>
+      <c r="AP39">
+        <v>330</v>
+      </c>
     </row>
     <row r="40" spans="2:45" x14ac:dyDescent="0.25">
       <c r="C40">
@@ -5304,6 +5496,9 @@
       <c r="AI40">
         <v>3654</v>
       </c>
+      <c r="AJ40">
+        <v>359</v>
+      </c>
       <c r="AM40">
         <v>3696</v>
       </c>
@@ -5312,6 +5507,9 @@
       </c>
       <c r="AO40">
         <v>3772</v>
+      </c>
+      <c r="AP40">
+        <v>428</v>
       </c>
     </row>
     <row r="41" spans="2:45" x14ac:dyDescent="0.25">
@@ -5387,6 +5585,9 @@
       <c r="AI41">
         <v>3102</v>
       </c>
+      <c r="AJ41">
+        <v>11776</v>
+      </c>
       <c r="AM41">
         <v>2930</v>
       </c>
@@ -5395,6 +5596,9 @@
       </c>
       <c r="AO41">
         <v>2886</v>
+      </c>
+      <c r="AP41">
+        <v>12316</v>
       </c>
       <c r="AS41" t="s">
         <v>80</v>
@@ -5473,6 +5677,9 @@
       <c r="AI42">
         <v>17182</v>
       </c>
+      <c r="AJ42">
+        <v>2389</v>
+      </c>
       <c r="AM42">
         <v>15644</v>
       </c>
@@ -5481,6 +5688,9 @@
       </c>
       <c r="AO42">
         <v>15903</v>
+      </c>
+      <c r="AP42">
+        <v>2402</v>
       </c>
     </row>
     <row r="43" spans="2:45" x14ac:dyDescent="0.25">
@@ -5556,6 +5766,9 @@
       <c r="AI43">
         <v>34313</v>
       </c>
+      <c r="AJ43">
+        <v>4597</v>
+      </c>
       <c r="AM43">
         <v>31208</v>
       </c>
@@ -5564,6 +5777,9 @@
       </c>
       <c r="AO43">
         <v>31685</v>
+      </c>
+      <c r="AP43">
+        <v>4742</v>
       </c>
     </row>
     <row r="44" spans="2:45" x14ac:dyDescent="0.25">
@@ -5639,6 +5855,9 @@
       <c r="AI44">
         <v>3492</v>
       </c>
+      <c r="AJ44">
+        <v>1230</v>
+      </c>
       <c r="AM44">
         <v>3562</v>
       </c>
@@ -5647,6 +5866,9 @@
       </c>
       <c r="AO44">
         <v>3587</v>
+      </c>
+      <c r="AP44">
+        <v>1235</v>
       </c>
     </row>
     <row r="45" spans="2:45" x14ac:dyDescent="0.25">
@@ -5722,6 +5944,9 @@
       <c r="AI45">
         <v>3373</v>
       </c>
+      <c r="AJ45">
+        <v>1224</v>
+      </c>
       <c r="AM45">
         <v>3449</v>
       </c>
@@ -5730,6 +5955,9 @@
       </c>
       <c r="AO45">
         <v>3526</v>
+      </c>
+      <c r="AP45">
+        <v>1228</v>
       </c>
     </row>
     <row r="46" spans="2:45" x14ac:dyDescent="0.25">
@@ -5805,6 +6033,9 @@
       <c r="AI46">
         <v>13242</v>
       </c>
+      <c r="AJ46">
+        <v>13122</v>
+      </c>
       <c r="AM46">
         <v>12547</v>
       </c>
@@ -5814,13 +6045,16 @@
       <c r="AO46">
         <v>12536</v>
       </c>
+      <c r="AP46">
+        <v>13586</v>
+      </c>
       <c r="AS46" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="48" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D48">
         <f>AVERAGE(D37:D46)</f>
@@ -5887,7 +6121,7 @@
         <v>1038280</v>
       </c>
       <c r="AF48" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AG48">
         <f>SUM(AG5:AG46)</f>
@@ -5901,6 +6135,10 @@
         <f>SUM(AI5:AI46)</f>
         <v>691779</v>
       </c>
+      <c r="AJ48">
+        <f>SUM(AJ5:AJ46)</f>
+        <v>451165</v>
+      </c>
       <c r="AM48">
         <f>SUM(AM5:AM46)</f>
         <v>680933</v>
@@ -5916,16 +6154,52 @@
     </row>
     <row r="50" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C50" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>33</v>
       </c>
+      <c r="C51" t="s">
+        <v>164</v>
+      </c>
+      <c r="D51" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51" t="s">
+        <v>97</v>
+      </c>
+      <c r="J51" t="s">
+        <v>26</v>
+      </c>
+      <c r="K51" t="s">
+        <v>96</v>
+      </c>
+      <c r="M51" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R51" t="s">
+        <v>96</v>
+      </c>
+      <c r="T51" t="s">
+        <v>97</v>
+      </c>
+      <c r="X51" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>97</v>
+      </c>
       <c r="AF51" t="s">
         <v>72</v>
       </c>
@@ -5938,6 +6212,9 @@
       <c r="AI51">
         <v>17071582</v>
       </c>
+      <c r="AJ51">
+        <v>16900049</v>
+      </c>
       <c r="AM51">
         <v>17405915</v>
       </c>
@@ -5947,11 +6224,74 @@
       <c r="AO51">
         <v>17507506</v>
       </c>
+      <c r="AP51">
+        <v>17271362</v>
+      </c>
       <c r="AS51" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52" t="s">
+        <v>4</v>
+      </c>
+      <c r="J52" t="s">
+        <v>5</v>
+      </c>
+      <c r="K52" t="s">
+        <v>3</v>
+      </c>
+      <c r="L52" t="s">
+        <v>4</v>
+      </c>
+      <c r="M52" t="s">
+        <v>3</v>
+      </c>
+      <c r="N52" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>5</v>
+      </c>
+      <c r="R52" t="s">
+        <v>3</v>
+      </c>
+      <c r="S52" t="s">
+        <v>4</v>
+      </c>
+      <c r="T52" t="s">
+        <v>3</v>
+      </c>
+      <c r="U52" t="s">
+        <v>4</v>
+      </c>
+      <c r="X52" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>4</v>
+      </c>
       <c r="AF52" t="s">
         <v>73</v>
       </c>
@@ -5964,6 +6304,9 @@
       <c r="AI52">
         <v>103445</v>
       </c>
+      <c r="AJ52">
+        <v>19496</v>
+      </c>
       <c r="AM52">
         <v>105728</v>
       </c>
@@ -5973,8 +6316,71 @@
       <c r="AO52">
         <v>107732</v>
       </c>
+      <c r="AP52">
+        <v>19843</v>
+      </c>
     </row>
     <row r="53" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>45049</v>
+      </c>
+      <c r="E53">
+        <v>50819</v>
+      </c>
+      <c r="F53">
+        <v>44363</v>
+      </c>
+      <c r="G53">
+        <v>50442</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>198752</v>
+      </c>
+      <c r="L53">
+        <v>229595</v>
+      </c>
+      <c r="M53">
+        <v>201373</v>
+      </c>
+      <c r="N53">
+        <v>233475</v>
+      </c>
+      <c r="Q53">
+        <v>1</v>
+      </c>
+      <c r="R53">
+        <v>391874</v>
+      </c>
+      <c r="S53">
+        <v>454542</v>
+      </c>
+      <c r="T53">
+        <v>398966</v>
+      </c>
+      <c r="U53">
+        <v>463874</v>
+      </c>
+      <c r="X53">
+        <v>1</v>
+      </c>
+      <c r="Y53">
+        <v>584680</v>
+      </c>
+      <c r="Z53">
+        <v>679112</v>
+      </c>
+      <c r="AA53">
+        <v>596091</v>
+      </c>
+      <c r="AB53">
+        <v>693950</v>
+      </c>
       <c r="AF53" t="s">
         <v>74</v>
       </c>
@@ -5987,6 +6393,9 @@
       <c r="AI53">
         <v>6608713</v>
       </c>
+      <c r="AJ53">
+        <v>507708</v>
+      </c>
       <c r="AM53">
         <v>6454577</v>
       </c>
@@ -5996,11 +6405,74 @@
       <c r="AO53">
         <v>6527939</v>
       </c>
+      <c r="AP53">
+        <v>512692</v>
+      </c>
       <c r="AS53" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>45070</v>
+      </c>
+      <c r="E54">
+        <v>50847</v>
+      </c>
+      <c r="F54">
+        <v>44333</v>
+      </c>
+      <c r="G54">
+        <v>50440</v>
+      </c>
+      <c r="J54">
+        <v>2</v>
+      </c>
+      <c r="K54">
+        <v>198758</v>
+      </c>
+      <c r="L54">
+        <v>229645</v>
+      </c>
+      <c r="M54">
+        <v>201380</v>
+      </c>
+      <c r="N54">
+        <v>233506</v>
+      </c>
+      <c r="Q54">
+        <v>2</v>
+      </c>
+      <c r="R54">
+        <v>391962</v>
+      </c>
+      <c r="S54">
+        <v>454380</v>
+      </c>
+      <c r="T54">
+        <v>398932</v>
+      </c>
+      <c r="U54">
+        <v>463969</v>
+      </c>
+      <c r="X54">
+        <v>2</v>
+      </c>
+      <c r="Y54">
+        <v>584845</v>
+      </c>
+      <c r="Z54">
+        <v>679117</v>
+      </c>
+      <c r="AA54">
+        <v>596627</v>
+      </c>
+      <c r="AB54">
+        <v>694402</v>
+      </c>
       <c r="AF54" t="s">
         <v>75</v>
       </c>
@@ -6013,6 +6485,9 @@
       <c r="AI54">
         <v>8988982</v>
       </c>
+      <c r="AJ54">
+        <v>636868</v>
+      </c>
       <c r="AM54">
         <v>9137022</v>
       </c>
@@ -6022,8 +6497,576 @@
       <c r="AO54">
         <v>9176962</v>
       </c>
+      <c r="AP54">
+        <v>644165</v>
+      </c>
       <c r="AS54" t="s">
-        <v>172</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>45075</v>
+      </c>
+      <c r="E55">
+        <v>50854</v>
+      </c>
+      <c r="F55">
+        <v>44348</v>
+      </c>
+      <c r="G55">
+        <v>50434</v>
+      </c>
+      <c r="J55">
+        <v>3</v>
+      </c>
+      <c r="K55">
+        <v>198817</v>
+      </c>
+      <c r="L55">
+        <v>229623</v>
+      </c>
+      <c r="M55">
+        <v>201453</v>
+      </c>
+      <c r="N55">
+        <v>233449</v>
+      </c>
+      <c r="Q55">
+        <v>3</v>
+      </c>
+      <c r="R55">
+        <v>391994</v>
+      </c>
+      <c r="S55">
+        <v>454506</v>
+      </c>
+      <c r="T55">
+        <v>399069</v>
+      </c>
+      <c r="U55">
+        <v>463902</v>
+      </c>
+      <c r="X55">
+        <v>3</v>
+      </c>
+      <c r="Y55">
+        <v>584755</v>
+      </c>
+      <c r="Z55">
+        <v>679152</v>
+      </c>
+      <c r="AA55">
+        <v>596374</v>
+      </c>
+      <c r="AB55">
+        <v>694115</v>
+      </c>
+    </row>
+    <row r="56" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <v>45051</v>
+      </c>
+      <c r="E56">
+        <v>50854</v>
+      </c>
+      <c r="F56">
+        <v>44344</v>
+      </c>
+      <c r="G56">
+        <v>50434</v>
+      </c>
+      <c r="J56">
+        <v>4</v>
+      </c>
+      <c r="K56">
+        <v>198771</v>
+      </c>
+      <c r="L56">
+        <v>229585</v>
+      </c>
+      <c r="M56">
+        <v>201412</v>
+      </c>
+      <c r="N56">
+        <v>233367</v>
+      </c>
+      <c r="Q56">
+        <v>4</v>
+      </c>
+      <c r="R56">
+        <v>391839</v>
+      </c>
+      <c r="S56">
+        <v>454754</v>
+      </c>
+      <c r="T56">
+        <v>399069</v>
+      </c>
+      <c r="U56">
+        <v>463908</v>
+      </c>
+      <c r="X56">
+        <v>4</v>
+      </c>
+      <c r="Y56">
+        <v>584905</v>
+      </c>
+      <c r="Z56">
+        <v>679197</v>
+      </c>
+      <c r="AA56">
+        <v>596572</v>
+      </c>
+      <c r="AB56">
+        <v>693883</v>
+      </c>
+    </row>
+    <row r="57" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>45053</v>
+      </c>
+      <c r="E57">
+        <v>50854</v>
+      </c>
+      <c r="F57">
+        <v>44333</v>
+      </c>
+      <c r="G57">
+        <v>50428</v>
+      </c>
+      <c r="J57">
+        <v>5</v>
+      </c>
+      <c r="K57">
+        <v>198794</v>
+      </c>
+      <c r="L57">
+        <v>229597</v>
+      </c>
+      <c r="M57">
+        <v>201408</v>
+      </c>
+      <c r="N57">
+        <v>233519</v>
+      </c>
+      <c r="Q57">
+        <v>5</v>
+      </c>
+      <c r="R57">
+        <v>391907</v>
+      </c>
+      <c r="S57">
+        <v>454475</v>
+      </c>
+      <c r="T57">
+        <v>398948</v>
+      </c>
+      <c r="U57">
+        <v>463817</v>
+      </c>
+      <c r="X57">
+        <v>5</v>
+      </c>
+      <c r="Y57">
+        <v>584878</v>
+      </c>
+      <c r="Z57">
+        <v>678885</v>
+      </c>
+      <c r="AA57">
+        <v>596265</v>
+      </c>
+      <c r="AB57">
+        <v>693997</v>
+      </c>
+    </row>
+    <row r="58" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>6</v>
+      </c>
+      <c r="D58">
+        <v>45053</v>
+      </c>
+      <c r="E58">
+        <v>50859</v>
+      </c>
+      <c r="F58">
+        <v>44374</v>
+      </c>
+      <c r="G58">
+        <v>50459</v>
+      </c>
+      <c r="J58">
+        <v>6</v>
+      </c>
+      <c r="K58">
+        <v>198768</v>
+      </c>
+      <c r="L58">
+        <v>229733</v>
+      </c>
+      <c r="M58">
+        <v>201462</v>
+      </c>
+      <c r="N58">
+        <v>233505</v>
+      </c>
+      <c r="Q58">
+        <v>6</v>
+      </c>
+      <c r="R58">
+        <v>391822</v>
+      </c>
+      <c r="S58">
+        <v>454488</v>
+      </c>
+      <c r="T58">
+        <v>398811</v>
+      </c>
+      <c r="U58">
+        <v>463566</v>
+      </c>
+      <c r="X58">
+        <v>6</v>
+      </c>
+      <c r="Y58">
+        <v>585016</v>
+      </c>
+      <c r="Z58">
+        <v>679328</v>
+      </c>
+      <c r="AA58">
+        <v>596427</v>
+      </c>
+      <c r="AB58">
+        <v>693998</v>
+      </c>
+    </row>
+    <row r="59" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>7</v>
+      </c>
+      <c r="D59">
+        <v>45079</v>
+      </c>
+      <c r="E59">
+        <v>50848</v>
+      </c>
+      <c r="F59">
+        <v>44361</v>
+      </c>
+      <c r="G59">
+        <v>50453</v>
+      </c>
+      <c r="J59">
+        <v>7</v>
+      </c>
+      <c r="K59">
+        <v>198737</v>
+      </c>
+      <c r="L59">
+        <v>229606</v>
+      </c>
+      <c r="M59">
+        <v>201364</v>
+      </c>
+      <c r="N59">
+        <v>233495</v>
+      </c>
+      <c r="Q59">
+        <v>7</v>
+      </c>
+      <c r="R59">
+        <v>391833</v>
+      </c>
+      <c r="S59">
+        <v>454426</v>
+      </c>
+      <c r="T59">
+        <v>398718</v>
+      </c>
+      <c r="U59">
+        <v>463679</v>
+      </c>
+      <c r="X59">
+        <v>7</v>
+      </c>
+      <c r="Y59">
+        <v>584709</v>
+      </c>
+      <c r="Z59">
+        <v>679267</v>
+      </c>
+      <c r="AA59">
+        <v>596379</v>
+      </c>
+      <c r="AB59">
+        <v>693914</v>
+      </c>
+    </row>
+    <row r="60" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>8</v>
+      </c>
+      <c r="D60">
+        <v>45052</v>
+      </c>
+      <c r="E60">
+        <v>50852</v>
+      </c>
+      <c r="F60">
+        <v>44358</v>
+      </c>
+      <c r="G60">
+        <v>50443</v>
+      </c>
+      <c r="J60">
+        <v>8</v>
+      </c>
+      <c r="K60">
+        <v>198666</v>
+      </c>
+      <c r="L60">
+        <v>229623</v>
+      </c>
+      <c r="M60">
+        <v>201355</v>
+      </c>
+      <c r="N60">
+        <v>233509</v>
+      </c>
+      <c r="Q60">
+        <v>8</v>
+      </c>
+      <c r="R60">
+        <v>391856</v>
+      </c>
+      <c r="S60">
+        <v>454569</v>
+      </c>
+      <c r="T60">
+        <v>398880</v>
+      </c>
+      <c r="U60">
+        <v>463877</v>
+      </c>
+      <c r="X60">
+        <v>8</v>
+      </c>
+      <c r="Y60">
+        <v>584739</v>
+      </c>
+      <c r="Z60">
+        <v>679070</v>
+      </c>
+      <c r="AA60">
+        <v>596149</v>
+      </c>
+      <c r="AB60">
+        <v>694056</v>
+      </c>
+    </row>
+    <row r="61" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>9</v>
+      </c>
+      <c r="D61">
+        <v>45046</v>
+      </c>
+      <c r="E61">
+        <v>50851</v>
+      </c>
+      <c r="F61">
+        <v>44370</v>
+      </c>
+      <c r="G61">
+        <v>50457</v>
+      </c>
+      <c r="J61">
+        <v>9</v>
+      </c>
+      <c r="K61">
+        <v>198785</v>
+      </c>
+      <c r="L61">
+        <v>229625</v>
+      </c>
+      <c r="M61">
+        <v>201203</v>
+      </c>
+      <c r="N61">
+        <v>233447</v>
+      </c>
+      <c r="Q61">
+        <v>9</v>
+      </c>
+      <c r="R61">
+        <v>391926</v>
+      </c>
+      <c r="S61">
+        <v>454509</v>
+      </c>
+      <c r="T61">
+        <v>398854</v>
+      </c>
+      <c r="U61">
+        <v>463909</v>
+      </c>
+      <c r="X61">
+        <v>9</v>
+      </c>
+      <c r="Y61">
+        <v>584969</v>
+      </c>
+      <c r="Z61">
+        <v>679122</v>
+      </c>
+      <c r="AA61">
+        <v>596438</v>
+      </c>
+      <c r="AB61">
+        <v>694005</v>
+      </c>
+    </row>
+    <row r="62" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>10</v>
+      </c>
+      <c r="D62">
+        <v>45056</v>
+      </c>
+      <c r="E62">
+        <v>50841</v>
+      </c>
+      <c r="F62">
+        <v>44345</v>
+      </c>
+      <c r="G62">
+        <v>50454</v>
+      </c>
+      <c r="J62">
+        <v>10</v>
+      </c>
+      <c r="K62">
+        <v>198799</v>
+      </c>
+      <c r="L62">
+        <v>229636</v>
+      </c>
+      <c r="M62">
+        <v>201441</v>
+      </c>
+      <c r="N62">
+        <v>233486</v>
+      </c>
+      <c r="Q62">
+        <v>10</v>
+      </c>
+      <c r="R62">
+        <v>391905</v>
+      </c>
+      <c r="S62">
+        <v>454388</v>
+      </c>
+      <c r="T62">
+        <v>398962</v>
+      </c>
+      <c r="U62">
+        <v>463828</v>
+      </c>
+      <c r="X62">
+        <v>10</v>
+      </c>
+      <c r="Y62">
+        <v>584981</v>
+      </c>
+      <c r="Z62">
+        <v>679104</v>
+      </c>
+      <c r="AA62">
+        <v>596331</v>
+      </c>
+      <c r="AB62">
+        <v>694157</v>
+      </c>
+    </row>
+    <row r="64" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D64">
+        <f>AVERAGE(D53:D62)</f>
+        <v>45058.400000000001</v>
+      </c>
+      <c r="E64">
+        <f>AVERAGE(E53:E62)</f>
+        <v>50847.9</v>
+      </c>
+      <c r="F64">
+        <f>AVERAGE(F53:F62)</f>
+        <v>44352.9</v>
+      </c>
+      <c r="G64">
+        <f>AVERAGE(G53:G62)</f>
+        <v>50444.4</v>
+      </c>
+      <c r="K64">
+        <f>AVERAGE(K53:K62)</f>
+        <v>198764.7</v>
+      </c>
+      <c r="L64">
+        <f>AVERAGE(L53:L62)</f>
+        <v>229626.8</v>
+      </c>
+      <c r="M64">
+        <f>AVERAGE(M53:M62)</f>
+        <v>201385.1</v>
+      </c>
+      <c r="N64">
+        <f>AVERAGE(N53:N62)</f>
+        <v>233475.8</v>
+      </c>
+      <c r="R64">
+        <f>AVERAGE(R53:R62)</f>
+        <v>391891.8</v>
+      </c>
+      <c r="S64">
+        <f>AVERAGE(S53:S62)</f>
+        <v>454503.7</v>
+      </c>
+      <c r="T64">
+        <f>AVERAGE(T53:T62)</f>
+        <v>398920.9</v>
+      </c>
+      <c r="U64">
+        <f>AVERAGE(U53:U62)</f>
+        <v>463832.9</v>
+      </c>
+      <c r="Y64">
+        <f>AVERAGE(Y53:Y62)</f>
+        <v>584847.69999999995</v>
+      </c>
+      <c r="Z64">
+        <f>AVERAGE(Z53:Z62)</f>
+        <v>679135.4</v>
+      </c>
+      <c r="AA64">
+        <f>AVERAGE(AA53:AA62)</f>
+        <v>596365.30000000005</v>
+      </c>
+      <c r="AB64">
+        <f>AVERAGE(AB53:AB62)</f>
+        <v>694047.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New benchmark results, removed unused variables in sketch
</commit_message>
<xml_diff>
--- a/BenchmarkDocs/Results.xlsx
+++ b/BenchmarkDocs/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f0dc99f0b729840/Teilen/edge-ml/feature-extraction/BenchmarkDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1257" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B9FCEEB-C682-4095-9202-07A7BAED7199}"/>
+  <xr:revisionPtr revIDLastSave="1516" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21F89C13-3EF6-42B3-B6CD-D15BCAAA8470}"/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="150" windowWidth="15960" windowHeight="14280" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="177">
   <si>
     <t>Arduino</t>
   </si>
@@ -560,6 +560,12 @@
   </si>
   <si>
     <t xml:space="preserve">06.02. </t>
+  </si>
+  <si>
+    <t>Stand: 05.02.</t>
+  </si>
+  <si>
+    <t>Neu:Iter fix, unused</t>
   </si>
 </sst>
 </file>
@@ -940,40 +946,40 @@
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" customWidth="1"/>
-    <col min="11" max="11" width="26.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" customWidth="1"/>
-    <col min="21" max="21" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" customWidth="1"/>
+    <col min="11" max="11" width="26.44140625" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" customWidth="1"/>
+    <col min="16" max="16" width="12.88671875" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" customWidth="1"/>
+    <col min="21" max="21" width="22.33203125" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" customWidth="1"/>
-    <col min="24" max="24" width="11.140625" customWidth="1"/>
-    <col min="25" max="25" width="16.42578125" customWidth="1"/>
-    <col min="26" max="26" width="11.28515625" customWidth="1"/>
-    <col min="29" max="29" width="16.140625" customWidth="1"/>
-    <col min="30" max="30" width="35.7109375" customWidth="1"/>
+    <col min="23" max="23" width="11.44140625" customWidth="1"/>
+    <col min="24" max="24" width="11.109375" customWidth="1"/>
+    <col min="25" max="25" width="16.44140625" customWidth="1"/>
+    <col min="26" max="26" width="11.33203125" customWidth="1"/>
+    <col min="29" max="29" width="16.109375" customWidth="1"/>
+    <col min="30" max="30" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>33</v>
       </c>
@@ -1005,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -1052,7 +1058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>1</v>
       </c>
@@ -1096,7 +1102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>2</v>
       </c>
@@ -1131,7 +1137,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>3</v>
       </c>
@@ -1166,7 +1172,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>4</v>
       </c>
@@ -1201,7 +1207,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>5</v>
       </c>
@@ -1236,7 +1242,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>6</v>
       </c>
@@ -1271,7 +1277,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>7</v>
       </c>
@@ -1306,7 +1312,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>8</v>
       </c>
@@ -1341,7 +1347,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>9</v>
       </c>
@@ -1376,7 +1382,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>10</v>
       </c>
@@ -1411,12 +1417,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -1457,7 +1463,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>5</v>
       </c>
@@ -1531,7 +1537,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>1</v>
       </c>
@@ -1587,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>2</v>
       </c>
@@ -1643,7 +1649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>3</v>
       </c>
@@ -1699,7 +1705,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>4</v>
       </c>
@@ -1755,7 +1761,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>5</v>
       </c>
@@ -1811,7 +1817,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>6</v>
       </c>
@@ -1867,7 +1873,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>7</v>
       </c>
@@ -1923,7 +1929,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>8</v>
       </c>
@@ -1979,7 +1985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>9</v>
       </c>
@@ -2035,7 +2041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>10</v>
       </c>
@@ -2091,7 +2097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T29">
         <v>10</v>
       </c>
@@ -2111,7 +2117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T30">
         <v>8</v>
       </c>
@@ -2131,7 +2137,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T31">
         <v>8</v>
       </c>
@@ -2151,7 +2157,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T32">
         <v>10</v>
       </c>
@@ -2171,7 +2177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>114</v>
       </c>
@@ -2194,7 +2200,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>98</v>
       </c>
@@ -2238,7 +2244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>97</v>
       </c>
@@ -2279,7 +2285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T36">
         <v>3</v>
       </c>
@@ -2299,7 +2305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T37">
         <v>20</v>
       </c>
@@ -2319,7 +2325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T38">
         <v>20</v>
       </c>
@@ -2339,7 +2345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>98</v>
       </c>
@@ -2371,7 +2377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>124</v>
       </c>
@@ -2403,7 +2409,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>127</v>
       </c>
@@ -2432,7 +2438,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>128</v>
       </c>
@@ -2446,7 +2452,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>136</v>
       </c>
@@ -2478,7 +2484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>139</v>
       </c>
@@ -2510,7 +2516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>140</v>
       </c>
@@ -2545,7 +2551,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>141</v>
       </c>
@@ -2577,7 +2583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>137</v>
       </c>
@@ -2591,7 +2597,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>148</v>
       </c>
@@ -2626,7 +2632,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>149</v>
       </c>
@@ -2658,7 +2664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>152</v>
       </c>
@@ -2693,7 +2699,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T51">
         <v>11</v>
       </c>
@@ -2713,7 +2719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T52">
         <v>16</v>
       </c>
@@ -2736,7 +2742,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T53">
         <v>11</v>
       </c>
@@ -2756,7 +2762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T54">
         <v>16</v>
       </c>
@@ -2776,7 +2782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T55">
         <v>16</v>
       </c>
@@ -2799,7 +2805,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T56">
         <v>8</v>
       </c>
@@ -2819,7 +2825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T57">
         <v>19</v>
       </c>
@@ -2839,7 +2845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T58">
         <v>17</v>
       </c>
@@ -2859,7 +2865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T59">
         <v>17</v>
       </c>
@@ -2879,12 +2885,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:30" x14ac:dyDescent="0.3">
       <c r="AD60" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T61">
         <v>15</v>
       </c>
@@ -2904,7 +2910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T63">
         <v>4</v>
       </c>
@@ -2912,7 +2918,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:30" x14ac:dyDescent="0.3">
       <c r="T64">
         <v>3</v>
       </c>
@@ -2920,7 +2926,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="20:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="20:21" x14ac:dyDescent="0.3">
       <c r="T65">
         <v>3</v>
       </c>
@@ -2928,7 +2934,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="20:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="20:21" x14ac:dyDescent="0.3">
       <c r="T66">
         <v>4</v>
       </c>
@@ -2944,36 +2950,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DC238C-8F4B-441F-9A1D-B395F114E22E}">
-  <dimension ref="A1:AS64"/>
+  <dimension ref="A1:AS80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA62" sqref="AA62"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" customWidth="1"/>
-    <col min="26" max="26" width="13.28515625" customWidth="1"/>
-    <col min="30" max="30" width="12.140625" customWidth="1"/>
-    <col min="31" max="31" width="9.5703125" customWidth="1"/>
-    <col min="32" max="32" width="23.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" customWidth="1"/>
+    <col min="16" max="16" width="13.109375" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" customWidth="1"/>
+    <col min="19" max="19" width="13.44140625" customWidth="1"/>
+    <col min="22" max="22" width="12.5546875" customWidth="1"/>
+    <col min="26" max="26" width="13.33203125" customWidth="1"/>
+    <col min="30" max="30" width="12.109375" customWidth="1"/>
+    <col min="31" max="31" width="9.5546875" customWidth="1"/>
+    <col min="32" max="32" width="23.5546875" customWidth="1"/>
     <col min="45" max="45" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>154</v>
       </c>
@@ -2981,7 +2987,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -3016,7 +3022,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="J4" t="s">
         <v>5</v>
       </c>
@@ -3087,7 +3093,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="J5">
         <v>1</v>
       </c>
@@ -3133,6 +3139,9 @@
       <c r="AJ5">
         <v>128</v>
       </c>
+      <c r="AK5">
+        <v>188</v>
+      </c>
       <c r="AM5">
         <v>1639</v>
       </c>
@@ -3145,8 +3154,11 @@
       <c r="AP5">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ5">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="J6">
         <v>2</v>
       </c>
@@ -3192,6 +3204,9 @@
       <c r="AJ6">
         <v>317</v>
       </c>
+      <c r="AK6">
+        <v>352</v>
+      </c>
       <c r="AM6">
         <v>4630</v>
       </c>
@@ -3204,8 +3219,11 @@
       <c r="AP6">
         <v>391</v>
       </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ6">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="J7">
         <v>3</v>
       </c>
@@ -3251,6 +3269,9 @@
       <c r="AJ7">
         <v>2128</v>
       </c>
+      <c r="AK7">
+        <v>2250</v>
+      </c>
       <c r="AM7">
         <v>52201</v>
       </c>
@@ -3263,8 +3284,11 @@
       <c r="AP7">
         <v>2140</v>
       </c>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ7">
+        <v>2186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="J8">
         <v>4</v>
       </c>
@@ -3310,6 +3334,9 @@
       <c r="AJ8">
         <v>2269</v>
       </c>
+      <c r="AK8">
+        <v>2348</v>
+      </c>
       <c r="AM8">
         <v>15579</v>
       </c>
@@ -3322,8 +3349,11 @@
       <c r="AP8">
         <v>2351</v>
       </c>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ8">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="J9">
         <v>5</v>
       </c>
@@ -3369,6 +3399,9 @@
       <c r="AJ9">
         <v>3922</v>
       </c>
+      <c r="AK9">
+        <v>3977</v>
+      </c>
       <c r="AM9">
         <v>19193</v>
       </c>
@@ -3381,8 +3414,11 @@
       <c r="AP9">
         <v>3977</v>
       </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ9">
+        <v>4011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="J10">
         <v>6</v>
       </c>
@@ -3428,6 +3464,9 @@
       <c r="AJ10">
         <v>3830</v>
       </c>
+      <c r="AK10">
+        <v>3882</v>
+      </c>
       <c r="AM10">
         <v>18477</v>
       </c>
@@ -3440,8 +3479,11 @@
       <c r="AP10">
         <v>3875</v>
       </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ10">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="J11">
         <v>7</v>
       </c>
@@ -3487,6 +3529,9 @@
       <c r="AJ11">
         <v>5377</v>
       </c>
+      <c r="AK11">
+        <v>5408</v>
+      </c>
       <c r="AM11">
         <v>33520</v>
       </c>
@@ -3499,8 +3544,11 @@
       <c r="AP11">
         <v>5439</v>
       </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ11">
+        <v>5450</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="J12">
         <v>8</v>
       </c>
@@ -3546,6 +3594,9 @@
       <c r="AJ12">
         <v>11866</v>
       </c>
+      <c r="AK12">
+        <v>11926</v>
+      </c>
       <c r="AM12">
         <v>5822</v>
       </c>
@@ -3558,8 +3609,11 @@
       <c r="AP12">
         <v>12347</v>
       </c>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ12">
+        <v>12354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="J13">
         <v>9</v>
       </c>
@@ -3605,6 +3659,9 @@
       <c r="AJ13">
         <v>289</v>
       </c>
+      <c r="AK13">
+        <v>322</v>
+      </c>
       <c r="AM13">
         <v>4641</v>
       </c>
@@ -3617,8 +3674,11 @@
       <c r="AP13">
         <v>435</v>
       </c>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ13">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="J14">
         <v>10</v>
       </c>
@@ -3664,6 +3724,9 @@
       <c r="AJ14">
         <v>11888</v>
       </c>
+      <c r="AK14">
+        <v>11916</v>
+      </c>
       <c r="AM14">
         <v>5741</v>
       </c>
@@ -3676,8 +3739,11 @@
       <c r="AP14">
         <v>12335</v>
       </c>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ14">
+        <v>12314</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="AF15" t="s">
         <v>45</v>
       </c>
@@ -3693,6 +3759,9 @@
       <c r="AJ15">
         <v>11716</v>
       </c>
+      <c r="AK15">
+        <v>11751</v>
+      </c>
       <c r="AM15">
         <v>2914</v>
       </c>
@@ -3705,8 +3774,11 @@
       <c r="AP15">
         <v>12271</v>
       </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AQ15">
+        <v>12263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>166</v>
       </c>
@@ -3757,6 +3829,9 @@
       <c r="AJ16">
         <v>172595</v>
       </c>
+      <c r="AK16">
+        <v>172628</v>
+      </c>
       <c r="AM16">
         <v>181033</v>
       </c>
@@ -3769,8 +3844,11 @@
       <c r="AP16">
         <v>176635</v>
       </c>
-    </row>
-    <row r="17" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ16">
+        <v>176607</v>
+      </c>
+    </row>
+    <row r="17" spans="2:45" x14ac:dyDescent="0.3">
       <c r="AF17" t="s">
         <v>47</v>
       </c>
@@ -3786,6 +3864,9 @@
       <c r="AJ17">
         <v>173288</v>
       </c>
+      <c r="AK17">
+        <v>173321</v>
+      </c>
       <c r="AM17">
         <v>181693</v>
       </c>
@@ -3798,8 +3879,11 @@
       <c r="AP17">
         <v>177095</v>
       </c>
-    </row>
-    <row r="18" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ17">
+        <v>177034</v>
+      </c>
+    </row>
+    <row r="18" spans="2:45" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>160</v>
       </c>
@@ -3821,6 +3905,9 @@
       <c r="AJ18">
         <v>989</v>
       </c>
+      <c r="AK18">
+        <v>1024</v>
+      </c>
       <c r="AM18">
         <v>4074</v>
       </c>
@@ -3833,8 +3920,11 @@
       <c r="AP18">
         <v>1030</v>
       </c>
-    </row>
-    <row r="19" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ18">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="19" spans="2:45" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>33</v>
       </c>
@@ -3875,7 +3965,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>5</v>
       </c>
@@ -3951,6 +4041,9 @@
       <c r="AJ20">
         <v>175</v>
       </c>
+      <c r="AK20">
+        <v>236</v>
+      </c>
       <c r="AM20">
         <v>1303</v>
       </c>
@@ -3963,8 +4056,11 @@
       <c r="AP20">
         <v>171</v>
       </c>
-    </row>
-    <row r="21" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ20">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>1</v>
       </c>
@@ -4040,6 +4136,9 @@
       <c r="AJ21">
         <v>219</v>
       </c>
+      <c r="AK21">
+        <v>255</v>
+      </c>
       <c r="AM21">
         <v>1194</v>
       </c>
@@ -4052,8 +4151,11 @@
       <c r="AP21">
         <v>216</v>
       </c>
-    </row>
-    <row r="22" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ21">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>2</v>
       </c>
@@ -4129,6 +4231,9 @@
       <c r="AJ22">
         <v>176</v>
       </c>
+      <c r="AK22">
+        <v>206</v>
+      </c>
       <c r="AM22">
         <v>1150</v>
       </c>
@@ -4141,8 +4246,11 @@
       <c r="AP22">
         <v>258</v>
       </c>
-    </row>
-    <row r="23" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ22">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>3</v>
       </c>
@@ -4218,6 +4326,9 @@
       <c r="AJ23">
         <v>828</v>
       </c>
+      <c r="AK23">
+        <v>921</v>
+      </c>
       <c r="AM23">
         <v>2829</v>
       </c>
@@ -4230,8 +4341,11 @@
       <c r="AP23">
         <v>802</v>
       </c>
-    </row>
-    <row r="24" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ23">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="24" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>4</v>
       </c>
@@ -4307,6 +4421,9 @@
       <c r="AJ24">
         <v>797</v>
       </c>
+      <c r="AK24">
+        <v>918</v>
+      </c>
       <c r="AM24">
         <v>2704</v>
       </c>
@@ -4319,8 +4436,11 @@
       <c r="AP24">
         <v>802</v>
       </c>
-    </row>
-    <row r="25" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ24">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="25" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>5</v>
       </c>
@@ -4396,6 +4516,9 @@
       <c r="AJ25">
         <v>305</v>
       </c>
+      <c r="AK25">
+        <v>428</v>
+      </c>
       <c r="AM25">
         <v>1709</v>
       </c>
@@ -4408,8 +4531,11 @@
       <c r="AP25">
         <v>301</v>
       </c>
-    </row>
-    <row r="26" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>6</v>
       </c>
@@ -4485,6 +4611,9 @@
       <c r="AJ26">
         <v>237</v>
       </c>
+      <c r="AK26">
+        <v>360</v>
+      </c>
       <c r="AM26">
         <v>1204</v>
       </c>
@@ -4497,11 +4626,14 @@
       <c r="AP26">
         <v>217</v>
       </c>
+      <c r="AQ26">
+        <v>877</v>
+      </c>
       <c r="AS26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>7</v>
       </c>
@@ -4577,6 +4709,9 @@
       <c r="AJ27">
         <v>2626</v>
       </c>
+      <c r="AK27">
+        <v>2626</v>
+      </c>
       <c r="AM27">
         <v>16089</v>
       </c>
@@ -4589,8 +4724,11 @@
       <c r="AP27">
         <v>2679</v>
       </c>
-    </row>
-    <row r="28" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ27">
+        <v>2663</v>
+      </c>
+    </row>
+    <row r="28" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>8</v>
       </c>
@@ -4652,7 +4790,7 @@
         <v>1039427</v>
       </c>
     </row>
-    <row r="29" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>9</v>
       </c>
@@ -4728,6 +4866,9 @@
       <c r="AJ29">
         <v>1868</v>
       </c>
+      <c r="AK29">
+        <v>1930</v>
+      </c>
       <c r="AM29">
         <v>5007</v>
       </c>
@@ -4740,8 +4881,11 @@
       <c r="AP29">
         <v>1885</v>
       </c>
-    </row>
-    <row r="30" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ29">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="30" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>10</v>
       </c>
@@ -4817,6 +4961,9 @@
       <c r="AJ30">
         <v>1854</v>
       </c>
+      <c r="AK30">
+        <v>1893</v>
+      </c>
       <c r="AM30">
         <v>5298</v>
       </c>
@@ -4829,8 +4976,11 @@
       <c r="AP30">
         <v>1885</v>
       </c>
-    </row>
-    <row r="31" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ30">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="31" spans="2:45" x14ac:dyDescent="0.3">
       <c r="AF31" t="s">
         <v>56</v>
       </c>
@@ -4846,6 +4996,9 @@
       <c r="AJ31">
         <v>1903</v>
       </c>
+      <c r="AK31">
+        <v>1997</v>
+      </c>
       <c r="AM31">
         <v>5098</v>
       </c>
@@ -4858,11 +5011,14 @@
       <c r="AP31">
         <v>1966</v>
       </c>
+      <c r="AQ31">
+        <v>2044</v>
+      </c>
       <c r="AS31" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:45" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>166</v>
       </c>
@@ -4945,6 +5101,9 @@
       <c r="AJ32">
         <v>2868</v>
       </c>
+      <c r="AK32">
+        <v>2896</v>
+      </c>
       <c r="AM32">
         <v>17526</v>
       </c>
@@ -4957,8 +5116,11 @@
       <c r="AP32">
         <v>2863</v>
       </c>
-    </row>
-    <row r="34" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ32">
+        <v>2829</v>
+      </c>
+    </row>
+    <row r="34" spans="2:45" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>167</v>
       </c>
@@ -4977,6 +5139,9 @@
       <c r="AJ34">
         <v>128</v>
       </c>
+      <c r="AK34">
+        <v>159</v>
+      </c>
       <c r="AM34">
         <v>1653</v>
       </c>
@@ -4989,11 +5154,14 @@
       <c r="AP34">
         <v>156</v>
       </c>
+      <c r="AQ34">
+        <v>230</v>
+      </c>
       <c r="AS34" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:45" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>33</v>
       </c>
@@ -5048,6 +5216,9 @@
       <c r="AJ35">
         <v>514</v>
       </c>
+      <c r="AK35">
+        <v>486</v>
+      </c>
       <c r="AM35">
         <v>2774</v>
       </c>
@@ -5060,8 +5231,11 @@
       <c r="AP35">
         <v>424</v>
       </c>
-    </row>
-    <row r="36" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ35">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="36" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
         <v>5</v>
       </c>
@@ -5137,6 +5311,9 @@
       <c r="AJ36">
         <v>312</v>
       </c>
+      <c r="AK36">
+        <v>255</v>
+      </c>
       <c r="AM36">
         <v>2944</v>
       </c>
@@ -5149,11 +5326,14 @@
       <c r="AP36">
         <v>316</v>
       </c>
+      <c r="AQ36">
+        <v>298</v>
+      </c>
       <c r="AS36" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C37">
         <v>1</v>
       </c>
@@ -5229,6 +5409,9 @@
       <c r="AJ37">
         <v>331</v>
       </c>
+      <c r="AK37">
+        <v>331</v>
+      </c>
       <c r="AM37">
         <v>2278</v>
       </c>
@@ -5241,8 +5424,11 @@
       <c r="AP37">
         <v>225</v>
       </c>
-    </row>
-    <row r="38" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ37">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="38" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C38">
         <v>2</v>
       </c>
@@ -5318,6 +5504,9 @@
       <c r="AJ38">
         <v>492</v>
       </c>
+      <c r="AK38">
+        <v>584</v>
+      </c>
       <c r="AM38">
         <v>3882</v>
       </c>
@@ -5330,11 +5519,14 @@
       <c r="AP38">
         <v>395</v>
       </c>
+      <c r="AQ38">
+        <v>419</v>
+      </c>
       <c r="AS38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>3</v>
       </c>
@@ -5410,6 +5602,9 @@
       <c r="AJ39">
         <v>233</v>
       </c>
+      <c r="AK39">
+        <v>233</v>
+      </c>
       <c r="AM39">
         <v>2098</v>
       </c>
@@ -5422,8 +5617,11 @@
       <c r="AP39">
         <v>330</v>
       </c>
-    </row>
-    <row r="40" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ39">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="40" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C40">
         <v>4</v>
       </c>
@@ -5499,6 +5697,9 @@
       <c r="AJ40">
         <v>359</v>
       </c>
+      <c r="AK40">
+        <v>455</v>
+      </c>
       <c r="AM40">
         <v>3696</v>
       </c>
@@ -5511,8 +5712,11 @@
       <c r="AP40">
         <v>428</v>
       </c>
-    </row>
-    <row r="41" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ40">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="41" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>5</v>
       </c>
@@ -5588,6 +5792,9 @@
       <c r="AJ41">
         <v>11776</v>
       </c>
+      <c r="AK41">
+        <v>11865</v>
+      </c>
       <c r="AM41">
         <v>2930</v>
       </c>
@@ -5600,11 +5807,14 @@
       <c r="AP41">
         <v>12316</v>
       </c>
+      <c r="AQ41">
+        <v>12344</v>
+      </c>
       <c r="AS41" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>6</v>
       </c>
@@ -5680,6 +5890,9 @@
       <c r="AJ42">
         <v>2389</v>
       </c>
+      <c r="AK42">
+        <v>2379</v>
+      </c>
       <c r="AM42">
         <v>15644</v>
       </c>
@@ -5692,8 +5905,11 @@
       <c r="AP42">
         <v>2402</v>
       </c>
-    </row>
-    <row r="43" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ42">
+        <v>2370</v>
+      </c>
+    </row>
+    <row r="43" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C43">
         <v>7</v>
       </c>
@@ -5769,6 +5985,9 @@
       <c r="AJ43">
         <v>4597</v>
       </c>
+      <c r="AK43">
+        <v>4775</v>
+      </c>
       <c r="AM43">
         <v>31208</v>
       </c>
@@ -5781,8 +6000,11 @@
       <c r="AP43">
         <v>4742</v>
       </c>
-    </row>
-    <row r="44" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ43">
+        <v>4733</v>
+      </c>
+    </row>
+    <row r="44" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C44">
         <v>8</v>
       </c>
@@ -5858,6 +6080,9 @@
       <c r="AJ44">
         <v>1230</v>
       </c>
+      <c r="AK44">
+        <v>1309</v>
+      </c>
       <c r="AM44">
         <v>3562</v>
       </c>
@@ -5870,8 +6095,11 @@
       <c r="AP44">
         <v>1235</v>
       </c>
-    </row>
-    <row r="45" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ44">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="45" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C45">
         <v>9</v>
       </c>
@@ -5947,6 +6175,9 @@
       <c r="AJ45">
         <v>1224</v>
       </c>
+      <c r="AK45">
+        <v>1316</v>
+      </c>
       <c r="AM45">
         <v>3449</v>
       </c>
@@ -5959,8 +6190,11 @@
       <c r="AP45">
         <v>1228</v>
       </c>
-    </row>
-    <row r="46" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ45">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="46" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C46">
         <v>10</v>
       </c>
@@ -6036,6 +6270,9 @@
       <c r="AJ46">
         <v>13122</v>
       </c>
+      <c r="AK46">
+        <v>13120</v>
+      </c>
       <c r="AM46">
         <v>12547</v>
       </c>
@@ -6048,11 +6285,14 @@
       <c r="AP46">
         <v>13586</v>
       </c>
+      <c r="AQ46">
+        <v>13498</v>
+      </c>
       <c r="AS46" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:45" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
         <v>166</v>
       </c>
@@ -6139,6 +6379,10 @@
         <f>SUM(AJ5:AJ46)</f>
         <v>451165</v>
       </c>
+      <c r="AK48">
+        <f>SUM(AK5:AK46)</f>
+        <v>453226</v>
+      </c>
       <c r="AM48">
         <f>SUM(AM5:AM46)</f>
         <v>680933</v>
@@ -6151,8 +6395,16 @@
         <f>SUM(AO5:AO46)</f>
         <v>687570</v>
       </c>
-    </row>
-    <row r="50" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AP48">
+        <f>SUM(AP5:AP46)</f>
+        <v>462274</v>
+      </c>
+      <c r="AQ48">
+        <f>SUM(AQ5:AQ46)</f>
+        <v>463613</v>
+      </c>
+    </row>
+    <row r="50" spans="2:45" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>172</v>
       </c>
@@ -6160,7 +6412,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:45" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>33</v>
       </c>
@@ -6215,6 +6467,9 @@
       <c r="AJ51">
         <v>16900049</v>
       </c>
+      <c r="AK51">
+        <v>16899798</v>
+      </c>
       <c r="AM51">
         <v>17405915</v>
       </c>
@@ -6227,11 +6482,14 @@
       <c r="AP51">
         <v>17271362</v>
       </c>
+      <c r="AQ51">
+        <v>17272073</v>
+      </c>
       <c r="AS51" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="52" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
         <v>5</v>
       </c>
@@ -6307,6 +6565,9 @@
       <c r="AJ52">
         <v>19496</v>
       </c>
+      <c r="AK52">
+        <v>19532</v>
+      </c>
       <c r="AM52">
         <v>105728</v>
       </c>
@@ -6319,8 +6580,11 @@
       <c r="AP52">
         <v>19843</v>
       </c>
-    </row>
-    <row r="53" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="AQ52">
+        <v>19809</v>
+      </c>
+    </row>
+    <row r="53" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C53">
         <v>1</v>
       </c>
@@ -6396,6 +6660,9 @@
       <c r="AJ53">
         <v>507708</v>
       </c>
+      <c r="AK53">
+        <v>507645</v>
+      </c>
       <c r="AM53">
         <v>6454577</v>
       </c>
@@ -6408,11 +6675,14 @@
       <c r="AP53">
         <v>512692</v>
       </c>
+      <c r="AQ53">
+        <v>512678</v>
+      </c>
       <c r="AS53" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="54" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C54">
         <v>2</v>
       </c>
@@ -6488,6 +6758,9 @@
       <c r="AJ54">
         <v>636868</v>
       </c>
+      <c r="AK54">
+        <v>636969</v>
+      </c>
       <c r="AM54">
         <v>9137022</v>
       </c>
@@ -6500,11 +6773,14 @@
       <c r="AP54">
         <v>644165</v>
       </c>
+      <c r="AQ54">
+        <v>643664</v>
+      </c>
       <c r="AS54" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C55">
         <v>3</v>
       </c>
@@ -6566,7 +6842,7 @@
         <v>694115</v>
       </c>
     </row>
-    <row r="56" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C56">
         <v>4</v>
       </c>
@@ -6628,7 +6904,7 @@
         <v>693883</v>
       </c>
     </row>
-    <row r="57" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C57">
         <v>5</v>
       </c>
@@ -6690,7 +6966,7 @@
         <v>693997</v>
       </c>
     </row>
-    <row r="58" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C58">
         <v>6</v>
       </c>
@@ -6752,7 +7028,7 @@
         <v>693998</v>
       </c>
     </row>
-    <row r="59" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C59">
         <v>7</v>
       </c>
@@ -6814,7 +7090,7 @@
         <v>693914</v>
       </c>
     </row>
-    <row r="60" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C60">
         <v>8</v>
       </c>
@@ -6876,7 +7152,7 @@
         <v>694056</v>
       </c>
     </row>
-    <row r="61" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C61">
         <v>9</v>
       </c>
@@ -6938,7 +7214,7 @@
         <v>694005</v>
       </c>
     </row>
-    <row r="62" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:45" x14ac:dyDescent="0.3">
       <c r="C62">
         <v>10</v>
       </c>
@@ -7000,7 +7276,7 @@
         <v>694157</v>
       </c>
     </row>
-    <row r="64" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:45" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
         <v>166</v>
       </c>
@@ -7067,6 +7343,806 @@
       <c r="AB64">
         <f>AVERAGE(AB53:AB62)</f>
         <v>694047.7</v>
+      </c>
+    </row>
+    <row r="66" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>175</v>
+      </c>
+      <c r="C66" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="67" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" t="s">
+        <v>164</v>
+      </c>
+      <c r="D67" t="s">
+        <v>96</v>
+      </c>
+      <c r="F67" t="s">
+        <v>97</v>
+      </c>
+      <c r="J67" t="s">
+        <v>26</v>
+      </c>
+      <c r="K67" t="s">
+        <v>96</v>
+      </c>
+      <c r="M67" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>1</v>
+      </c>
+      <c r="R67" t="s">
+        <v>96</v>
+      </c>
+      <c r="T67" t="s">
+        <v>97</v>
+      </c>
+      <c r="X67" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA67" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="68" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>4</v>
+      </c>
+      <c r="F68" t="s">
+        <v>3</v>
+      </c>
+      <c r="G68" t="s">
+        <v>4</v>
+      </c>
+      <c r="J68" t="s">
+        <v>5</v>
+      </c>
+      <c r="K68" t="s">
+        <v>3</v>
+      </c>
+      <c r="L68" t="s">
+        <v>4</v>
+      </c>
+      <c r="M68" t="s">
+        <v>3</v>
+      </c>
+      <c r="N68" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>5</v>
+      </c>
+      <c r="R68" t="s">
+        <v>3</v>
+      </c>
+      <c r="S68" t="s">
+        <v>4</v>
+      </c>
+      <c r="T68" t="s">
+        <v>3</v>
+      </c>
+      <c r="U68" t="s">
+        <v>4</v>
+      </c>
+      <c r="X68" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA68" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>45050</v>
+      </c>
+      <c r="E69">
+        <v>50850</v>
+      </c>
+      <c r="F69">
+        <v>44317</v>
+      </c>
+      <c r="G69">
+        <v>50430</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <v>198805</v>
+      </c>
+      <c r="L69">
+        <v>229668</v>
+      </c>
+      <c r="M69">
+        <v>201360</v>
+      </c>
+      <c r="N69">
+        <v>233458</v>
+      </c>
+      <c r="Q69">
+        <v>1</v>
+      </c>
+      <c r="R69">
+        <v>391988</v>
+      </c>
+      <c r="S69">
+        <v>454373</v>
+      </c>
+      <c r="T69">
+        <v>398918</v>
+      </c>
+      <c r="U69">
+        <v>463717</v>
+      </c>
+      <c r="X69">
+        <v>1</v>
+      </c>
+      <c r="Y69">
+        <v>584895</v>
+      </c>
+      <c r="Z69">
+        <v>679029</v>
+      </c>
+      <c r="AA69">
+        <v>596305</v>
+      </c>
+      <c r="AB69">
+        <v>693930</v>
+      </c>
+    </row>
+    <row r="70" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>45053</v>
+      </c>
+      <c r="E70">
+        <v>50849</v>
+      </c>
+      <c r="F70">
+        <v>44334</v>
+      </c>
+      <c r="G70">
+        <v>50392</v>
+      </c>
+      <c r="J70">
+        <v>2</v>
+      </c>
+      <c r="K70">
+        <v>198765</v>
+      </c>
+      <c r="L70">
+        <v>229747</v>
+      </c>
+      <c r="M70">
+        <v>201342</v>
+      </c>
+      <c r="N70">
+        <v>233467</v>
+      </c>
+      <c r="Q70">
+        <v>2</v>
+      </c>
+      <c r="R70">
+        <v>391928</v>
+      </c>
+      <c r="S70">
+        <v>454264</v>
+      </c>
+      <c r="T70">
+        <v>398976</v>
+      </c>
+      <c r="U70">
+        <v>463754</v>
+      </c>
+      <c r="X70">
+        <v>2</v>
+      </c>
+      <c r="Y70">
+        <v>584909</v>
+      </c>
+      <c r="Z70">
+        <v>679251</v>
+      </c>
+      <c r="AA70">
+        <v>596509</v>
+      </c>
+      <c r="AB70">
+        <v>694477</v>
+      </c>
+    </row>
+    <row r="71" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>45042</v>
+      </c>
+      <c r="E71">
+        <v>50870</v>
+      </c>
+      <c r="F71">
+        <v>44312</v>
+      </c>
+      <c r="G71">
+        <v>50432</v>
+      </c>
+      <c r="J71">
+        <v>3</v>
+      </c>
+      <c r="K71">
+        <v>198708</v>
+      </c>
+      <c r="L71">
+        <v>229592</v>
+      </c>
+      <c r="M71">
+        <v>201352</v>
+      </c>
+      <c r="N71">
+        <v>233512</v>
+      </c>
+      <c r="Q71">
+        <v>3</v>
+      </c>
+      <c r="R71">
+        <v>391876</v>
+      </c>
+      <c r="S71">
+        <v>454419</v>
+      </c>
+      <c r="T71">
+        <v>398942</v>
+      </c>
+      <c r="U71">
+        <v>463974</v>
+      </c>
+      <c r="X71">
+        <v>3</v>
+      </c>
+      <c r="Y71">
+        <v>585131</v>
+      </c>
+      <c r="Z71">
+        <v>678898</v>
+      </c>
+      <c r="AA71">
+        <v>596337</v>
+      </c>
+      <c r="AB71">
+        <v>694283</v>
+      </c>
+    </row>
+    <row r="72" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <v>45046</v>
+      </c>
+      <c r="E72">
+        <v>50856</v>
+      </c>
+      <c r="F72">
+        <v>44328</v>
+      </c>
+      <c r="G72">
+        <v>50419</v>
+      </c>
+      <c r="J72">
+        <v>4</v>
+      </c>
+      <c r="K72">
+        <v>198788</v>
+      </c>
+      <c r="L72">
+        <v>229501</v>
+      </c>
+      <c r="M72">
+        <v>201096</v>
+      </c>
+      <c r="N72">
+        <v>233527</v>
+      </c>
+      <c r="Q72">
+        <v>4</v>
+      </c>
+      <c r="R72">
+        <v>391963</v>
+      </c>
+      <c r="S72">
+        <v>454368</v>
+      </c>
+      <c r="T72">
+        <v>398981</v>
+      </c>
+      <c r="U72">
+        <v>463986</v>
+      </c>
+      <c r="X72">
+        <v>4</v>
+      </c>
+      <c r="Y72">
+        <v>584923</v>
+      </c>
+      <c r="Z72">
+        <v>679021</v>
+      </c>
+      <c r="AA72">
+        <v>596246</v>
+      </c>
+      <c r="AB72">
+        <v>694253</v>
+      </c>
+    </row>
+    <row r="73" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C73">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>45047</v>
+      </c>
+      <c r="E73">
+        <v>50856</v>
+      </c>
+      <c r="F73">
+        <v>44339</v>
+      </c>
+      <c r="G73">
+        <v>50410</v>
+      </c>
+      <c r="J73">
+        <v>5</v>
+      </c>
+      <c r="K73">
+        <v>198786</v>
+      </c>
+      <c r="L73">
+        <v>229617</v>
+      </c>
+      <c r="M73">
+        <v>201277</v>
+      </c>
+      <c r="N73">
+        <v>233528</v>
+      </c>
+      <c r="Q73">
+        <v>5</v>
+      </c>
+      <c r="R73">
+        <v>391961</v>
+      </c>
+      <c r="S73">
+        <v>454515</v>
+      </c>
+      <c r="T73">
+        <v>399077</v>
+      </c>
+      <c r="U73">
+        <v>463891</v>
+      </c>
+      <c r="X73">
+        <v>5</v>
+      </c>
+      <c r="Y73">
+        <v>584988</v>
+      </c>
+      <c r="Z73">
+        <v>679050</v>
+      </c>
+      <c r="AA73">
+        <v>596433</v>
+      </c>
+      <c r="AB73">
+        <v>694410</v>
+      </c>
+    </row>
+    <row r="74" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C74">
+        <v>6</v>
+      </c>
+      <c r="D74">
+        <v>45051</v>
+      </c>
+      <c r="E74">
+        <v>50856</v>
+      </c>
+      <c r="F74">
+        <v>44329</v>
+      </c>
+      <c r="G74">
+        <v>50436</v>
+      </c>
+      <c r="J74">
+        <v>6</v>
+      </c>
+      <c r="K74">
+        <v>198816</v>
+      </c>
+      <c r="L74">
+        <v>229680</v>
+      </c>
+      <c r="M74">
+        <v>201367</v>
+      </c>
+      <c r="N74">
+        <v>233483</v>
+      </c>
+      <c r="Q74">
+        <v>6</v>
+      </c>
+      <c r="R74">
+        <v>391795</v>
+      </c>
+      <c r="S74">
+        <v>454591</v>
+      </c>
+      <c r="T74">
+        <v>398929</v>
+      </c>
+      <c r="U74">
+        <v>463805</v>
+      </c>
+      <c r="X74">
+        <v>6</v>
+      </c>
+      <c r="Y74">
+        <v>584794</v>
+      </c>
+      <c r="Z74">
+        <v>678982</v>
+      </c>
+      <c r="AA74">
+        <v>596249</v>
+      </c>
+      <c r="AB74">
+        <v>694207</v>
+      </c>
+    </row>
+    <row r="75" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C75">
+        <v>7</v>
+      </c>
+      <c r="D75">
+        <v>45055</v>
+      </c>
+      <c r="E75">
+        <v>50838</v>
+      </c>
+      <c r="F75">
+        <v>44327</v>
+      </c>
+      <c r="G75">
+        <v>50424</v>
+      </c>
+      <c r="J75">
+        <v>7</v>
+      </c>
+      <c r="K75">
+        <v>198747</v>
+      </c>
+      <c r="L75">
+        <v>229628</v>
+      </c>
+      <c r="M75">
+        <v>201433</v>
+      </c>
+      <c r="N75">
+        <v>233422</v>
+      </c>
+      <c r="Q75">
+        <v>7</v>
+      </c>
+      <c r="R75">
+        <v>391966</v>
+      </c>
+      <c r="S75">
+        <v>454488</v>
+      </c>
+      <c r="T75">
+        <v>399062</v>
+      </c>
+      <c r="U75">
+        <v>464005</v>
+      </c>
+      <c r="X75">
+        <v>7</v>
+      </c>
+      <c r="Y75">
+        <v>584891</v>
+      </c>
+      <c r="Z75">
+        <v>679141</v>
+      </c>
+      <c r="AA75">
+        <v>596517</v>
+      </c>
+      <c r="AB75">
+        <v>694230</v>
+      </c>
+    </row>
+    <row r="76" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <v>8</v>
+      </c>
+      <c r="D76">
+        <v>45044</v>
+      </c>
+      <c r="E76">
+        <v>50855</v>
+      </c>
+      <c r="F76">
+        <v>44299</v>
+      </c>
+      <c r="G76">
+        <v>50411</v>
+      </c>
+      <c r="J76">
+        <v>8</v>
+      </c>
+      <c r="K76">
+        <v>198680</v>
+      </c>
+      <c r="L76">
+        <v>229651</v>
+      </c>
+      <c r="M76">
+        <v>201439</v>
+      </c>
+      <c r="N76">
+        <v>233458</v>
+      </c>
+      <c r="Q76">
+        <v>8</v>
+      </c>
+      <c r="R76">
+        <v>391949</v>
+      </c>
+      <c r="S76">
+        <v>454404</v>
+      </c>
+      <c r="T76">
+        <v>398892</v>
+      </c>
+      <c r="U76">
+        <v>463878</v>
+      </c>
+      <c r="X76">
+        <v>8</v>
+      </c>
+      <c r="Y76">
+        <v>584665</v>
+      </c>
+      <c r="Z76">
+        <v>679091</v>
+      </c>
+      <c r="AA76">
+        <v>596703</v>
+      </c>
+      <c r="AB76">
+        <v>694136</v>
+      </c>
+    </row>
+    <row r="77" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <v>9</v>
+      </c>
+      <c r="D77">
+        <v>45048</v>
+      </c>
+      <c r="E77">
+        <v>50867</v>
+      </c>
+      <c r="F77">
+        <v>44360</v>
+      </c>
+      <c r="G77">
+        <v>50432</v>
+      </c>
+      <c r="J77">
+        <v>9</v>
+      </c>
+      <c r="K77">
+        <v>198734</v>
+      </c>
+      <c r="L77">
+        <v>229678</v>
+      </c>
+      <c r="M77">
+        <v>201384</v>
+      </c>
+      <c r="N77">
+        <v>233460</v>
+      </c>
+      <c r="Q77">
+        <v>9</v>
+      </c>
+      <c r="R77">
+        <v>391825</v>
+      </c>
+      <c r="S77">
+        <v>454552</v>
+      </c>
+      <c r="T77">
+        <v>399022</v>
+      </c>
+      <c r="U77">
+        <v>463883</v>
+      </c>
+      <c r="X77">
+        <v>9</v>
+      </c>
+      <c r="Y77">
+        <v>585072</v>
+      </c>
+      <c r="Z77">
+        <v>679064</v>
+      </c>
+      <c r="AA77">
+        <v>596563</v>
+      </c>
+      <c r="AB77">
+        <v>694309</v>
+      </c>
+    </row>
+    <row r="78" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C78">
+        <v>10</v>
+      </c>
+      <c r="D78">
+        <v>45047</v>
+      </c>
+      <c r="E78">
+        <v>50849</v>
+      </c>
+      <c r="F78">
+        <v>44291</v>
+      </c>
+      <c r="G78">
+        <v>50392</v>
+      </c>
+      <c r="J78">
+        <v>10</v>
+      </c>
+      <c r="K78">
+        <v>198783</v>
+      </c>
+      <c r="L78">
+        <v>229570</v>
+      </c>
+      <c r="M78">
+        <v>201431</v>
+      </c>
+      <c r="N78">
+        <v>233453</v>
+      </c>
+      <c r="Q78">
+        <v>10</v>
+      </c>
+      <c r="R78">
+        <v>391922</v>
+      </c>
+      <c r="S78">
+        <v>454535</v>
+      </c>
+      <c r="T78">
+        <v>398846</v>
+      </c>
+      <c r="U78">
+        <v>463866</v>
+      </c>
+      <c r="X78">
+        <v>10</v>
+      </c>
+      <c r="Y78">
+        <v>584694</v>
+      </c>
+      <c r="Z78">
+        <v>679258</v>
+      </c>
+      <c r="AA78">
+        <v>596349</v>
+      </c>
+      <c r="AB78">
+        <v>693908</v>
+      </c>
+    </row>
+    <row r="80" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B80" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D80">
+        <f>AVERAGE(D69:D78)</f>
+        <v>45048.3</v>
+      </c>
+      <c r="E80">
+        <f>AVERAGE(E69:E78)</f>
+        <v>50854.6</v>
+      </c>
+      <c r="F80">
+        <f>AVERAGE(F69:F78)</f>
+        <v>44323.6</v>
+      </c>
+      <c r="G80">
+        <f>AVERAGE(G69:G78)</f>
+        <v>50417.8</v>
+      </c>
+      <c r="K80">
+        <f>AVERAGE(K69:K78)</f>
+        <v>198761.2</v>
+      </c>
+      <c r="L80">
+        <f>AVERAGE(L69:L78)</f>
+        <v>229633.2</v>
+      </c>
+      <c r="M80">
+        <f>AVERAGE(M69:M78)</f>
+        <v>201348.1</v>
+      </c>
+      <c r="N80">
+        <f>AVERAGE(N69:N78)</f>
+        <v>233476.8</v>
+      </c>
+      <c r="R80">
+        <f>AVERAGE(R69:R78)</f>
+        <v>391917.3</v>
+      </c>
+      <c r="S80">
+        <f>AVERAGE(S69:S78)</f>
+        <v>454450.9</v>
+      </c>
+      <c r="T80">
+        <f>AVERAGE(T69:T78)</f>
+        <v>398964.5</v>
+      </c>
+      <c r="U80">
+        <f>AVERAGE(U69:U78)</f>
+        <v>463875.9</v>
+      </c>
+      <c r="Y80">
+        <f>AVERAGE(Y69:Y78)</f>
+        <v>584896.19999999995</v>
+      </c>
+      <c r="Z80">
+        <f>AVERAGE(Z69:Z78)</f>
+        <v>679078.5</v>
+      </c>
+      <c r="AA80">
+        <f>AVERAGE(AA69:AA78)</f>
+        <v>596421.1</v>
+      </c>
+      <c r="AB80">
+        <f>AVERAGE(AB69:AB78)</f>
+        <v>694214.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed usage of pow function, changed calculation of changes, new benchmarks
</commit_message>
<xml_diff>
--- a/BenchmarkDocs/Results.xlsx
+++ b/BenchmarkDocs/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f0dc99f0b729840/Teilen/edge-ml/feature-extraction/BenchmarkDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1516" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21F89C13-3EF6-42B3-B6CD-D15BCAAA8470}"/>
+  <xr:revisionPtr revIDLastSave="1776" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F25C433-0DE6-472F-B835-79B341E02BF5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
+    <workbookView xWindow="8670" yWindow="150" windowWidth="19875" windowHeight="14280" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="180">
   <si>
     <t>Arduino</t>
   </si>
@@ -566,6 +566,15 @@
   </si>
   <si>
     <t>Neu:Iter fix, unused</t>
+  </si>
+  <si>
+    <t>Stand: 06.02.</t>
+  </si>
+  <si>
+    <t>Neu:Pow removed</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>
@@ -946,40 +955,40 @@
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" customWidth="1"/>
-    <col min="11" max="11" width="26.44140625" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" customWidth="1"/>
-    <col min="16" max="16" width="12.88671875" customWidth="1"/>
-    <col min="17" max="17" width="12.5546875" customWidth="1"/>
-    <col min="21" max="21" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
+    <col min="21" max="21" width="22.28515625" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="23" max="23" width="11.44140625" customWidth="1"/>
-    <col min="24" max="24" width="11.109375" customWidth="1"/>
-    <col min="25" max="25" width="16.44140625" customWidth="1"/>
-    <col min="26" max="26" width="11.33203125" customWidth="1"/>
-    <col min="29" max="29" width="16.109375" customWidth="1"/>
-    <col min="30" max="30" width="35.6640625" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" customWidth="1"/>
+    <col min="24" max="24" width="11.140625" customWidth="1"/>
+    <col min="25" max="25" width="16.42578125" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" customWidth="1"/>
+    <col min="29" max="29" width="16.140625" customWidth="1"/>
+    <col min="30" max="30" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>33</v>
       </c>
@@ -1011,7 +1020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -1058,7 +1067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
@@ -1102,7 +1111,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
@@ -1137,7 +1146,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>3</v>
       </c>
@@ -1172,7 +1181,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>4</v>
       </c>
@@ -1207,7 +1216,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>5</v>
       </c>
@@ -1242,7 +1251,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>6</v>
       </c>
@@ -1277,7 +1286,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>7</v>
       </c>
@@ -1312,7 +1321,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>8</v>
       </c>
@@ -1347,7 +1356,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>9</v>
       </c>
@@ -1382,7 +1391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>10</v>
       </c>
@@ -1417,12 +1426,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -1463,7 +1472,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>5</v>
       </c>
@@ -1537,7 +1546,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>1</v>
       </c>
@@ -1593,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>2</v>
       </c>
@@ -1649,7 +1658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>3</v>
       </c>
@@ -1705,7 +1714,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>4</v>
       </c>
@@ -1761,7 +1770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>5</v>
       </c>
@@ -1817,7 +1826,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>6</v>
       </c>
@@ -1873,7 +1882,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>7</v>
       </c>
@@ -1929,7 +1938,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>8</v>
       </c>
@@ -1985,7 +1994,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>9</v>
       </c>
@@ -2041,7 +2050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>10</v>
       </c>
@@ -2097,7 +2106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T29">
         <v>10</v>
       </c>
@@ -2117,7 +2126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T30">
         <v>8</v>
       </c>
@@ -2137,7 +2146,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T31">
         <v>8</v>
       </c>
@@ -2157,7 +2166,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T32">
         <v>10</v>
       </c>
@@ -2177,7 +2186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>114</v>
       </c>
@@ -2200,7 +2209,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>98</v>
       </c>
@@ -2244,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>97</v>
       </c>
@@ -2285,7 +2294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T36">
         <v>3</v>
       </c>
@@ -2305,7 +2314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T37">
         <v>20</v>
       </c>
@@ -2325,7 +2334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T38">
         <v>20</v>
       </c>
@@ -2345,7 +2354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>98</v>
       </c>
@@ -2377,7 +2386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>124</v>
       </c>
@@ -2409,7 +2418,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>127</v>
       </c>
@@ -2438,7 +2447,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>128</v>
       </c>
@@ -2452,7 +2461,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="43" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>136</v>
       </c>
@@ -2484,7 +2493,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>139</v>
       </c>
@@ -2516,7 +2525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>140</v>
       </c>
@@ -2551,7 +2560,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>141</v>
       </c>
@@ -2583,7 +2592,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>137</v>
       </c>
@@ -2597,7 +2606,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>148</v>
       </c>
@@ -2632,7 +2641,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>149</v>
       </c>
@@ -2664,7 +2673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>152</v>
       </c>
@@ -2699,7 +2708,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T51">
         <v>11</v>
       </c>
@@ -2719,7 +2728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T52">
         <v>16</v>
       </c>
@@ -2742,7 +2751,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T53">
         <v>11</v>
       </c>
@@ -2762,7 +2771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T54">
         <v>16</v>
       </c>
@@ -2782,7 +2791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T55">
         <v>16</v>
       </c>
@@ -2805,7 +2814,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T56">
         <v>8</v>
       </c>
@@ -2825,7 +2834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T57">
         <v>19</v>
       </c>
@@ -2845,7 +2854,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T58">
         <v>17</v>
       </c>
@@ -2865,7 +2874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T59">
         <v>17</v>
       </c>
@@ -2885,12 +2894,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:30" x14ac:dyDescent="0.25">
       <c r="AD60" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T61">
         <v>15</v>
       </c>
@@ -2910,7 +2919,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T63">
         <v>4</v>
       </c>
@@ -2918,7 +2927,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T64">
         <v>3</v>
       </c>
@@ -2926,7 +2935,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="20:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="20:21" x14ac:dyDescent="0.25">
       <c r="T65">
         <v>3</v>
       </c>
@@ -2934,7 +2943,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="20:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="20:21" x14ac:dyDescent="0.25">
       <c r="T66">
         <v>4</v>
       </c>
@@ -2950,36 +2959,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DC238C-8F4B-441F-9A1D-B395F114E22E}">
-  <dimension ref="A1:AS80"/>
+  <dimension ref="A1:AT96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="P73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA94" sqref="AA94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" customWidth="1"/>
-    <col min="16" max="16" width="13.109375" customWidth="1"/>
-    <col min="18" max="18" width="10.6640625" customWidth="1"/>
-    <col min="19" max="19" width="13.44140625" customWidth="1"/>
-    <col min="22" max="22" width="12.5546875" customWidth="1"/>
-    <col min="26" max="26" width="13.33203125" customWidth="1"/>
-    <col min="30" max="30" width="12.109375" customWidth="1"/>
-    <col min="31" max="31" width="9.5546875" customWidth="1"/>
-    <col min="32" max="32" width="23.5546875" customWidth="1"/>
-    <col min="45" max="45" width="38" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" customWidth="1"/>
+    <col min="31" max="31" width="9.5703125" customWidth="1"/>
+    <col min="32" max="32" width="23.5703125" customWidth="1"/>
+    <col min="45" max="45" width="11.7109375" customWidth="1"/>
+    <col min="46" max="46" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>154</v>
       </c>
@@ -2987,7 +2997,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -3015,14 +3025,14 @@
       <c r="AG3" t="s">
         <v>98</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AN3" t="s">
         <v>97</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AT3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
         <v>5</v>
       </c>
@@ -3074,26 +3084,26 @@
       <c r="AL4" t="s">
         <v>174</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AN4" t="s">
         <v>156</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AO4" t="s">
         <v>157</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AP4" t="s">
         <v>158</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AQ4" t="s">
         <v>173</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AR4" t="s">
         <v>159</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AS4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J5">
         <v>1</v>
       </c>
@@ -3142,23 +3152,29 @@
       <c r="AK5">
         <v>188</v>
       </c>
-      <c r="AM5">
+      <c r="AL5">
+        <v>159</v>
+      </c>
+      <c r="AN5">
         <v>1639</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>1654</v>
       </c>
-      <c r="AO5">
+      <c r="AP5">
         <v>1622</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>125</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>226</v>
       </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AS5">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J6">
         <v>2</v>
       </c>
@@ -3207,23 +3223,29 @@
       <c r="AK6">
         <v>352</v>
       </c>
-      <c r="AM6">
+      <c r="AL6">
+        <v>350</v>
+      </c>
+      <c r="AN6">
         <v>4630</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>4628</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>4663</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>391</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>458</v>
       </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AS6">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J7">
         <v>3</v>
       </c>
@@ -3272,23 +3294,29 @@
       <c r="AK7">
         <v>2250</v>
       </c>
-      <c r="AM7">
+      <c r="AL7">
+        <v>2196</v>
+      </c>
+      <c r="AN7">
         <v>52201</v>
       </c>
-      <c r="AN7">
+      <c r="AO7">
         <v>52873</v>
       </c>
-      <c r="AO7">
+      <c r="AP7">
         <v>52940</v>
       </c>
-      <c r="AP7">
+      <c r="AQ7">
         <v>2140</v>
       </c>
-      <c r="AQ7">
+      <c r="AR7">
         <v>2186</v>
       </c>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AS7">
+        <v>2192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J8">
         <v>4</v>
       </c>
@@ -3337,23 +3365,29 @@
       <c r="AK8">
         <v>2348</v>
       </c>
-      <c r="AM8">
+      <c r="AL8">
+        <v>2347</v>
+      </c>
+      <c r="AN8">
         <v>15579</v>
       </c>
-      <c r="AN8">
+      <c r="AO8">
         <v>15766</v>
       </c>
-      <c r="AO8">
+      <c r="AP8">
         <v>15857</v>
       </c>
-      <c r="AP8">
+      <c r="AQ8">
         <v>2351</v>
       </c>
-      <c r="AQ8">
+      <c r="AR8">
         <v>2331</v>
       </c>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AS8">
+        <v>2411</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J9">
         <v>5</v>
       </c>
@@ -3402,23 +3436,29 @@
       <c r="AK9">
         <v>3977</v>
       </c>
-      <c r="AM9">
+      <c r="AL9">
+        <v>4144</v>
+      </c>
+      <c r="AN9">
         <v>19193</v>
       </c>
-      <c r="AN9">
+      <c r="AO9">
         <v>19348</v>
       </c>
-      <c r="AO9">
+      <c r="AP9">
         <v>19443</v>
       </c>
-      <c r="AP9">
+      <c r="AQ9">
         <v>3977</v>
       </c>
-      <c r="AQ9">
+      <c r="AR9">
         <v>4011</v>
       </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AS9">
+        <v>4167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J10">
         <v>6</v>
       </c>
@@ -3467,23 +3507,29 @@
       <c r="AK10">
         <v>3882</v>
       </c>
-      <c r="AM10">
+      <c r="AL10">
+        <v>3898</v>
+      </c>
+      <c r="AN10">
         <v>18477</v>
       </c>
-      <c r="AN10">
+      <c r="AO10">
         <v>18687</v>
       </c>
-      <c r="AO10">
+      <c r="AP10">
         <v>18758</v>
       </c>
-      <c r="AP10">
+      <c r="AQ10">
         <v>3875</v>
       </c>
-      <c r="AQ10">
+      <c r="AR10">
         <v>3946</v>
       </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AS10">
+        <v>3972</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J11">
         <v>7</v>
       </c>
@@ -3532,23 +3578,29 @@
       <c r="AK11">
         <v>5408</v>
       </c>
-      <c r="AM11">
+      <c r="AL11">
+        <v>5411</v>
+      </c>
+      <c r="AN11">
         <v>33520</v>
       </c>
-      <c r="AN11">
+      <c r="AO11">
         <v>33835</v>
       </c>
-      <c r="AO11">
+      <c r="AP11">
         <v>34072</v>
       </c>
-      <c r="AP11">
+      <c r="AQ11">
         <v>5439</v>
       </c>
-      <c r="AQ11">
+      <c r="AR11">
         <v>5450</v>
       </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AS11">
+        <v>5484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J12">
         <v>8</v>
       </c>
@@ -3597,23 +3649,29 @@
       <c r="AK12">
         <v>11926</v>
       </c>
-      <c r="AM12">
+      <c r="AL12">
+        <v>316</v>
+      </c>
+      <c r="AN12">
         <v>5822</v>
       </c>
-      <c r="AN12">
+      <c r="AO12">
         <v>5845</v>
       </c>
-      <c r="AO12">
+      <c r="AP12">
         <v>5832</v>
       </c>
-      <c r="AP12">
+      <c r="AQ12">
         <v>12347</v>
       </c>
-      <c r="AQ12">
+      <c r="AR12">
         <v>12354</v>
       </c>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AS12">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J13">
         <v>9</v>
       </c>
@@ -3662,23 +3720,29 @@
       <c r="AK13">
         <v>322</v>
       </c>
-      <c r="AM13">
+      <c r="AL13">
+        <v>350</v>
+      </c>
+      <c r="AN13">
         <v>4641</v>
       </c>
-      <c r="AN13">
+      <c r="AO13">
         <v>4694</v>
       </c>
-      <c r="AO13">
+      <c r="AP13">
         <v>4662</v>
       </c>
-      <c r="AP13">
+      <c r="AQ13">
         <v>435</v>
       </c>
-      <c r="AQ13">
+      <c r="AR13">
         <v>414</v>
       </c>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AS13">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J14">
         <v>10</v>
       </c>
@@ -3727,23 +3791,29 @@
       <c r="AK14">
         <v>11916</v>
       </c>
-      <c r="AM14">
+      <c r="AL14">
+        <v>306</v>
+      </c>
+      <c r="AN14">
         <v>5741</v>
       </c>
-      <c r="AN14">
+      <c r="AO14">
         <v>5824</v>
       </c>
-      <c r="AO14">
+      <c r="AP14">
         <v>5746</v>
       </c>
-      <c r="AP14">
+      <c r="AQ14">
         <v>12335</v>
       </c>
-      <c r="AQ14">
+      <c r="AR14">
         <v>12314</v>
       </c>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AS14">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AF15" t="s">
         <v>45</v>
       </c>
@@ -3762,23 +3832,29 @@
       <c r="AK15">
         <v>11751</v>
       </c>
-      <c r="AM15">
+      <c r="AL15">
+        <v>190</v>
+      </c>
+      <c r="AN15">
         <v>2914</v>
       </c>
-      <c r="AN15">
+      <c r="AO15">
         <v>2778</v>
       </c>
-      <c r="AO15">
+      <c r="AP15">
         <v>2820</v>
       </c>
-      <c r="AP15">
+      <c r="AQ15">
         <v>12271</v>
       </c>
-      <c r="AQ15">
+      <c r="AR15">
         <v>12263</v>
       </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AS15">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>166</v>
       </c>
@@ -3832,23 +3908,29 @@
       <c r="AK16">
         <v>172628</v>
       </c>
-      <c r="AM16">
+      <c r="AL16">
+        <v>902</v>
+      </c>
+      <c r="AN16">
         <v>181033</v>
       </c>
-      <c r="AN16">
+      <c r="AO16">
         <v>181761</v>
       </c>
-      <c r="AO16">
+      <c r="AP16">
         <v>181849</v>
       </c>
-      <c r="AP16">
+      <c r="AQ16">
         <v>176635</v>
       </c>
-      <c r="AQ16">
+      <c r="AR16">
         <v>176607</v>
       </c>
-    </row>
-    <row r="17" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS16">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="17" spans="2:46" x14ac:dyDescent="0.25">
       <c r="AF17" t="s">
         <v>47</v>
       </c>
@@ -3867,23 +3949,29 @@
       <c r="AK17">
         <v>173321</v>
       </c>
-      <c r="AM17">
+      <c r="AL17">
+        <v>842</v>
+      </c>
+      <c r="AN17">
         <v>181693</v>
       </c>
-      <c r="AN17">
+      <c r="AO17">
         <v>182843</v>
       </c>
-      <c r="AO17">
+      <c r="AP17">
         <v>182862</v>
       </c>
-      <c r="AP17">
+      <c r="AQ17">
         <v>177095</v>
       </c>
-      <c r="AQ17">
+      <c r="AR17">
         <v>177034</v>
       </c>
-    </row>
-    <row r="18" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS17">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="18" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>160</v>
       </c>
@@ -3908,23 +3996,29 @@
       <c r="AK18">
         <v>1024</v>
       </c>
-      <c r="AM18">
+      <c r="AL18">
+        <v>1046</v>
+      </c>
+      <c r="AN18">
         <v>4074</v>
       </c>
-      <c r="AN18">
+      <c r="AO18">
         <v>4067</v>
       </c>
-      <c r="AO18">
+      <c r="AP18">
         <v>4069</v>
       </c>
-      <c r="AP18">
+      <c r="AQ18">
         <v>1030</v>
       </c>
-      <c r="AQ18">
+      <c r="AR18">
         <v>1036</v>
       </c>
-    </row>
-    <row r="19" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS18">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="19" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>33</v>
       </c>
@@ -3965,7 +4059,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>5</v>
       </c>
@@ -4044,23 +4138,29 @@
       <c r="AK20">
         <v>236</v>
       </c>
-      <c r="AM20">
+      <c r="AL20">
+        <v>205</v>
+      </c>
+      <c r="AN20">
         <v>1303</v>
       </c>
-      <c r="AN20">
+      <c r="AO20">
         <v>1335</v>
       </c>
-      <c r="AO20">
+      <c r="AP20">
         <v>1309</v>
       </c>
-      <c r="AP20">
+      <c r="AQ20">
         <v>171</v>
       </c>
-      <c r="AQ20">
+      <c r="AR20">
         <v>202</v>
       </c>
-    </row>
-    <row r="21" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS20">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="21" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>1</v>
       </c>
@@ -4139,23 +4239,29 @@
       <c r="AK21">
         <v>255</v>
       </c>
-      <c r="AM21">
+      <c r="AL21">
+        <v>253</v>
+      </c>
+      <c r="AN21">
         <v>1194</v>
       </c>
-      <c r="AN21">
+      <c r="AO21">
         <v>1254</v>
       </c>
-      <c r="AO21">
+      <c r="AP21">
         <v>1238</v>
       </c>
-      <c r="AP21">
+      <c r="AQ21">
         <v>216</v>
       </c>
-      <c r="AQ21">
+      <c r="AR21">
         <v>250</v>
       </c>
-    </row>
-    <row r="22" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS21">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>2</v>
       </c>
@@ -4234,23 +4340,29 @@
       <c r="AK22">
         <v>206</v>
       </c>
-      <c r="AM22">
+      <c r="AL22">
+        <v>204</v>
+      </c>
+      <c r="AN22">
         <v>1150</v>
       </c>
-      <c r="AN22">
+      <c r="AO22">
         <v>1165</v>
       </c>
-      <c r="AO22">
+      <c r="AP22">
         <v>1172</v>
       </c>
-      <c r="AP22">
+      <c r="AQ22">
         <v>258</v>
       </c>
-      <c r="AQ22">
+      <c r="AR22">
         <v>283</v>
       </c>
-    </row>
-    <row r="23" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS22">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="23" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>3</v>
       </c>
@@ -4329,23 +4441,29 @@
       <c r="AK23">
         <v>921</v>
       </c>
-      <c r="AM23">
+      <c r="AL23">
+        <v>874</v>
+      </c>
+      <c r="AN23">
         <v>2829</v>
       </c>
-      <c r="AN23">
+      <c r="AO23">
         <v>2846</v>
       </c>
-      <c r="AO23">
+      <c r="AP23">
         <v>2903</v>
       </c>
-      <c r="AP23">
+      <c r="AQ23">
         <v>802</v>
       </c>
-      <c r="AQ23">
+      <c r="AR23">
         <v>804</v>
       </c>
-    </row>
-    <row r="24" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS23">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="24" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>4</v>
       </c>
@@ -4424,23 +4542,29 @@
       <c r="AK24">
         <v>918</v>
       </c>
-      <c r="AM24">
+      <c r="AL24">
+        <v>872</v>
+      </c>
+      <c r="AN24">
         <v>2704</v>
       </c>
-      <c r="AN24">
+      <c r="AO24">
         <v>2730</v>
       </c>
-      <c r="AO24">
+      <c r="AP24">
         <v>2706</v>
       </c>
-      <c r="AP24">
+      <c r="AQ24">
         <v>802</v>
       </c>
-      <c r="AQ24">
+      <c r="AR24">
         <v>877</v>
       </c>
-    </row>
-    <row r="25" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS24">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="25" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>5</v>
       </c>
@@ -4519,23 +4643,29 @@
       <c r="AK25">
         <v>428</v>
       </c>
-      <c r="AM25">
+      <c r="AL25">
+        <v>395</v>
+      </c>
+      <c r="AN25">
         <v>1709</v>
-      </c>
-      <c r="AN25">
-        <v>1777</v>
       </c>
       <c r="AO25">
         <v>1777</v>
       </c>
       <c r="AP25">
+        <v>1777</v>
+      </c>
+      <c r="AQ25">
         <v>301</v>
       </c>
-      <c r="AQ25">
+      <c r="AR25">
         <v>362</v>
       </c>
-    </row>
-    <row r="26" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="26" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>6</v>
       </c>
@@ -4614,26 +4744,32 @@
       <c r="AK26">
         <v>360</v>
       </c>
-      <c r="AM26">
+      <c r="AL26">
+        <v>332</v>
+      </c>
+      <c r="AN26">
         <v>1204</v>
       </c>
-      <c r="AN26">
+      <c r="AO26">
         <v>1218</v>
       </c>
-      <c r="AO26">
+      <c r="AP26">
         <v>1252</v>
       </c>
-      <c r="AP26">
+      <c r="AQ26">
         <v>217</v>
       </c>
-      <c r="AQ26">
+      <c r="AR26">
         <v>877</v>
       </c>
-      <c r="AS26" t="s">
+      <c r="AS26">
+        <v>398</v>
+      </c>
+      <c r="AT26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>7</v>
       </c>
@@ -4712,23 +4848,29 @@
       <c r="AK27">
         <v>2626</v>
       </c>
-      <c r="AM27">
+      <c r="AL27">
+        <v>2628</v>
+      </c>
+      <c r="AN27">
         <v>16089</v>
       </c>
-      <c r="AN27">
+      <c r="AO27">
         <v>16233</v>
       </c>
-      <c r="AO27">
+      <c r="AP27">
         <v>16367</v>
       </c>
-      <c r="AP27">
+      <c r="AQ27">
         <v>2679</v>
       </c>
-      <c r="AQ27">
+      <c r="AR27">
         <v>2663</v>
       </c>
-    </row>
-    <row r="28" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS27">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="28" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>8</v>
       </c>
@@ -4790,7 +4932,7 @@
         <v>1039427</v>
       </c>
     </row>
-    <row r="29" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>9</v>
       </c>
@@ -4869,23 +5011,29 @@
       <c r="AK29">
         <v>1930</v>
       </c>
-      <c r="AM29">
+      <c r="AL29">
+        <v>1030</v>
+      </c>
+      <c r="AN29">
         <v>5007</v>
       </c>
-      <c r="AN29">
+      <c r="AO29">
         <v>4628</v>
       </c>
-      <c r="AO29">
+      <c r="AP29">
         <v>5058</v>
       </c>
-      <c r="AP29">
+      <c r="AQ29">
         <v>1885</v>
       </c>
-      <c r="AQ29">
+      <c r="AR29">
         <v>1921</v>
       </c>
-    </row>
-    <row r="30" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS29">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="30" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>10</v>
       </c>
@@ -4964,23 +5112,29 @@
       <c r="AK30">
         <v>1893</v>
       </c>
-      <c r="AM30">
+      <c r="AL30">
+        <v>968</v>
+      </c>
+      <c r="AN30">
         <v>5298</v>
       </c>
-      <c r="AN30">
+      <c r="AO30">
         <v>5283</v>
       </c>
-      <c r="AO30">
+      <c r="AP30">
         <v>5331</v>
       </c>
-      <c r="AP30">
+      <c r="AQ30">
         <v>1885</v>
       </c>
-      <c r="AQ30">
+      <c r="AR30">
         <v>1921</v>
       </c>
-    </row>
-    <row r="31" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS30">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="31" spans="2:46" x14ac:dyDescent="0.25">
       <c r="AF31" t="s">
         <v>56</v>
       </c>
@@ -4999,26 +5153,32 @@
       <c r="AK31">
         <v>1997</v>
       </c>
-      <c r="AM31">
+      <c r="AL31">
+        <v>1099</v>
+      </c>
+      <c r="AN31">
         <v>5098</v>
       </c>
-      <c r="AN31">
+      <c r="AO31">
         <v>5267</v>
       </c>
-      <c r="AO31">
+      <c r="AP31">
         <v>5308</v>
       </c>
-      <c r="AP31">
+      <c r="AQ31">
         <v>1966</v>
       </c>
-      <c r="AQ31">
+      <c r="AR31">
         <v>2044</v>
       </c>
-      <c r="AS31" t="s">
+      <c r="AS31">
+        <v>1101</v>
+      </c>
+      <c r="AT31" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>166</v>
       </c>
@@ -5104,23 +5264,29 @@
       <c r="AK32">
         <v>2896</v>
       </c>
-      <c r="AM32">
+      <c r="AL32">
+        <v>2875</v>
+      </c>
+      <c r="AN32">
         <v>17526</v>
       </c>
-      <c r="AN32">
+      <c r="AO32">
         <v>17953</v>
       </c>
-      <c r="AO32">
+      <c r="AP32">
         <v>18025</v>
       </c>
-      <c r="AP32">
+      <c r="AQ32">
         <v>2863</v>
       </c>
-      <c r="AQ32">
+      <c r="AR32">
         <v>2829</v>
       </c>
-    </row>
-    <row r="34" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS32">
+        <v>2863</v>
+      </c>
+    </row>
+    <row r="34" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>167</v>
       </c>
@@ -5142,26 +5308,32 @@
       <c r="AK34">
         <v>159</v>
       </c>
-      <c r="AM34">
+      <c r="AL34">
+        <v>158</v>
+      </c>
+      <c r="AN34">
         <v>1653</v>
       </c>
-      <c r="AN34">
+      <c r="AO34">
         <v>1822</v>
       </c>
-      <c r="AO34">
+      <c r="AP34">
         <v>1840</v>
       </c>
-      <c r="AP34">
+      <c r="AQ34">
         <v>156</v>
       </c>
-      <c r="AQ34">
+      <c r="AR34">
         <v>230</v>
       </c>
-      <c r="AS34" t="s">
+      <c r="AS34">
+        <v>187</v>
+      </c>
+      <c r="AT34" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>33</v>
       </c>
@@ -5219,23 +5391,29 @@
       <c r="AK35">
         <v>486</v>
       </c>
-      <c r="AM35">
+      <c r="AL35">
+        <v>488</v>
+      </c>
+      <c r="AN35">
         <v>2774</v>
       </c>
-      <c r="AN35">
+      <c r="AO35">
         <v>2817</v>
       </c>
-      <c r="AO35">
+      <c r="AP35">
         <v>2831</v>
       </c>
-      <c r="AP35">
+      <c r="AQ35">
         <v>424</v>
       </c>
-      <c r="AQ35">
+      <c r="AR35">
         <v>407</v>
       </c>
-    </row>
-    <row r="36" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS35">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="36" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>5</v>
       </c>
@@ -5314,26 +5492,32 @@
       <c r="AK36">
         <v>255</v>
       </c>
-      <c r="AM36">
+      <c r="AL36">
+        <v>280</v>
+      </c>
+      <c r="AN36">
         <v>2944</v>
       </c>
-      <c r="AN36">
+      <c r="AO36">
         <v>2896</v>
       </c>
-      <c r="AO36">
+      <c r="AP36">
         <v>2884</v>
       </c>
-      <c r="AP36">
+      <c r="AQ36">
         <v>316</v>
       </c>
-      <c r="AQ36">
+      <c r="AR36">
         <v>298</v>
       </c>
-      <c r="AS36" t="s">
+      <c r="AS36">
+        <v>327</v>
+      </c>
+      <c r="AT36" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>1</v>
       </c>
@@ -5412,23 +5596,29 @@
       <c r="AK37">
         <v>331</v>
       </c>
-      <c r="AM37">
+      <c r="AL37">
+        <v>238</v>
+      </c>
+      <c r="AN37">
         <v>2278</v>
       </c>
-      <c r="AN37">
+      <c r="AO37">
         <v>2361</v>
       </c>
-      <c r="AO37">
+      <c r="AP37">
         <v>2375</v>
       </c>
-      <c r="AP37">
+      <c r="AQ37">
         <v>225</v>
       </c>
-      <c r="AQ37">
+      <c r="AR37">
         <v>224</v>
       </c>
-    </row>
-    <row r="38" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS37">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="38" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>2</v>
       </c>
@@ -5507,26 +5697,32 @@
       <c r="AK38">
         <v>584</v>
       </c>
-      <c r="AM38">
+      <c r="AL38">
+        <v>562</v>
+      </c>
+      <c r="AN38">
         <v>3882</v>
       </c>
-      <c r="AN38">
+      <c r="AO38">
         <v>3965</v>
       </c>
-      <c r="AO38">
+      <c r="AP38">
         <v>3948</v>
       </c>
-      <c r="AP38">
+      <c r="AQ38">
         <v>395</v>
       </c>
-      <c r="AQ38">
+      <c r="AR38">
         <v>419</v>
       </c>
-      <c r="AS38" t="s">
+      <c r="AS38">
+        <v>437</v>
+      </c>
+      <c r="AT38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>3</v>
       </c>
@@ -5605,23 +5801,29 @@
       <c r="AK39">
         <v>233</v>
       </c>
-      <c r="AM39">
+      <c r="AL39">
+        <v>306</v>
+      </c>
+      <c r="AN39">
         <v>2098</v>
       </c>
-      <c r="AN39">
+      <c r="AO39">
         <v>2154</v>
       </c>
-      <c r="AO39">
+      <c r="AP39">
         <v>2156</v>
       </c>
-      <c r="AP39">
+      <c r="AQ39">
         <v>330</v>
       </c>
-      <c r="AQ39">
+      <c r="AR39">
         <v>356</v>
       </c>
-    </row>
-    <row r="40" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS39">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="40" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>4</v>
       </c>
@@ -5700,23 +5902,29 @@
       <c r="AK40">
         <v>455</v>
       </c>
-      <c r="AM40">
+      <c r="AL40">
+        <v>483</v>
+      </c>
+      <c r="AN40">
         <v>3696</v>
-      </c>
-      <c r="AN40">
-        <v>3772</v>
       </c>
       <c r="AO40">
         <v>3772</v>
       </c>
       <c r="AP40">
+        <v>3772</v>
+      </c>
+      <c r="AQ40">
         <v>428</v>
       </c>
-      <c r="AQ40">
+      <c r="AR40">
         <v>517</v>
       </c>
-    </row>
-    <row r="41" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS40">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="41" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>5</v>
       </c>
@@ -5795,26 +6003,32 @@
       <c r="AK41">
         <v>11865</v>
       </c>
-      <c r="AM41">
+      <c r="AL41">
+        <v>309</v>
+      </c>
+      <c r="AN41">
         <v>2930</v>
       </c>
-      <c r="AN41">
+      <c r="AO41">
         <v>2878</v>
       </c>
-      <c r="AO41">
+      <c r="AP41">
         <v>2886</v>
       </c>
-      <c r="AP41">
+      <c r="AQ41">
         <v>12316</v>
       </c>
-      <c r="AQ41">
+      <c r="AR41">
         <v>12344</v>
       </c>
-      <c r="AS41" t="s">
+      <c r="AS41">
+        <v>260</v>
+      </c>
+      <c r="AT41" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>6</v>
       </c>
@@ -5893,23 +6107,29 @@
       <c r="AK42">
         <v>2379</v>
       </c>
-      <c r="AM42">
+      <c r="AL42">
+        <v>2331</v>
+      </c>
+      <c r="AN42">
         <v>15644</v>
       </c>
-      <c r="AN42">
+      <c r="AO42">
         <v>15788</v>
       </c>
-      <c r="AO42">
+      <c r="AP42">
         <v>15903</v>
       </c>
-      <c r="AP42">
+      <c r="AQ42">
         <v>2402</v>
       </c>
-      <c r="AQ42">
+      <c r="AR42">
         <v>2370</v>
       </c>
-    </row>
-    <row r="43" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS42">
+        <v>2439</v>
+      </c>
+    </row>
+    <row r="43" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>7</v>
       </c>
@@ -5988,23 +6208,29 @@
       <c r="AK43">
         <v>4775</v>
       </c>
-      <c r="AM43">
+      <c r="AL43">
+        <v>4732</v>
+      </c>
+      <c r="AN43">
         <v>31208</v>
       </c>
-      <c r="AN43">
+      <c r="AO43">
         <v>31852</v>
       </c>
-      <c r="AO43">
+      <c r="AP43">
         <v>31685</v>
       </c>
-      <c r="AP43">
+      <c r="AQ43">
         <v>4742</v>
       </c>
-      <c r="AQ43">
+      <c r="AR43">
         <v>4733</v>
       </c>
-    </row>
-    <row r="44" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS43">
+        <v>4832</v>
+      </c>
+    </row>
+    <row r="44" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>8</v>
       </c>
@@ -6083,23 +6309,29 @@
       <c r="AK44">
         <v>1309</v>
       </c>
-      <c r="AM44">
-        <v>3562</v>
+      <c r="AL44">
+        <v>1306</v>
       </c>
       <c r="AN44">
         <v>3562</v>
       </c>
       <c r="AO44">
+        <v>3562</v>
+      </c>
+      <c r="AP44">
         <v>3587</v>
       </c>
-      <c r="AP44">
+      <c r="AQ44">
         <v>1235</v>
       </c>
-      <c r="AQ44">
+      <c r="AR44">
         <v>1280</v>
       </c>
-    </row>
-    <row r="45" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS44">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="45" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>9</v>
       </c>
@@ -6178,23 +6410,29 @@
       <c r="AK45">
         <v>1316</v>
       </c>
-      <c r="AM45">
+      <c r="AL45">
+        <v>1300</v>
+      </c>
+      <c r="AN45">
         <v>3449</v>
       </c>
-      <c r="AN45">
+      <c r="AO45">
         <v>3545</v>
       </c>
-      <c r="AO45">
+      <c r="AP45">
         <v>3526</v>
       </c>
-      <c r="AP45">
+      <c r="AQ45">
         <v>1228</v>
       </c>
-      <c r="AQ45">
+      <c r="AR45">
         <v>1274</v>
       </c>
-    </row>
-    <row r="46" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS45">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="46" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>10</v>
       </c>
@@ -6273,26 +6511,32 @@
       <c r="AK46">
         <v>13120</v>
       </c>
-      <c r="AM46">
+      <c r="AL46">
+        <v>1497</v>
+      </c>
+      <c r="AN46">
         <v>12547</v>
       </c>
-      <c r="AN46">
+      <c r="AO46">
         <v>12551</v>
       </c>
-      <c r="AO46">
+      <c r="AP46">
         <v>12536</v>
       </c>
-      <c r="AP46">
+      <c r="AQ46">
         <v>13586</v>
       </c>
-      <c r="AQ46">
+      <c r="AR46">
         <v>13498</v>
       </c>
-      <c r="AS46" t="s">
+      <c r="AS46">
+        <v>1545</v>
+      </c>
+      <c r="AT46" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>166</v>
       </c>
@@ -6383,28 +6627,36 @@
         <f>SUM(AK5:AK46)</f>
         <v>453226</v>
       </c>
-      <c r="AM48">
-        <f>SUM(AM5:AM46)</f>
-        <v>680933</v>
+      <c r="AL48">
+        <f>SUM(AL5:AL46)</f>
+        <v>48182</v>
       </c>
       <c r="AN48">
         <f>SUM(AN5:AN46)</f>
-        <v>686255</v>
+        <v>680933</v>
       </c>
       <c r="AO48">
         <f>SUM(AO5:AO46)</f>
-        <v>687570</v>
+        <v>686255</v>
       </c>
       <c r="AP48">
         <f>SUM(AP5:AP46)</f>
-        <v>462274</v>
+        <v>687570</v>
       </c>
       <c r="AQ48">
         <f>SUM(AQ5:AQ46)</f>
+        <v>462274</v>
+      </c>
+      <c r="AR48">
+        <f>SUM(AR5:AR46)</f>
         <v>463613</v>
       </c>
-    </row>
-    <row r="50" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS48">
+        <f>SUM(AS5:AS46)</f>
+        <v>49627</v>
+      </c>
+    </row>
+    <row r="50" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>172</v>
       </c>
@@ -6412,7 +6664,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>33</v>
       </c>
@@ -6470,26 +6722,32 @@
       <c r="AK51">
         <v>16899798</v>
       </c>
-      <c r="AM51">
+      <c r="AL51">
+        <v>15542206</v>
+      </c>
+      <c r="AN51">
         <v>17405915</v>
       </c>
-      <c r="AN51">
+      <c r="AO51">
         <v>17508299</v>
       </c>
-      <c r="AO51">
+      <c r="AP51">
         <v>17507506</v>
       </c>
-      <c r="AP51">
+      <c r="AQ51">
         <v>17271362</v>
       </c>
-      <c r="AQ51">
+      <c r="AR51">
         <v>17272073</v>
       </c>
-      <c r="AS51" t="s">
+      <c r="AS51">
+        <v>15862952</v>
+      </c>
+      <c r="AT51" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="52" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>5</v>
       </c>
@@ -6568,23 +6826,29 @@
       <c r="AK52">
         <v>19532</v>
       </c>
-      <c r="AM52">
+      <c r="AL52">
+        <v>19521</v>
+      </c>
+      <c r="AN52">
         <v>105728</v>
       </c>
-      <c r="AN52">
+      <c r="AO52">
         <v>107789</v>
       </c>
-      <c r="AO52">
+      <c r="AP52">
         <v>107732</v>
       </c>
-      <c r="AP52">
+      <c r="AQ52">
         <v>19843</v>
       </c>
-      <c r="AQ52">
+      <c r="AR52">
         <v>19809</v>
       </c>
-    </row>
-    <row r="53" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AS52">
+        <v>19921</v>
+      </c>
+    </row>
+    <row r="53" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>1</v>
       </c>
@@ -6663,26 +6927,32 @@
       <c r="AK53">
         <v>507645</v>
       </c>
-      <c r="AM53">
+      <c r="AL53">
+        <v>506970</v>
+      </c>
+      <c r="AN53">
         <v>6454577</v>
       </c>
-      <c r="AN53">
+      <c r="AO53">
         <v>6531258</v>
       </c>
-      <c r="AO53">
+      <c r="AP53">
         <v>6527939</v>
       </c>
-      <c r="AP53">
+      <c r="AQ53">
         <v>512692</v>
       </c>
-      <c r="AQ53">
+      <c r="AR53">
         <v>512678</v>
       </c>
-      <c r="AS53" t="s">
+      <c r="AS53">
+        <v>511651</v>
+      </c>
+      <c r="AT53" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="54" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>2</v>
       </c>
@@ -6761,26 +7031,32 @@
       <c r="AK54">
         <v>636969</v>
       </c>
-      <c r="AM54">
+      <c r="AL54">
+        <v>636142</v>
+      </c>
+      <c r="AN54">
         <v>9137022</v>
       </c>
-      <c r="AN54">
+      <c r="AO54">
         <v>9176671</v>
       </c>
-      <c r="AO54">
+      <c r="AP54">
         <v>9176962</v>
       </c>
-      <c r="AP54">
+      <c r="AQ54">
         <v>644165</v>
       </c>
-      <c r="AQ54">
+      <c r="AR54">
         <v>643664</v>
       </c>
-      <c r="AS54" t="s">
+      <c r="AS54">
+        <v>642830</v>
+      </c>
+      <c r="AT54" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C55">
         <v>3</v>
       </c>
@@ -6842,7 +7118,7 @@
         <v>694115</v>
       </c>
     </row>
-    <row r="56" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>4</v>
       </c>
@@ -6904,7 +7180,7 @@
         <v>693883</v>
       </c>
     </row>
-    <row r="57" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>5</v>
       </c>
@@ -6966,7 +7242,7 @@
         <v>693997</v>
       </c>
     </row>
-    <row r="58" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>6</v>
       </c>
@@ -7028,7 +7304,7 @@
         <v>693998</v>
       </c>
     </row>
-    <row r="59" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>7</v>
       </c>
@@ -7090,7 +7366,7 @@
         <v>693914</v>
       </c>
     </row>
-    <row r="60" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>8</v>
       </c>
@@ -7152,7 +7428,7 @@
         <v>694056</v>
       </c>
     </row>
-    <row r="61" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>9</v>
       </c>
@@ -7214,7 +7490,7 @@
         <v>694005</v>
       </c>
     </row>
-    <row r="62" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C62">
         <v>10</v>
       </c>
@@ -7276,7 +7552,7 @@
         <v>694157</v>
       </c>
     </row>
-    <row r="64" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>166</v>
       </c>
@@ -7345,7 +7621,7 @@
         <v>694047.7</v>
       </c>
     </row>
-    <row r="66" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>175</v>
       </c>
@@ -7353,7 +7629,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>33</v>
       </c>
@@ -7394,7 +7670,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>5</v>
       </c>
@@ -7456,7 +7732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>1</v>
       </c>
@@ -7518,7 +7794,7 @@
         <v>693930</v>
       </c>
     </row>
-    <row r="70" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C70">
         <v>2</v>
       </c>
@@ -7580,7 +7856,7 @@
         <v>694477</v>
       </c>
     </row>
-    <row r="71" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>3</v>
       </c>
@@ -7642,7 +7918,7 @@
         <v>694283</v>
       </c>
     </row>
-    <row r="72" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>4</v>
       </c>
@@ -7704,7 +7980,7 @@
         <v>694253</v>
       </c>
     </row>
-    <row r="73" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>5</v>
       </c>
@@ -7766,7 +8042,7 @@
         <v>694410</v>
       </c>
     </row>
-    <row r="74" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C74">
         <v>6</v>
       </c>
@@ -7828,7 +8104,7 @@
         <v>694207</v>
       </c>
     </row>
-    <row r="75" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C75">
         <v>7</v>
       </c>
@@ -7890,7 +8166,7 @@
         <v>694230</v>
       </c>
     </row>
-    <row r="76" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C76">
         <v>8</v>
       </c>
@@ -7952,7 +8228,7 @@
         <v>694136</v>
       </c>
     </row>
-    <row r="77" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C77">
         <v>9</v>
       </c>
@@ -8014,7 +8290,7 @@
         <v>694309</v>
       </c>
     </row>
-    <row r="78" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C78">
         <v>10</v>
       </c>
@@ -8076,7 +8352,7 @@
         <v>693908</v>
       </c>
     </row>
-    <row r="80" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>166</v>
       </c>
@@ -8143,6 +8419,806 @@
       <c r="AB80">
         <f>AVERAGE(AB69:AB78)</f>
         <v>694214.3</v>
+      </c>
+    </row>
+    <row r="82" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>177</v>
+      </c>
+      <c r="C82" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="83" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>33</v>
+      </c>
+      <c r="C83" t="s">
+        <v>164</v>
+      </c>
+      <c r="D83" t="s">
+        <v>96</v>
+      </c>
+      <c r="F83" t="s">
+        <v>97</v>
+      </c>
+      <c r="J83" t="s">
+        <v>26</v>
+      </c>
+      <c r="K83" t="s">
+        <v>96</v>
+      </c>
+      <c r="M83" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>1</v>
+      </c>
+      <c r="R83" t="s">
+        <v>96</v>
+      </c>
+      <c r="T83" t="s">
+        <v>97</v>
+      </c>
+      <c r="X83" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y83" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA83" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="84" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>3</v>
+      </c>
+      <c r="E84" t="s">
+        <v>4</v>
+      </c>
+      <c r="F84" t="s">
+        <v>3</v>
+      </c>
+      <c r="G84" t="s">
+        <v>4</v>
+      </c>
+      <c r="J84" t="s">
+        <v>5</v>
+      </c>
+      <c r="K84" t="s">
+        <v>3</v>
+      </c>
+      <c r="L84" t="s">
+        <v>4</v>
+      </c>
+      <c r="M84" t="s">
+        <v>3</v>
+      </c>
+      <c r="N84" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>5</v>
+      </c>
+      <c r="R84" t="s">
+        <v>3</v>
+      </c>
+      <c r="S84" t="s">
+        <v>4</v>
+      </c>
+      <c r="T84" t="s">
+        <v>3</v>
+      </c>
+      <c r="U84" t="s">
+        <v>4</v>
+      </c>
+      <c r="X84" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y84" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z84" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA84" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>10270</v>
+      </c>
+      <c r="E85">
+        <v>10246</v>
+      </c>
+      <c r="F85">
+        <v>8858</v>
+      </c>
+      <c r="G85">
+        <v>8925</v>
+      </c>
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="K85">
+        <v>25074</v>
+      </c>
+      <c r="L85">
+        <v>27000</v>
+      </c>
+      <c r="M85">
+        <v>24048</v>
+      </c>
+      <c r="N85">
+        <v>26179</v>
+      </c>
+      <c r="Q85">
+        <v>1</v>
+      </c>
+      <c r="R85">
+        <v>45101</v>
+      </c>
+      <c r="S85">
+        <v>49494</v>
+      </c>
+      <c r="T85">
+        <v>44673</v>
+      </c>
+      <c r="U85">
+        <v>49332</v>
+      </c>
+      <c r="X85">
+        <v>1</v>
+      </c>
+      <c r="Y85">
+        <v>65127</v>
+      </c>
+      <c r="Z85">
+        <v>72019</v>
+      </c>
+      <c r="AA85">
+        <v>65286</v>
+      </c>
+      <c r="AB85">
+        <v>72558</v>
+      </c>
+    </row>
+    <row r="86" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86">
+        <v>10266</v>
+      </c>
+      <c r="E86">
+        <v>10272</v>
+      </c>
+      <c r="F86">
+        <v>8854</v>
+      </c>
+      <c r="G86">
+        <v>8922</v>
+      </c>
+      <c r="J86">
+        <v>2</v>
+      </c>
+      <c r="K86">
+        <v>25084</v>
+      </c>
+      <c r="L86">
+        <v>26992</v>
+      </c>
+      <c r="M86">
+        <v>24102</v>
+      </c>
+      <c r="N86">
+        <v>26130</v>
+      </c>
+      <c r="Q86">
+        <v>2</v>
+      </c>
+      <c r="R86">
+        <v>45153</v>
+      </c>
+      <c r="S86">
+        <v>49479</v>
+      </c>
+      <c r="T86">
+        <v>44424</v>
+      </c>
+      <c r="U86">
+        <v>49457</v>
+      </c>
+      <c r="X86">
+        <v>2</v>
+      </c>
+      <c r="Y86">
+        <v>65145</v>
+      </c>
+      <c r="Z86">
+        <v>72359</v>
+      </c>
+      <c r="AA86">
+        <v>65152</v>
+      </c>
+      <c r="AB86">
+        <v>72659</v>
+      </c>
+    </row>
+    <row r="87" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87">
+        <v>10271</v>
+      </c>
+      <c r="E87">
+        <v>10245</v>
+      </c>
+      <c r="F87">
+        <v>8858</v>
+      </c>
+      <c r="G87">
+        <v>8914</v>
+      </c>
+      <c r="J87">
+        <v>3</v>
+      </c>
+      <c r="K87">
+        <v>25066</v>
+      </c>
+      <c r="L87">
+        <v>26989</v>
+      </c>
+      <c r="M87">
+        <v>24086</v>
+      </c>
+      <c r="N87">
+        <v>26129</v>
+      </c>
+      <c r="Q87">
+        <v>3</v>
+      </c>
+      <c r="R87">
+        <v>45033</v>
+      </c>
+      <c r="S87">
+        <v>49622</v>
+      </c>
+      <c r="T87">
+        <v>44506</v>
+      </c>
+      <c r="U87">
+        <v>49440</v>
+      </c>
+      <c r="X87">
+        <v>3</v>
+      </c>
+      <c r="Y87">
+        <v>65077</v>
+      </c>
+      <c r="Z87">
+        <v>72266</v>
+      </c>
+      <c r="AA87">
+        <v>65047</v>
+      </c>
+      <c r="AB87">
+        <v>72682</v>
+      </c>
+    </row>
+    <row r="88" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>4</v>
+      </c>
+      <c r="D88">
+        <v>10293</v>
+      </c>
+      <c r="E88">
+        <v>10245</v>
+      </c>
+      <c r="F88">
+        <v>8825</v>
+      </c>
+      <c r="G88">
+        <v>8921</v>
+      </c>
+      <c r="J88">
+        <v>4</v>
+      </c>
+      <c r="K88">
+        <v>25082</v>
+      </c>
+      <c r="L88">
+        <v>26942</v>
+      </c>
+      <c r="M88">
+        <v>24037</v>
+      </c>
+      <c r="N88">
+        <v>26117</v>
+      </c>
+      <c r="Q88">
+        <v>4</v>
+      </c>
+      <c r="R88">
+        <v>45061</v>
+      </c>
+      <c r="S88">
+        <v>49577</v>
+      </c>
+      <c r="T88">
+        <v>44490</v>
+      </c>
+      <c r="U88">
+        <v>49248</v>
+      </c>
+      <c r="X88">
+        <v>4</v>
+      </c>
+      <c r="Y88">
+        <v>65034</v>
+      </c>
+      <c r="Z88">
+        <v>72294</v>
+      </c>
+      <c r="AA88">
+        <v>65223</v>
+      </c>
+      <c r="AB88">
+        <v>72665</v>
+      </c>
+    </row>
+    <row r="89" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <v>5</v>
+      </c>
+      <c r="D89">
+        <v>10295</v>
+      </c>
+      <c r="E89">
+        <v>10244</v>
+      </c>
+      <c r="F89">
+        <v>8852</v>
+      </c>
+      <c r="G89">
+        <v>8925</v>
+      </c>
+      <c r="J89">
+        <v>5</v>
+      </c>
+      <c r="K89">
+        <v>25094</v>
+      </c>
+      <c r="L89">
+        <v>27001</v>
+      </c>
+      <c r="M89">
+        <v>24064</v>
+      </c>
+      <c r="N89">
+        <v>26113</v>
+      </c>
+      <c r="Q89">
+        <v>5</v>
+      </c>
+      <c r="R89">
+        <v>45031</v>
+      </c>
+      <c r="S89">
+        <v>49511</v>
+      </c>
+      <c r="T89">
+        <v>44350</v>
+      </c>
+      <c r="U89">
+        <v>49365</v>
+      </c>
+      <c r="X89">
+        <v>5</v>
+      </c>
+      <c r="Y89">
+        <v>65019</v>
+      </c>
+      <c r="Z89">
+        <v>72268</v>
+      </c>
+      <c r="AA89">
+        <v>65028</v>
+      </c>
+      <c r="AB89">
+        <v>72475</v>
+      </c>
+    </row>
+    <row r="90" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>6</v>
+      </c>
+      <c r="D90">
+        <v>10297</v>
+      </c>
+      <c r="E90">
+        <v>10245</v>
+      </c>
+      <c r="F90">
+        <v>8855</v>
+      </c>
+      <c r="G90">
+        <v>8921</v>
+      </c>
+      <c r="J90">
+        <v>6</v>
+      </c>
+      <c r="K90">
+        <v>25101</v>
+      </c>
+      <c r="L90">
+        <v>26970</v>
+      </c>
+      <c r="M90">
+        <v>24076</v>
+      </c>
+      <c r="N90">
+        <v>26152</v>
+      </c>
+      <c r="Q90">
+        <v>6</v>
+      </c>
+      <c r="R90">
+        <v>45071</v>
+      </c>
+      <c r="S90">
+        <v>49506</v>
+      </c>
+      <c r="T90">
+        <v>44544</v>
+      </c>
+      <c r="U90">
+        <v>49311</v>
+      </c>
+      <c r="X90">
+        <v>6</v>
+      </c>
+      <c r="Y90">
+        <v>65035</v>
+      </c>
+      <c r="Z90">
+        <v>72390</v>
+      </c>
+      <c r="AA90">
+        <v>65110</v>
+      </c>
+      <c r="AB90">
+        <v>72971</v>
+      </c>
+    </row>
+    <row r="91" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>7</v>
+      </c>
+      <c r="D91">
+        <v>10267</v>
+      </c>
+      <c r="E91">
+        <v>10245</v>
+      </c>
+      <c r="F91">
+        <v>8852</v>
+      </c>
+      <c r="G91">
+        <v>8914</v>
+      </c>
+      <c r="J91">
+        <v>7</v>
+      </c>
+      <c r="K91">
+        <v>25062</v>
+      </c>
+      <c r="L91">
+        <v>26936</v>
+      </c>
+      <c r="M91">
+        <v>24049</v>
+      </c>
+      <c r="N91">
+        <v>26142</v>
+      </c>
+      <c r="Q91">
+        <v>7</v>
+      </c>
+      <c r="R91">
+        <v>44873</v>
+      </c>
+      <c r="S91">
+        <v>49485</v>
+      </c>
+      <c r="T91">
+        <v>44602</v>
+      </c>
+      <c r="U91">
+        <v>49370</v>
+      </c>
+      <c r="X91">
+        <v>7</v>
+      </c>
+      <c r="Y91">
+        <v>65090</v>
+      </c>
+      <c r="Z91">
+        <v>72216</v>
+      </c>
+      <c r="AA91">
+        <v>64990</v>
+      </c>
+      <c r="AB91">
+        <v>72782</v>
+      </c>
+    </row>
+    <row r="92" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>8</v>
+      </c>
+      <c r="D92">
+        <v>10272</v>
+      </c>
+      <c r="E92">
+        <v>10245</v>
+      </c>
+      <c r="F92">
+        <v>8854</v>
+      </c>
+      <c r="G92">
+        <v>8919</v>
+      </c>
+      <c r="J92">
+        <v>8</v>
+      </c>
+      <c r="K92">
+        <v>25069</v>
+      </c>
+      <c r="L92">
+        <v>26971</v>
+      </c>
+      <c r="M92">
+        <v>24127</v>
+      </c>
+      <c r="N92">
+        <v>26100</v>
+      </c>
+      <c r="Q92">
+        <v>8</v>
+      </c>
+      <c r="R92">
+        <v>45130</v>
+      </c>
+      <c r="S92">
+        <v>49536</v>
+      </c>
+      <c r="T92">
+        <v>44743</v>
+      </c>
+      <c r="U92">
+        <v>49254</v>
+      </c>
+      <c r="X92">
+        <v>8</v>
+      </c>
+      <c r="Y92">
+        <v>65107</v>
+      </c>
+      <c r="Z92">
+        <v>72341</v>
+      </c>
+      <c r="AA92">
+        <v>65048</v>
+      </c>
+      <c r="AB92">
+        <v>72820</v>
+      </c>
+    </row>
+    <row r="93" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>9</v>
+      </c>
+      <c r="D93">
+        <v>10272</v>
+      </c>
+      <c r="E93">
+        <v>10249</v>
+      </c>
+      <c r="F93">
+        <v>8828</v>
+      </c>
+      <c r="G93">
+        <v>8923</v>
+      </c>
+      <c r="J93">
+        <v>9</v>
+      </c>
+      <c r="K93">
+        <v>25077</v>
+      </c>
+      <c r="L93">
+        <v>26956</v>
+      </c>
+      <c r="M93">
+        <v>24046</v>
+      </c>
+      <c r="N93">
+        <v>26180</v>
+      </c>
+      <c r="Q93">
+        <v>9</v>
+      </c>
+      <c r="R93">
+        <v>45080</v>
+      </c>
+      <c r="S93">
+        <v>49417</v>
+      </c>
+      <c r="T93">
+        <v>44701</v>
+      </c>
+      <c r="U93">
+        <v>49399</v>
+      </c>
+      <c r="X93">
+        <v>9</v>
+      </c>
+      <c r="Y93">
+        <v>65062</v>
+      </c>
+      <c r="Z93">
+        <v>72344</v>
+      </c>
+      <c r="AA93">
+        <v>65146</v>
+      </c>
+      <c r="AB93">
+        <v>72988</v>
+      </c>
+    </row>
+    <row r="94" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>10</v>
+      </c>
+      <c r="D94">
+        <v>10270</v>
+      </c>
+      <c r="E94">
+        <v>10241</v>
+      </c>
+      <c r="F94">
+        <v>8855</v>
+      </c>
+      <c r="G94">
+        <v>8891</v>
+      </c>
+      <c r="J94">
+        <v>10</v>
+      </c>
+      <c r="K94">
+        <v>25078</v>
+      </c>
+      <c r="L94">
+        <v>26978</v>
+      </c>
+      <c r="M94" t="s">
+        <v>179</v>
+      </c>
+      <c r="N94">
+        <v>26217</v>
+      </c>
+      <c r="Q94">
+        <v>10</v>
+      </c>
+      <c r="R94">
+        <v>45017</v>
+      </c>
+      <c r="S94">
+        <v>49512</v>
+      </c>
+      <c r="T94">
+        <v>44680</v>
+      </c>
+      <c r="U94">
+        <v>49440</v>
+      </c>
+      <c r="X94">
+        <v>10</v>
+      </c>
+      <c r="Y94">
+        <v>65151</v>
+      </c>
+      <c r="Z94">
+        <v>72347</v>
+      </c>
+      <c r="AA94">
+        <v>65383</v>
+      </c>
+      <c r="AB94">
+        <v>72675</v>
+      </c>
+    </row>
+    <row r="96" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B96" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D96">
+        <f>AVERAGE(D85:D94)</f>
+        <v>10277.299999999999</v>
+      </c>
+      <c r="E96">
+        <f>AVERAGE(E85:E94)</f>
+        <v>10247.700000000001</v>
+      </c>
+      <c r="F96">
+        <f>AVERAGE(F85:F94)</f>
+        <v>8849.1</v>
+      </c>
+      <c r="G96">
+        <f>AVERAGE(G85:G94)</f>
+        <v>8917.5</v>
+      </c>
+      <c r="K96">
+        <f>AVERAGE(K85:K94)</f>
+        <v>25078.7</v>
+      </c>
+      <c r="L96">
+        <f>AVERAGE(L85:L94)</f>
+        <v>26973.5</v>
+      </c>
+      <c r="M96">
+        <f>AVERAGE(M85:M94)</f>
+        <v>24070.555555555555</v>
+      </c>
+      <c r="N96">
+        <f>AVERAGE(N85:N94)</f>
+        <v>26145.9</v>
+      </c>
+      <c r="R96">
+        <f>AVERAGE(R85:R94)</f>
+        <v>45055</v>
+      </c>
+      <c r="S96">
+        <f>AVERAGE(S85:S94)</f>
+        <v>49513.9</v>
+      </c>
+      <c r="T96">
+        <f>AVERAGE(T85:T94)</f>
+        <v>44571.3</v>
+      </c>
+      <c r="U96">
+        <f>AVERAGE(U85:U94)</f>
+        <v>49361.599999999999</v>
+      </c>
+      <c r="Y96">
+        <f>AVERAGE(Y85:Y94)</f>
+        <v>65084.7</v>
+      </c>
+      <c r="Z96">
+        <f>AVERAGE(Z85:Z94)</f>
+        <v>72284.399999999994</v>
+      </c>
+      <c r="AA96">
+        <f>AVERAGE(AA85:AA94)</f>
+        <v>65141.3</v>
+      </c>
+      <c r="AB96">
+        <f>AVERAGE(AB85:AB94)</f>
+        <v>72727.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created python runtime prediction script
</commit_message>
<xml_diff>
--- a/BenchmarkDocs/Results.xlsx
+++ b/BenchmarkDocs/Results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f0dc99f0b729840/Teilen/edge-ml/feature-extraction/BenchmarkDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1776" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F25C433-0DE6-472F-B835-79B341E02BF5}"/>
+  <xr:revisionPtr revIDLastSave="1955" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA0C6665-0ED2-4C6B-AA34-5355F1A59EC3}"/>
   <bookViews>
-    <workbookView xWindow="8670" yWindow="150" windowWidth="19875" windowHeight="14280" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="222">
   <si>
     <t>Arduino</t>
   </si>
@@ -574,14 +575,140 @@
     <t>Neu:Pow removed</t>
   </si>
   <si>
-    <t>l</t>
+    <t>Abhängigkeiten</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Inputeigenschaften</t>
+  </si>
+  <si>
+    <t>Inputgröße</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>10 Werte</t>
+  </si>
+  <si>
+    <t>20 Werte</t>
+  </si>
+  <si>
+    <t>30 Werte</t>
+  </si>
+  <si>
+    <t>40 Werte</t>
+  </si>
+  <si>
+    <t>50 Werte</t>
+  </si>
+  <si>
+    <t>60 Werte</t>
+  </si>
+  <si>
+    <t>70 Werte</t>
+  </si>
+  <si>
+    <t>80 Werte</t>
+  </si>
+  <si>
+    <t>90 Werte</t>
+  </si>
+  <si>
+    <t>150 Werte</t>
+  </si>
+  <si>
+    <t>200 Werte</t>
+  </si>
+  <si>
+    <t>300 Werte</t>
+  </si>
+  <si>
+    <t>400 Werte</t>
+  </si>
+  <si>
+    <t>600 Werte</t>
+  </si>
+  <si>
+    <t>700 Werte</t>
+  </si>
+  <si>
+    <t>800 Werte</t>
+  </si>
+  <si>
+    <t>900 Werte</t>
+  </si>
+  <si>
+    <t>1100 Werte</t>
+  </si>
+  <si>
+    <t>1200 Werte</t>
+  </si>
+  <si>
+    <t>1300 Werte</t>
+  </si>
+  <si>
+    <t>1400 Werte</t>
+  </si>
+  <si>
+    <t>1600 Werte</t>
+  </si>
+  <si>
+    <t>1700 Werte</t>
+  </si>
+  <si>
+    <t>1800 Werte</t>
+  </si>
+  <si>
+    <t>1900 Werte</t>
+  </si>
+  <si>
+    <t>2000 Werte</t>
+  </si>
+  <si>
+    <t>364/392</t>
+  </si>
+  <si>
+    <t>462/491</t>
+  </si>
+  <si>
+    <t>700/727</t>
+  </si>
+  <si>
+    <t>1107/1136</t>
+  </si>
+  <si>
+    <t>1338/1365</t>
+  </si>
+  <si>
+    <t>1547/1573</t>
+  </si>
+  <si>
+    <t>2010/2031</t>
+  </si>
+  <si>
+    <t>2319/2345</t>
+  </si>
+  <si>
+    <t>Laufzeiten in µs</t>
+  </si>
+  <si>
+    <t>Komplexität</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nlogn </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,6 +737,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -631,10 +770,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2961,9 +3102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DC238C-8F4B-441F-9A1D-B395F114E22E}">
   <dimension ref="A1:AT96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA94" sqref="AA94"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5174,9 +5313,6 @@
       <c r="AS31">
         <v>1101</v>
       </c>
-      <c r="AT31" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="32" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
@@ -5285,6 +5421,9 @@
       <c r="AS32">
         <v>2863</v>
       </c>
+      <c r="AT32" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="34" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
@@ -5329,9 +5468,6 @@
       <c r="AS34">
         <v>187</v>
       </c>
-      <c r="AT34" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="35" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
@@ -5412,6 +5548,9 @@
       <c r="AS35">
         <v>426</v>
       </c>
+      <c r="AT35" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="36" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
@@ -5513,9 +5652,6 @@
       <c r="AS36">
         <v>327</v>
       </c>
-      <c r="AT36" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="37" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C37">
@@ -5617,6 +5753,9 @@
       <c r="AS37">
         <v>224</v>
       </c>
+      <c r="AT37" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="38" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C38">
@@ -5718,9 +5857,6 @@
       <c r="AS38">
         <v>437</v>
       </c>
-      <c r="AT38" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="39" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C39">
@@ -5821,6 +5957,9 @@
       </c>
       <c r="AS39">
         <v>347</v>
+      </c>
+      <c r="AT39" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="2:46" x14ac:dyDescent="0.25">
@@ -6024,9 +6163,6 @@
       <c r="AS41">
         <v>260</v>
       </c>
-      <c r="AT41" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="42" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C42">
@@ -6128,6 +6264,9 @@
       <c r="AS42">
         <v>2439</v>
       </c>
+      <c r="AT42" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="43" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C43">
@@ -6608,51 +6747,51 @@
         <v>162</v>
       </c>
       <c r="AG48">
-        <f>SUM(AG5:AG46)</f>
+        <f t="shared" ref="AG48:AL48" si="0">SUM(AG5:AG46)</f>
         <v>707062</v>
       </c>
       <c r="AH48">
-        <f>SUM(AH5:AH46)</f>
+        <f t="shared" si="0"/>
         <v>692100</v>
       </c>
       <c r="AI48">
-        <f>SUM(AI5:AI46)</f>
+        <f t="shared" si="0"/>
         <v>691779</v>
       </c>
       <c r="AJ48">
-        <f>SUM(AJ5:AJ46)</f>
+        <f t="shared" si="0"/>
         <v>451165</v>
       </c>
       <c r="AK48">
-        <f>SUM(AK5:AK46)</f>
+        <f t="shared" si="0"/>
         <v>453226</v>
       </c>
       <c r="AL48">
-        <f>SUM(AL5:AL46)</f>
+        <f t="shared" si="0"/>
         <v>48182</v>
       </c>
       <c r="AN48">
-        <f>SUM(AN5:AN46)</f>
+        <f t="shared" ref="AN48:AS48" si="1">SUM(AN5:AN46)</f>
         <v>680933</v>
       </c>
       <c r="AO48">
-        <f>SUM(AO5:AO46)</f>
+        <f t="shared" si="1"/>
         <v>686255</v>
       </c>
       <c r="AP48">
-        <f>SUM(AP5:AP46)</f>
+        <f t="shared" si="1"/>
         <v>687570</v>
       </c>
       <c r="AQ48">
-        <f>SUM(AQ5:AQ46)</f>
+        <f t="shared" si="1"/>
         <v>462274</v>
       </c>
       <c r="AR48">
-        <f>SUM(AR5:AR46)</f>
+        <f t="shared" si="1"/>
         <v>463613</v>
       </c>
       <c r="AS48">
-        <f>SUM(AS5:AS46)</f>
+        <f t="shared" si="1"/>
         <v>49627</v>
       </c>
     </row>
@@ -9115,8 +9254,8 @@
       <c r="L94">
         <v>26978</v>
       </c>
-      <c r="M94" t="s">
-        <v>179</v>
+      <c r="M94">
+        <v>24081</v>
       </c>
       <c r="N94">
         <v>26217</v>
@@ -9182,7 +9321,7 @@
       </c>
       <c r="M96">
         <f>AVERAGE(M85:M94)</f>
-        <v>24070.555555555555</v>
+        <v>24071.599999999999</v>
       </c>
       <c r="N96">
         <f>AVERAGE(N85:N94)</f>
@@ -9226,4 +9365,389 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31CA096-D3C7-4D8F-9AA2-1D5E4DEB070E}">
+  <dimension ref="A1:AK8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I3" t="s">
+        <v>185</v>
+      </c>
+      <c r="J3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L3" t="s">
+        <v>188</v>
+      </c>
+      <c r="M3" t="s">
+        <v>189</v>
+      </c>
+      <c r="N3" t="s">
+        <v>190</v>
+      </c>
+      <c r="O3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P3" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>164</v>
+      </c>
+      <c r="R3" t="s">
+        <v>193</v>
+      </c>
+      <c r="S3" t="s">
+        <v>194</v>
+      </c>
+      <c r="T3" t="s">
+        <v>195</v>
+      </c>
+      <c r="U3" t="s">
+        <v>196</v>
+      </c>
+      <c r="V3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" t="s">
+        <v>197</v>
+      </c>
+      <c r="X3" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>202</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>165</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>206</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>208</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="H4">
+        <v>47</v>
+      </c>
+      <c r="I4">
+        <v>49</v>
+      </c>
+      <c r="J4">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <v>51</v>
+      </c>
+      <c r="L4">
+        <v>52</v>
+      </c>
+      <c r="M4">
+        <v>53</v>
+      </c>
+      <c r="N4">
+        <v>55</v>
+      </c>
+      <c r="O4">
+        <v>56</v>
+      </c>
+      <c r="P4">
+        <v>56</v>
+      </c>
+      <c r="Q4">
+        <v>58</v>
+      </c>
+      <c r="R4">
+        <v>63</v>
+      </c>
+      <c r="S4">
+        <v>69</v>
+      </c>
+      <c r="T4">
+        <v>83</v>
+      </c>
+      <c r="U4">
+        <v>94</v>
+      </c>
+      <c r="V4">
+        <v>105</v>
+      </c>
+      <c r="W4">
+        <v>116</v>
+      </c>
+      <c r="X4">
+        <v>127</v>
+      </c>
+      <c r="Y4">
+        <v>137</v>
+      </c>
+      <c r="Z4">
+        <v>148</v>
+      </c>
+      <c r="AA4">
+        <v>159</v>
+      </c>
+      <c r="AB4">
+        <v>170</v>
+      </c>
+      <c r="AC4">
+        <v>182</v>
+      </c>
+      <c r="AD4">
+        <v>192</v>
+      </c>
+      <c r="AE4">
+        <v>204</v>
+      </c>
+      <c r="AF4">
+        <v>215</v>
+      </c>
+      <c r="AG4">
+        <v>225</v>
+      </c>
+      <c r="AH4">
+        <v>237</v>
+      </c>
+      <c r="AI4">
+        <v>247</v>
+      </c>
+      <c r="AJ4">
+        <v>258</v>
+      </c>
+      <c r="AK4">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="H5">
+        <v>132</v>
+      </c>
+      <c r="I5">
+        <v>147</v>
+      </c>
+      <c r="J5">
+        <v>158</v>
+      </c>
+      <c r="K5">
+        <v>170</v>
+      </c>
+      <c r="L5">
+        <v>192</v>
+      </c>
+      <c r="M5">
+        <v>204</v>
+      </c>
+      <c r="N5">
+        <v>215</v>
+      </c>
+      <c r="O5">
+        <v>242</v>
+      </c>
+      <c r="P5">
+        <v>251</v>
+      </c>
+      <c r="Q5">
+        <v>270</v>
+      </c>
+      <c r="R5" t="s">
+        <v>210</v>
+      </c>
+      <c r="S5" t="s">
+        <v>211</v>
+      </c>
+      <c r="T5" t="s">
+        <v>212</v>
+      </c>
+      <c r="U5">
+        <v>890</v>
+      </c>
+      <c r="V5" t="s">
+        <v>213</v>
+      </c>
+      <c r="W5" t="s">
+        <v>214</v>
+      </c>
+      <c r="X5" t="s">
+        <v>215</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z5">
+        <v>2070</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB5">
+        <v>2601</v>
+      </c>
+      <c r="AC5">
+        <v>2870</v>
+      </c>
+      <c r="AD5">
+        <v>3031</v>
+      </c>
+      <c r="AE5">
+        <v>3353</v>
+      </c>
+      <c r="AF5">
+        <v>3576</v>
+      </c>
+      <c r="AG5">
+        <v>3825</v>
+      </c>
+      <c r="AH5">
+        <v>4060</v>
+      </c>
+      <c r="AI5">
+        <v>4300</v>
+      </c>
+      <c r="AJ5">
+        <v>4483</v>
+      </c>
+      <c r="AK5">
+        <v>4798</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="G6" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed Strings in delegate, added compare mode
</commit_message>
<xml_diff>
--- a/BenchmarkDocs/Results.xlsx
+++ b/BenchmarkDocs/Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3293" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B24D8858-C0A1-43CB-BB4E-5AF0469205A9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
+    <workbookView minimized="1" xWindow="6810" yWindow="555" windowWidth="21990" windowHeight="14280" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1136,40 +1136,40 @@
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" customWidth="1"/>
-    <col min="11" max="11" width="26.44140625" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" customWidth="1"/>
-    <col min="16" max="16" width="12.88671875" customWidth="1"/>
-    <col min="17" max="17" width="12.5546875" customWidth="1"/>
-    <col min="21" max="21" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
+    <col min="21" max="21" width="22.28515625" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="23" max="23" width="11.44140625" customWidth="1"/>
-    <col min="24" max="24" width="11.109375" customWidth="1"/>
-    <col min="25" max="25" width="16.44140625" customWidth="1"/>
-    <col min="26" max="26" width="11.33203125" customWidth="1"/>
-    <col min="29" max="29" width="16.109375" customWidth="1"/>
-    <col min="30" max="30" width="35.6640625" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" customWidth="1"/>
+    <col min="24" max="24" width="11.140625" customWidth="1"/>
+    <col min="25" max="25" width="16.42578125" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" customWidth="1"/>
+    <col min="29" max="29" width="16.140625" customWidth="1"/>
+    <col min="30" max="30" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>33</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>3</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>4</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>5</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>6</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>7</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>8</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>9</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>10</v>
       </c>
@@ -1607,12 +1607,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>5</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>1</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>2</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>3</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>4</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>5</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>6</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>7</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>8</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>9</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>10</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T29">
         <v>10</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T30">
         <v>8</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T31">
         <v>8</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T32">
         <v>10</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>114</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>98</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>97</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T36">
         <v>3</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T37">
         <v>20</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T38">
         <v>20</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>98</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>124</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>127</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>128</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="43" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>136</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>139</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>140</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>141</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>137</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>148</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>149</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>152</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T51">
         <v>11</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T52">
         <v>16</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T53">
         <v>11</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T54">
         <v>16</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T55">
         <v>16</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T56">
         <v>8</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T57">
         <v>19</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T58">
         <v>17</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T59">
         <v>17</v>
       </c>
@@ -3075,12 +3075,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:30" x14ac:dyDescent="0.25">
       <c r="AD60" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T61">
         <v>15</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T63">
         <v>4</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:30" x14ac:dyDescent="0.25">
       <c r="T64">
         <v>3</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="20:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="20:21" x14ac:dyDescent="0.25">
       <c r="T65">
         <v>3</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="20:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="20:21" x14ac:dyDescent="0.25">
       <c r="T66">
         <v>4</v>
       </c>
@@ -3142,35 +3142,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DC238C-8F4B-441F-9A1D-B395F114E22E}">
   <dimension ref="A1:AT96"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I90" sqref="I90"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" customWidth="1"/>
-    <col min="16" max="16" width="13.109375" customWidth="1"/>
-    <col min="18" max="18" width="10.6640625" customWidth="1"/>
-    <col min="19" max="19" width="13.44140625" customWidth="1"/>
-    <col min="22" max="22" width="12.5546875" customWidth="1"/>
-    <col min="26" max="26" width="13.33203125" customWidth="1"/>
-    <col min="30" max="30" width="12.109375" customWidth="1"/>
-    <col min="31" max="31" width="9.5546875" customWidth="1"/>
-    <col min="32" max="32" width="23.5546875" customWidth="1"/>
-    <col min="45" max="45" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" customWidth="1"/>
+    <col min="31" max="31" width="9.5703125" customWidth="1"/>
+    <col min="32" max="32" width="23.5703125" customWidth="1"/>
+    <col min="45" max="45" width="11.7109375" customWidth="1"/>
     <col min="46" max="46" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>154</v>
       </c>
@@ -3178,7 +3176,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -3213,7 +3211,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
         <v>5</v>
       </c>
@@ -3284,7 +3282,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J5">
         <v>1</v>
       </c>
@@ -3355,7 +3353,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J6">
         <v>2</v>
       </c>
@@ -3426,7 +3424,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J7">
         <v>3</v>
       </c>
@@ -3497,7 +3495,7 @@
         <v>2192</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J8">
         <v>4</v>
       </c>
@@ -3568,7 +3566,7 @@
         <v>2411</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J9">
         <v>5</v>
       </c>
@@ -3639,7 +3637,7 @@
         <v>4167</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J10">
         <v>6</v>
       </c>
@@ -3710,7 +3708,7 @@
         <v>3972</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J11">
         <v>7</v>
       </c>
@@ -3781,7 +3779,7 @@
         <v>5484</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J12">
         <v>8</v>
       </c>
@@ -3852,7 +3850,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J13">
         <v>9</v>
       </c>
@@ -3923,7 +3921,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="J14">
         <v>10</v>
       </c>
@@ -3994,7 +3992,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AF15" t="s">
         <v>45</v>
       </c>
@@ -4035,7 +4033,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>166</v>
       </c>
@@ -4111,7 +4109,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="17" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:46" x14ac:dyDescent="0.25">
       <c r="AF17" t="s">
         <v>47</v>
       </c>
@@ -4152,7 +4150,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="18" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>160</v>
       </c>
@@ -4199,7 +4197,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="19" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>33</v>
       </c>
@@ -4240,7 +4238,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>5</v>
       </c>
@@ -4341,7 +4339,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="21" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>1</v>
       </c>
@@ -4442,7 +4440,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="22" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>2</v>
       </c>
@@ -4543,7 +4541,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="23" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>3</v>
       </c>
@@ -4644,7 +4642,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="24" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>4</v>
       </c>
@@ -4745,7 +4743,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="25" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>5</v>
       </c>
@@ -4846,7 +4844,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="26" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>6</v>
       </c>
@@ -4950,7 +4948,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>7</v>
       </c>
@@ -5051,7 +5049,7 @@
         <v>2665</v>
       </c>
     </row>
-    <row r="28" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>8</v>
       </c>
@@ -5113,7 +5111,7 @@
         <v>1039427</v>
       </c>
     </row>
-    <row r="29" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>9</v>
       </c>
@@ -5214,7 +5212,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>10</v>
       </c>
@@ -5315,7 +5313,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="31" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:46" x14ac:dyDescent="0.25">
       <c r="AF31" t="s">
         <v>56</v>
       </c>
@@ -5356,7 +5354,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="32" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>166</v>
       </c>
@@ -5467,7 +5465,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>167</v>
       </c>
@@ -5511,7 +5509,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="35" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>33</v>
       </c>
@@ -5594,7 +5592,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>5</v>
       </c>
@@ -5695,7 +5693,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="37" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>1</v>
       </c>
@@ -5799,7 +5797,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>2</v>
       </c>
@@ -5900,7 +5898,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="39" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>3</v>
       </c>
@@ -6004,7 +6002,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>4</v>
       </c>
@@ -6105,7 +6103,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="41" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>5</v>
       </c>
@@ -6206,7 +6204,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="42" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>6</v>
       </c>
@@ -6310,7 +6308,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>7</v>
       </c>
@@ -6411,7 +6409,7 @@
         <v>4832</v>
       </c>
     </row>
-    <row r="44" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>8</v>
       </c>
@@ -6512,7 +6510,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="45" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>9</v>
       </c>
@@ -6613,7 +6611,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="46" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>10</v>
       </c>
@@ -6717,7 +6715,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>166</v>
       </c>
@@ -6837,7 +6835,7 @@
         <v>49627</v>
       </c>
     </row>
-    <row r="50" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>172</v>
       </c>
@@ -6845,7 +6843,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>33</v>
       </c>
@@ -6928,7 +6926,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="52" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>5</v>
       </c>
@@ -7029,7 +7027,7 @@
         <v>19921</v>
       </c>
     </row>
-    <row r="53" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>1</v>
       </c>
@@ -7133,7 +7131,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="54" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>2</v>
       </c>
@@ -7237,7 +7235,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C55">
         <v>3</v>
       </c>
@@ -7299,7 +7297,7 @@
         <v>694115</v>
       </c>
     </row>
-    <row r="56" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>4</v>
       </c>
@@ -7361,7 +7359,7 @@
         <v>693883</v>
       </c>
     </row>
-    <row r="57" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>5</v>
       </c>
@@ -7423,7 +7421,7 @@
         <v>693997</v>
       </c>
     </row>
-    <row r="58" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>6</v>
       </c>
@@ -7485,7 +7483,7 @@
         <v>693998</v>
       </c>
     </row>
-    <row r="59" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>7</v>
       </c>
@@ -7547,7 +7545,7 @@
         <v>693914</v>
       </c>
     </row>
-    <row r="60" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>8</v>
       </c>
@@ -7609,7 +7607,7 @@
         <v>694056</v>
       </c>
     </row>
-    <row r="61" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>9</v>
       </c>
@@ -7671,7 +7669,7 @@
         <v>694005</v>
       </c>
     </row>
-    <row r="62" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C62">
         <v>10</v>
       </c>
@@ -7733,7 +7731,7 @@
         <v>694157</v>
       </c>
     </row>
-    <row r="64" spans="2:46" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>166</v>
       </c>
@@ -7802,7 +7800,7 @@
         <v>694047.7</v>
       </c>
     </row>
-    <row r="66" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>175</v>
       </c>
@@ -7810,7 +7808,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>33</v>
       </c>
@@ -7851,7 +7849,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>5</v>
       </c>
@@ -7913,7 +7911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>1</v>
       </c>
@@ -7975,7 +7973,7 @@
         <v>693930</v>
       </c>
     </row>
-    <row r="70" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C70">
         <v>2</v>
       </c>
@@ -8037,7 +8035,7 @@
         <v>694477</v>
       </c>
     </row>
-    <row r="71" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>3</v>
       </c>
@@ -8099,7 +8097,7 @@
         <v>694283</v>
       </c>
     </row>
-    <row r="72" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>4</v>
       </c>
@@ -8161,7 +8159,7 @@
         <v>694253</v>
       </c>
     </row>
-    <row r="73" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>5</v>
       </c>
@@ -8223,7 +8221,7 @@
         <v>694410</v>
       </c>
     </row>
-    <row r="74" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C74">
         <v>6</v>
       </c>
@@ -8285,7 +8283,7 @@
         <v>694207</v>
       </c>
     </row>
-    <row r="75" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C75">
         <v>7</v>
       </c>
@@ -8347,7 +8345,7 @@
         <v>694230</v>
       </c>
     </row>
-    <row r="76" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C76">
         <v>8</v>
       </c>
@@ -8409,7 +8407,7 @@
         <v>694136</v>
       </c>
     </row>
-    <row r="77" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C77">
         <v>9</v>
       </c>
@@ -8471,7 +8469,7 @@
         <v>694309</v>
       </c>
     </row>
-    <row r="78" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C78">
         <v>10</v>
       </c>
@@ -8533,7 +8531,7 @@
         <v>693908</v>
       </c>
     </row>
-    <row r="80" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>166</v>
       </c>
@@ -8602,7 +8600,7 @@
         <v>694214.3</v>
       </c>
     </row>
-    <row r="82" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>177</v>
       </c>
@@ -8610,7 +8608,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="83" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>33</v>
       </c>
@@ -8651,7 +8649,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>5</v>
       </c>
@@ -8713,7 +8711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C85" s="5">
         <v>1</v>
       </c>
@@ -8775,7 +8773,7 @@
         <v>72558</v>
       </c>
     </row>
-    <row r="86" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C86" s="5">
         <v>2</v>
       </c>
@@ -8837,7 +8835,7 @@
         <v>72659</v>
       </c>
     </row>
-    <row r="87" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C87" s="5">
         <v>3</v>
       </c>
@@ -8899,7 +8897,7 @@
         <v>72682</v>
       </c>
     </row>
-    <row r="88" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C88" s="5">
         <v>4</v>
       </c>
@@ -8961,7 +8959,7 @@
         <v>72665</v>
       </c>
     </row>
-    <row r="89" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C89" s="5">
         <v>5</v>
       </c>
@@ -9023,7 +9021,7 @@
         <v>72475</v>
       </c>
     </row>
-    <row r="90" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C90" s="5">
         <v>6</v>
       </c>
@@ -9085,7 +9083,7 @@
         <v>72971</v>
       </c>
     </row>
-    <row r="91" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C91" s="5">
         <v>7</v>
       </c>
@@ -9147,7 +9145,7 @@
         <v>72782</v>
       </c>
     </row>
-    <row r="92" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C92" s="5">
         <v>8</v>
       </c>
@@ -9209,7 +9207,7 @@
         <v>72820</v>
       </c>
     </row>
-    <row r="93" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C93" s="5">
         <v>9</v>
       </c>
@@ -9271,7 +9269,7 @@
         <v>72988</v>
       </c>
     </row>
-    <row r="94" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C94" s="5">
         <v>10</v>
       </c>
@@ -9333,7 +9331,7 @@
         <v>72675</v>
       </c>
     </row>
-    <row r="96" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
         <v>166</v>
       </c>
@@ -9413,26 +9411,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31CA096-D3C7-4D8F-9AA2-1D5E4DEB070E}">
   <dimension ref="A1:AK42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="D2" s="5" t="s">
         <v>179</v>
       </c>
@@ -9440,7 +9438,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>34</v>
       </c>
@@ -9550,7 +9548,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>45</v>
       </c>
@@ -9654,7 +9652,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>50</v>
       </c>
@@ -9755,7 +9753,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>56</v>
       </c>
@@ -9856,7 +9854,7 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>43</v>
       </c>
@@ -9960,7 +9958,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>63</v>
       </c>
@@ -10064,7 +10062,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>65</v>
       </c>
@@ -10168,7 +10166,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>87</v>
       </c>
@@ -10275,7 +10273,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>88</v>
       </c>
@@ -10382,7 +10380,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>68</v>
       </c>
@@ -10486,7 +10484,7 @@
         <v>9841</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>46</v>
       </c>
@@ -10590,7 +10588,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>85</v>
       </c>
@@ -10697,7 +10695,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>86</v>
       </c>
@@ -10804,7 +10802,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>49</v>
       </c>
@@ -10908,7 +10906,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="17" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>35</v>
       </c>
@@ -11013,7 +11011,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>54</v>
       </c>
@@ -11114,7 +11112,7 @@
         <v>1917</v>
       </c>
     </row>
-    <row r="19" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>36</v>
       </c>
@@ -11218,7 +11216,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="20" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>55</v>
       </c>
@@ -11319,7 +11317,7 @@
         <v>1884</v>
       </c>
     </row>
-    <row r="21" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>37</v>
       </c>
@@ -11420,7 +11418,7 @@
         <v>4132</v>
       </c>
     </row>
-    <row r="22" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>38</v>
       </c>
@@ -11528,7 +11526,7 @@
         <v>4798</v>
       </c>
     </row>
-    <row r="23" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>41</v>
       </c>
@@ -11635,7 +11633,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="24" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>39</v>
       </c>
@@ -11739,7 +11737,7 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="25" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>40</v>
       </c>
@@ -11843,7 +11841,7 @@
         <v>8243</v>
       </c>
     </row>
-    <row r="26" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>52</v>
       </c>
@@ -11947,7 +11945,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="27" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>69</v>
       </c>
@@ -12048,7 +12046,7 @@
         <v>2479</v>
       </c>
     </row>
-    <row r="28" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>61</v>
       </c>
@@ -12149,7 +12147,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="29" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
         <v>70</v>
       </c>
@@ -12250,7 +12248,7 @@
         <v>2426</v>
       </c>
     </row>
-    <row r="30" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>66</v>
       </c>
@@ -12354,7 +12352,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="31" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
         <v>47</v>
       </c>
@@ -12458,7 +12456,7 @@
         <v>1663</v>
       </c>
     </row>
-    <row r="32" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>42</v>
       </c>
@@ -12562,7 +12560,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="33" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>59</v>
       </c>
@@ -12663,7 +12661,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="34" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>44</v>
       </c>
@@ -12768,7 +12766,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="35" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>48</v>
       </c>
@@ -12869,7 +12867,7 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="36" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>53</v>
       </c>
@@ -12976,7 +12974,7 @@
         <v>5435</v>
       </c>
     </row>
-    <row r="37" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>57</v>
       </c>
@@ -13080,7 +13078,7 @@
         <v>5465</v>
       </c>
     </row>
-    <row r="38" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>60</v>
       </c>
@@ -13184,7 +13182,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="39" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>62</v>
       </c>
@@ -13288,7 +13286,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="40" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
         <v>64</v>
       </c>
@@ -13392,7 +13390,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="41" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
         <v>67</v>
       </c>
@@ -13496,7 +13494,7 @@
         <v>4884</v>
       </c>
     </row>
-    <row r="42" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
Uncommitted fixes in prediction algorithm, more runtime results
</commit_message>
<xml_diff>
--- a/BenchmarkDocs/Results.xlsx
+++ b/BenchmarkDocs/Results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f0dc99f0b729840/Teilen/edge-ml/feature-extraction/BenchmarkDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3293" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B24D8858-C0A1-43CB-BB4E-5AF0469205A9}"/>
+  <xr:revisionPtr revIDLastSave="3435" documentId="13_ncr:1_{A4998A85-1724-47F3-8083-8F6F99AF08C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D38CD0F-3DD5-4308-84B4-2700097356E0}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6810" yWindow="555" windowWidth="21990" windowHeight="14280" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
+    <workbookView xWindow="1830" yWindow="150" windowWidth="21990" windowHeight="14280" activeTab="1" xr2:uid="{BD4ED9CD-8936-4570-81FB-899C72BF223C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabelle4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="238">
   <si>
     <t>Arduino</t>
   </si>
@@ -717,6 +718,39 @@
   </si>
   <si>
     <t>n log n  bzw 1 (cache)</t>
+  </si>
+  <si>
+    <t>Extract Start</t>
+  </si>
+  <si>
+    <t>O(1)</t>
+  </si>
+  <si>
+    <t>O(n)</t>
+  </si>
+  <si>
+    <t>median_abs_changes</t>
+  </si>
+  <si>
+    <t>median_changes</t>
+  </si>
+  <si>
+    <t>O(3n)</t>
+  </si>
+  <si>
+    <t>O(2n)</t>
+  </si>
+  <si>
+    <t>libxtract</t>
+  </si>
+  <si>
+    <t>edgefel iter</t>
+  </si>
+  <si>
+    <t>edgefel some</t>
+  </si>
+  <si>
+    <t>edgefel cache</t>
   </si>
 </sst>
 </file>
@@ -806,7 +840,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -816,6 +850,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1132,7 +1169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B09DA97-D620-4F66-8E45-7C0B77C13B9B}">
   <dimension ref="B1:AD66"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
@@ -3142,7 +3179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DC238C-8F4B-441F-9A1D-B395F114E22E}">
   <dimension ref="A1:AT96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AF31" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9411,8 +9448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31CA096-D3C7-4D8F-9AA2-1D5E4DEB070E}">
   <dimension ref="A1:AK42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13605,4 +13642,585 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5B531B-4ECE-4B93-951B-3E79254AD1C0}">
+  <dimension ref="A1:K51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" t="s">
+        <v>217</v>
+      </c>
+      <c r="I7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I8">
+        <v>2956</v>
+      </c>
+      <c r="J8">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H9" t="s">
+        <v>227</v>
+      </c>
+      <c r="I9">
+        <v>9488</v>
+      </c>
+      <c r="J9">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10">
+        <v>57</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12">
+        <v>51</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13">
+        <v>51</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14">
+        <v>66</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15">
+        <v>66</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H15" t="s">
+        <v>235</v>
+      </c>
+      <c r="I15" t="s">
+        <v>236</v>
+      </c>
+      <c r="J15" t="s">
+        <v>237</v>
+      </c>
+      <c r="K15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16">
+        <v>4060</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="H16">
+        <v>4776</v>
+      </c>
+      <c r="I16">
+        <v>4824</v>
+      </c>
+      <c r="J16">
+        <v>3756</v>
+      </c>
+      <c r="K16">
+        <v>34650</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18">
+        <v>63</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19">
+        <v>63</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J20" t="s">
+        <v>74</v>
+      </c>
+      <c r="K20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H21">
+        <v>19857</v>
+      </c>
+      <c r="J21">
+        <v>24731</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22">
+        <v>51</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25">
+        <v>57</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26">
+        <v>4000</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C27">
+        <v>4057</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28">
+        <v>4000</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C29">
+        <v>4000</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31">
+        <v>54</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33">
+        <v>54</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34">
+        <v>51</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40">
+        <v>4017</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41">
+        <v>4065</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42">
+        <v>36</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45">
+        <v>4000</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46">
+        <v>20</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48">
+        <v>8192</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49">
+        <v>8211</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>